<commit_message>
End to End Applications Types data are fed from new tabs.
</commit_message>
<xml_diff>
--- a/src/test/java/BaseFramework/Data/DA.xlsx
+++ b/src/test/java/BaseFramework/Data/DA.xlsx
@@ -3,25 +3,26 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syadav12\Documents\Admissions_Workspace\DA\src\test\java\BaseFramework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14445" windowHeight="8160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14445" windowHeight="8160" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Create Account" sheetId="1" r:id="rId1"/>
-    <sheet name="Program2" sheetId="2" r:id="rId2"/>
-    <sheet name="Drop Down Values" sheetId="6" r:id="rId3"/>
-    <sheet name="Requirments Sheet" sheetId="3" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId6"/>
+    <sheet name="Complete_Application" sheetId="2" r:id="rId2"/>
+    <sheet name="RequestDeferral_Application" sheetId="7" r:id="rId3"/>
+    <sheet name="Withdraw_Application" sheetId="8" r:id="rId4"/>
+    <sheet name="Drop Down Values" sheetId="6" r:id="rId5"/>
+    <sheet name="Requirments Sheet" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="232">
   <si>
     <t>First Name</t>
   </si>
@@ -535,21 +536,6 @@
     <t>I work part time at Liverpool Central Store.</t>
   </si>
   <si>
-    <t>Mobin</t>
-  </si>
-  <si>
-    <t>Pai</t>
-  </si>
-  <si>
-    <t>m.pai@mailinator.com</t>
-  </si>
-  <si>
-    <t>Record</t>
-  </si>
-  <si>
-    <t>James Andreson</t>
-  </si>
-  <si>
     <t>Reject at source</t>
   </si>
   <si>
@@ -572,14 +558,206 @@
   </si>
   <si>
     <t>s.bishop@mailinator.com</t>
+  </si>
+  <si>
+    <t>Shauny</t>
+  </si>
+  <si>
+    <t>Parrt</t>
+  </si>
+  <si>
+    <t>s.parrt@mailinator.com</t>
+  </si>
+  <si>
+    <t>CRM - WFE Sync</t>
+  </si>
+  <si>
+    <t>CRM</t>
+  </si>
+  <si>
+    <t>WFE</t>
+  </si>
+  <si>
+    <t>Withdrawn</t>
+  </si>
+  <si>
+    <t>Un-withdrawn</t>
+  </si>
+  <si>
+    <t>Submitted</t>
+  </si>
+  <si>
+    <t>Genearte Reports in CRM</t>
+  </si>
+  <si>
+    <t>CRM Only tests</t>
+  </si>
+  <si>
+    <t>WFE Only Test</t>
+  </si>
+  <si>
+    <t>CRM Department Only Test</t>
+  </si>
+  <si>
+    <t>E.g. Login/Logout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application per category </t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Post Grad</t>
+  </si>
+  <si>
+    <t>TBC</t>
+  </si>
+  <si>
+    <t>MRC Doctoral Training Program</t>
+  </si>
+  <si>
+    <t>Visiting Student (Non Degree), Summer School, Pre-sessional English</t>
+  </si>
+  <si>
+    <t>Pre-Sessional English Programme (12 week)</t>
+  </si>
+  <si>
+    <t>Mathematics Research (Occasional FT)</t>
+  </si>
+  <si>
+    <t>Mastering Lab Skills</t>
+  </si>
+  <si>
+    <t>PGTR</t>
+  </si>
+  <si>
+    <t>Advanced Chemical Engineering (MSc 1YFT)</t>
+  </si>
+  <si>
+    <t>Human Vaccinology (MRes 1YFT)</t>
+  </si>
+  <si>
+    <t>Business Analytics (MSc 1YFT)</t>
+  </si>
+  <si>
+    <t>Management (MBA 1YFT)</t>
+  </si>
+  <si>
+    <t>Medical Sciences with Humanities, Philosophy and Law BSc (1YFT - Intercalated)</t>
+  </si>
+  <si>
+    <t>Chemistry Research (PhD)</t>
+  </si>
+  <si>
+    <t>Self Funding</t>
+  </si>
+  <si>
+    <t>4 Users</t>
+  </si>
+  <si>
+    <t>Deparment Decision</t>
+  </si>
+  <si>
+    <t>Offer and Save
+Sent Back to Registry</t>
+  </si>
+  <si>
+    <t>Special case procedure</t>
+  </si>
+  <si>
+    <t>Steps required</t>
+  </si>
+  <si>
+    <t>Offered</t>
+  </si>
+  <si>
+    <t>Accept</t>
+  </si>
+  <si>
+    <t>Declined</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">courseCode - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"A100"</t>
+    </r>
+  </si>
+  <si>
+    <t>UG Course Applciation</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">courseCode - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"F303"</t>
+    </r>
+  </si>
+  <si>
+    <t>Internal Clearning</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>DA and UG</t>
+  </si>
+  <si>
+    <t>Financial Support (UG NA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confidential Information </t>
+  </si>
+  <si>
+    <t>Only For A100</t>
+  </si>
+  <si>
+    <t>Assgine , Steps Required</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>pgr</t>
+  </si>
+  <si>
+    <t>xyz.efg@mailinator.com</t>
+  </si>
+  <si>
+    <t>withdraw</t>
+  </si>
+  <si>
+    <t>passon</t>
+  </si>
+  <si>
+    <t>withfaw.draw@mailinator.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
-  <fonts count="8">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -631,6 +809,19 @@
     <font>
       <sz val="8"/>
       <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF008000"/>
       <name val="Courier New"/>
       <family val="3"/>
     </font>
@@ -924,7 +1115,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -937,7 +1128,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -946,9 +1136,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -970,6 +1158,23 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -998,6 +1203,14 @@
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D11A-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
 </file>
 
+<file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D11A-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX3.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D11A-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -1021,6 +1234,110 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2049"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>51</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>457200</xdr:colOff>
+          <xdr:row>52</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8193" name="Control 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s8193"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>51</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>457200</xdr:colOff>
+          <xdr:row>52</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9217" name="Control 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s9217"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1315,124 +1632,124 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="46.28515625" collapsed="true"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="46.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
-        <v>176</v>
-      </c>
-      <c r="B2" s="37"/>
+      <c r="A2" s="39" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="34"/>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="36" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="33" t="s">
-        <v>178</v>
+      <c r="B4" s="30" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="33" t="s">
-        <v>179</v>
+      <c r="B5" s="30" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="30" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="30" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="34" t="s">
-        <v>180</v>
+      <c r="B8" s="31" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="30" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="30" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="30" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="30" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="38" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="24" t="s">
-        <v>177</v>
-      </c>
-      <c r="B15" s="25"/>
+      <c r="A15" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="B15" s="22"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1471,17 +1788,17 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="89.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="51.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="5" max="6" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="1" max="1" width="89.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1491,7 +1808,7 @@
       <c r="B1" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="28" t="s">
         <v>139</v>
       </c>
     </row>
@@ -1500,7 +1817,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1508,13 +1825,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="E3" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="E3" s="36" t="s">
-        <v>174</v>
-      </c>
-      <c r="F3" s="36" t="s">
-        <v>175</v>
+      <c r="F3" s="33" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1525,10 +1842,10 @@
         <v>18</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>171</v>
+        <v>22</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>172</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1538,23 +1855,17 @@
       <c r="B5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="28" t="s">
         <v>139</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>170</v>
+      <c r="B6" s="12" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1588,7 +1899,7 @@
       <c r="B10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="28" t="s">
         <v>139</v>
       </c>
     </row>
@@ -1609,10 +1920,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1623,22 +1934,22 @@
       <c r="B16" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="28" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>125</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="28" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>126</v>
       </c>
@@ -1646,7 +1957,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>29</v>
       </c>
@@ -1654,7 +1965,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>30</v>
       </c>
@@ -1662,7 +1973,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>32</v>
       </c>
@@ -1670,7 +1981,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>34</v>
       </c>
@@ -1678,42 +1989,31 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>44</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="H23">
-        <v>3800</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>37</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="H24">
-        <f>2300+800+300</f>
-        <v>3400</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="H25">
-        <f>+H23-H24</f>
-        <v>400</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>39</v>
       </c>
@@ -1721,7 +2021,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>40</v>
       </c>
@@ -1729,7 +2029,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>41</v>
       </c>
@@ -1737,7 +2037,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>47</v>
       </c>
@@ -1745,16 +2045,16 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B30" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="31"/>
-    </row>
-    <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="C30" s="28"/>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>50</v>
       </c>
@@ -1762,7 +2062,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>42</v>
       </c>
@@ -1779,22 +2079,22 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="C37" s="31"/>
+      <c r="C37" s="28"/>
       <c r="K37" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
+      <c r="A38" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="14" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1874,7 +2174,7 @@
       <c r="A48" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B48" s="13" t="s">
+      <c r="B48" s="12" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1882,7 +2182,7 @@
       <c r="A49" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B49" s="13" t="s">
+      <c r="B49" s="12" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1890,7 +2190,7 @@
       <c r="A50" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="B50" s="12" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1898,12 +2198,12 @@
       <c r="A51" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B51" s="13" t="s">
+      <c r="B51" s="12" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="15" t="s">
+      <c r="A53" s="14" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1916,10 +2216,10 @@
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="14" t="s">
+      <c r="A57" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B57" s="14" t="s">
+      <c r="B57" s="13" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1927,7 +2227,7 @@
       <c r="A58" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B58" s="13" t="s">
+      <c r="B58" s="12" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1935,7 +2235,7 @@
       <c r="A59" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B59" s="13" t="s">
+      <c r="B59" s="12" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1943,7 +2243,7 @@
       <c r="A60" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B60" s="16" t="s">
+      <c r="B60" s="15" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1951,12 +2251,12 @@
       <c r="A61" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B61" s="13" t="s">
+      <c r="B61" s="12" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="15" t="s">
+      <c r="A62" s="14" t="s">
         <v>101</v>
       </c>
       <c r="B62" s="6" t="s">
@@ -1964,15 +2264,15 @@
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="14" t="s">
+      <c r="A65" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="B65" s="14" t="s">
+      <c r="B65" s="13" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="15" t="s">
+      <c r="A66" s="14" t="s">
         <v>104</v>
       </c>
       <c r="B66" s="3" t="s">
@@ -1980,7 +2280,7 @@
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="15" t="s">
+      <c r="A67" s="14" t="s">
         <v>105</v>
       </c>
       <c r="B67" s="6"/>
@@ -1989,15 +2289,15 @@
       <c r="A68" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="B68" s="13" t="s">
+      <c r="B68" s="12" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="14" t="s">
+      <c r="A71" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="B71" s="14" t="s">
+      <c r="B71" s="13" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2005,7 +2305,7 @@
       <c r="A72" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B72" s="13" t="s">
+      <c r="B72" s="12" t="s">
         <v>119</v>
       </c>
     </row>
@@ -2013,7 +2313,7 @@
       <c r="A73" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B73" s="13" t="s">
+      <c r="B73" s="12" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2021,15 +2321,15 @@
       <c r="A74" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B74" s="13" t="s">
+      <c r="B74" s="12" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="14" t="s">
+      <c r="A77" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="B77" s="14" t="s">
+      <c r="B77" s="13" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2037,7 +2337,7 @@
       <c r="A78" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B78" s="13" t="s">
+      <c r="B78" s="12" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2045,15 +2345,15 @@
       <c r="A79" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B79" s="13" t="s">
+      <c r="B79" s="12" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="14" t="s">
+      <c r="A84" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="B84" s="14" t="s">
+      <c r="B84" s="13" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2061,7 +2361,7 @@
       <c r="A85" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B85" s="13" t="s">
+      <c r="B85" s="12" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2069,7 +2369,7 @@
       <c r="A86" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="B86" s="13" t="s">
+      <c r="B86" s="12" t="s">
         <v>156</v>
       </c>
     </row>
@@ -2077,7 +2377,7 @@
       <c r="A87" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="B87" s="13" t="s">
+      <c r="B87" s="12" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2085,7 +2385,7 @@
       <c r="A88" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="B88" s="13" t="s">
+      <c r="B88" s="12" t="s">
         <v>157</v>
       </c>
     </row>
@@ -2093,7 +2393,7 @@
       <c r="A89" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="B89" s="13" t="s">
+      <c r="B89" s="12" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2101,7 +2401,7 @@
       <c r="A90" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="B90" s="13" t="s">
+      <c r="B90" s="12" t="s">
         <v>157</v>
       </c>
     </row>
@@ -2109,15 +2409,15 @@
       <c r="A91" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="B91" s="13" t="s">
+      <c r="B91" s="12" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="14" t="s">
+      <c r="A94" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="B94" s="14" t="s">
+      <c r="B94" s="13" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2125,7 +2425,7 @@
       <c r="A95" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B95" s="13" t="s">
+      <c r="B95" s="12" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2133,7 +2433,7 @@
       <c r="A96" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="B96" s="13" t="s">
+      <c r="B96" s="12" t="s">
         <v>161</v>
       </c>
     </row>
@@ -2141,7 +2441,7 @@
       <c r="A97" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="B97" s="13" t="s">
+      <c r="B97" s="12" t="s">
         <v>162</v>
       </c>
     </row>
@@ -2149,7 +2449,7 @@
       <c r="A98" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="B98" s="13" t="s">
+      <c r="B98" s="12" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2157,7 +2457,7 @@
       <c r="A99" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="B99" s="13" t="s">
+      <c r="B99" s="12" t="s">
         <v>166</v>
       </c>
     </row>
@@ -2165,7 +2465,7 @@
       <c r="A100" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="B100" s="13" t="s">
+      <c r="B100" s="12" t="s">
         <v>165</v>
       </c>
     </row>
@@ -2173,7 +2473,7 @@
       <c r="A101" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="B101" s="13" t="s">
+      <c r="B101" s="12" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2182,7 +2482,7 @@
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <controls>
-    <mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
         <control shapeId="2049" r:id="rId3" name="Control 1">
           <controlPr defaultSize="0" r:id="rId4">
@@ -2209,7 +2509,7 @@
     </mc:AlternateContent>
   </controls>
   <extLst>
-    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -2245,7 +2545,7 @@
           <x14:formula1>
             <xm:f>'Drop Down Values'!$G$3:$G$5</xm:f>
           </x14:formula1>
-          <xm:sqref>F5</xm:sqref>
+          <xm:sqref>F4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2254,6 +2554,1546 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:K101"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="89.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="28"/>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C37" s="28"/>
+      <c r="K37" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A44" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A46" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A48" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A49" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A50" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A51" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A54" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A58" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A59" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A60" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B60" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A61" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B61" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B65" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="B67" s="6"/>
+    </row>
+    <row r="68" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A68" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B68" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B71" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A72" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B72" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A73" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B73" s="12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A74" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B74" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B77" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A78" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B78" s="12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A79" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B79" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B84" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A85" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B85" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A86" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B86" s="12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A87" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B87" s="12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A88" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B88" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A89" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B89" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A90" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B90" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A91" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B91" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B94" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A95" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B95" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A96" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B96" s="12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A97" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B97" s="12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A98" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B98" s="12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A99" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B99" s="12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A100" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B100" s="12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A101" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B101" s="12" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <controls>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="8193" r:id="rId3" name="Control 1">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>51</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>457200</xdr:colOff>
+                <xdr:row>52</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="8193" r:id="rId3" name="Control 1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </controls>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$G$3:$G$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>F4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$C$30:$C$31</xm:f>
+          </x14:formula1>
+          <xm:sqref>B17</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$C$22:$C$27</xm:f>
+          </x14:formula1>
+          <xm:sqref>B16</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$C$15:$C$16</xm:f>
+          </x14:formula1>
+          <xm:sqref>B10</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$C$3:$C$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$C$11:$C$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>B5</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:K101"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="89.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="28"/>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C37" s="28"/>
+      <c r="K37" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A44" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A46" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A48" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A49" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A50" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A51" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A54" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A58" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A59" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A60" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B60" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A61" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B61" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B65" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="B67" s="6"/>
+    </row>
+    <row r="68" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A68" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B68" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B71" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A72" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B72" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A73" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B73" s="12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A74" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B74" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B77" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A78" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B78" s="12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A79" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B79" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B84" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A85" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B85" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A86" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B86" s="12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A87" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B87" s="12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A88" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B88" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A89" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B89" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A90" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B90" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A91" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B91" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B94" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A95" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B95" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A96" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B96" s="12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A97" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B97" s="12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A98" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B98" s="12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A99" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B99" s="12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A100" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B100" s="12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A101" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B101" s="12" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <controls>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="9217" r:id="rId3" name="Control 1">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>51</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>457200</xdr:colOff>
+                <xdr:row>52</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="9217" r:id="rId3" name="Control 1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </controls>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$C$11:$C$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>B5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$C$3:$C$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$C$15:$C$16</xm:f>
+          </x14:formula1>
+          <xm:sqref>B10</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$C$22:$C$27</xm:f>
+          </x14:formula1>
+          <xm:sqref>B16</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$C$30:$C$31</xm:f>
+          </x14:formula1>
+          <xm:sqref>B17</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$G$3:$G$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>F4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
@@ -2263,99 +4103,99 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="48.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="48.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="40" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="23" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="27"/>
-      <c r="C4" s="28" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="F4" s="27"/>
-      <c r="G4" s="28" t="s">
+      <c r="F4" s="24"/>
+      <c r="G4" s="25" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="27"/>
-      <c r="C5" s="28" t="s">
+      <c r="B5" s="24"/>
+      <c r="C5" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="F5" s="24"/>
-      <c r="G5" s="29" t="s">
-        <v>173</v>
+      <c r="F5" s="21"/>
+      <c r="G5" s="26" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="27"/>
-      <c r="C6" s="28" t="s">
+      <c r="B6" s="24"/>
+      <c r="C6" s="25" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="27"/>
-      <c r="C7" s="28" t="s">
+      <c r="B7" s="24"/>
+      <c r="C7" s="25" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="27"/>
-      <c r="C8" s="28" t="s">
+      <c r="B8" s="24"/>
+      <c r="C8" s="25" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="24"/>
-      <c r="C9" s="29" t="s">
+      <c r="B9" s="21"/>
+      <c r="C9" s="26" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="23" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="27"/>
-      <c r="C12" s="28" t="s">
+      <c r="B12" s="24"/>
+      <c r="C12" s="25" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="24"/>
-      <c r="C13" s="29" t="s">
+      <c r="B13" s="21"/>
+      <c r="C13" s="26" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2363,89 +4203,89 @@
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="23" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="24"/>
-      <c r="C16" s="25"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="22"/>
     </row>
     <row r="17" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="2:3" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="23" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="27"/>
-      <c r="C19" s="28" t="s">
+      <c r="B19" s="24"/>
+      <c r="C19" s="25" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="24"/>
-      <c r="C20" s="29" t="s">
+      <c r="B20" s="21"/>
+      <c r="C20" s="26" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="2:3" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="23" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="27"/>
-      <c r="C23" s="28" t="s">
+      <c r="B23" s="24"/>
+      <c r="C23" s="25" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="27"/>
-      <c r="C24" s="28" t="s">
+      <c r="B24" s="24"/>
+      <c r="C24" s="25" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="27"/>
-      <c r="C25" s="28" t="s">
+      <c r="B25" s="24"/>
+      <c r="C25" s="25" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="27"/>
-      <c r="C26" s="28" t="s">
+      <c r="B26" s="24"/>
+      <c r="C26" s="25" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="24"/>
-      <c r="C27" s="29" t="s">
+      <c r="B27" s="21"/>
+      <c r="C27" s="26" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="2:3" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="23" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="31" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="24"/>
-      <c r="C31" s="29" t="s">
+      <c r="B31" s="21"/>
+      <c r="C31" s="26" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2457,99 +4297,133 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F14:J29"/>
+  <dimension ref="E11:P43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="25.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="33.42578125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="41" customWidth="1"/>
+    <col min="15" max="15" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="70" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="14" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F14" s="17" t="s">
+    <row r="11" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F11" s="41" t="s">
+        <v>221</v>
+      </c>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
+    </row>
+    <row r="12" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="13" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="14" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F14" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="H14" s="17" t="s">
+      <c r="H14" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="I14" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="J14" s="20" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="15" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F15" s="18" t="s">
+      <c r="I14" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="15" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F15" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="G15" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="H15" s="18" t="s">
+      <c r="H15" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="I15" s="21" t="s">
+      <c r="I15" s="46" t="s">
+        <v>206</v>
+      </c>
+      <c r="J15" s="46" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>191</v>
+      </c>
+      <c r="F16" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="G16" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="H16" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="I16" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="J15" s="23" t="s">
+      <c r="J16" s="47" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F16" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="G16" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="H16" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="I16" s="18"/>
-      <c r="J16" s="12"/>
-    </row>
     <row r="17" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F17" s="18" t="s">
+      <c r="F17" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="G17" s="18" t="s">
+      <c r="G17" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="H17" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="I17" s="18"/>
+      <c r="I17" s="17"/>
     </row>
     <row r="18" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F18" s="18" t="s">
+      <c r="F18" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="G18" s="18" t="s">
+      <c r="G18" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
     </row>
     <row r="19" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F19" s="18"/>
-      <c r="G19" s="18" t="s">
+      <c r="F19" s="45"/>
+      <c r="G19" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+    </row>
+    <row r="21" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F21" s="2"/>
     </row>
     <row r="26" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
@@ -2557,7 +4431,7 @@
       </c>
     </row>
     <row r="27" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F27" s="19" t="s">
+      <c r="F27" s="18" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2567,37 +4441,258 @@
       </c>
     </row>
     <row r="29" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F29" s="22" t="s">
+      <c r="F29" s="20" t="s">
         <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E34" s="42" t="s">
+        <v>179</v>
+      </c>
+      <c r="F34" s="42"/>
+      <c r="G34" s="42"/>
+      <c r="I34" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="J34" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="K34" s="17"/>
+      <c r="M34" t="s">
+        <v>199</v>
+      </c>
+      <c r="N34" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="O34" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="P34" s="43" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="I35" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="J35" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="K35" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="M35" t="s">
+        <v>192</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O35" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="P35" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="36" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E36" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="I36" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="J36" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="K36" s="17"/>
+    </row>
+    <row r="37" spans="5:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="E37" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="G37" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="I37" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="J37" s="49" t="s">
+        <v>209</v>
+      </c>
+      <c r="K37" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="N37" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="O37" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="P37" s="43" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E38" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="F38" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="I38" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="J38" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="K38" s="17"/>
+      <c r="N38" t="s">
+        <v>193</v>
+      </c>
+      <c r="O38" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="P38" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="39" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E39" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="F39" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="G39" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="N39" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="O39" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="P39" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="40" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="N40" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="P40" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="41" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="I41" t="s">
+        <v>187</v>
+      </c>
+      <c r="N41" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="42" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="N42" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="43" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="N43" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="F11:J11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E6:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>216</v>
+      </c>
+      <c r="F6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="7" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="48" t="s">
+        <v>217</v>
+      </c>
+      <c r="F8" s="46" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="47" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>180</v>
+      </c>
+      <c r="F12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>218</v>
+      </c>
+      <c r="F13" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Application - Doctoral Chemistry Research PDH - in-progress
</commit_message>
<xml_diff>
--- a/src/test/java/BaseFramework/Data/DA.xlsx
+++ b/src/test/java/BaseFramework/Data/DA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14445" windowHeight="8160" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14445" windowHeight="8160" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Create Account" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Drop Down Values" sheetId="6" r:id="rId6"/>
     <sheet name="Requirments Sheet" sheetId="3" r:id="rId7"/>
     <sheet name="Sheet3" sheetId="9" r:id="rId8"/>
+    <sheet name="Result Summary" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="295">
   <si>
     <t>First Name</t>
   </si>
@@ -603,31 +604,7 @@
     <t>Visiting Student (Non Degree), Summer School, Pre-sessional English</t>
   </si>
   <si>
-    <t>Pre-Sessional English Programme (12 week)</t>
-  </si>
-  <si>
-    <t>Mathematics Research (Occasional FT)</t>
-  </si>
-  <si>
-    <t>Mastering Lab Skills</t>
-  </si>
-  <si>
     <t>PGTR</t>
-  </si>
-  <si>
-    <t>Advanced Chemical Engineering (MSc 1YFT)</t>
-  </si>
-  <si>
-    <t>Human Vaccinology (MRes 1YFT)</t>
-  </si>
-  <si>
-    <t>Business Analytics (MSc 1YFT)</t>
-  </si>
-  <si>
-    <t>Management (MBA 1YFT)</t>
-  </si>
-  <si>
-    <t>Medical Sciences with Humanities, Philosophy and Law BSc (1YFT - Intercalated)</t>
   </si>
   <si>
     <t>Chemistry Research (PhD)</t>
@@ -724,21 +701,12 @@
     <t>Chemistry</t>
   </si>
   <si>
-    <t>d.chemistry@mailinator.com</t>
-  </si>
-  <si>
     <t>Drop</t>
   </si>
   <si>
     <t>Oct218</t>
   </si>
   <si>
-    <t>Drop18</t>
-  </si>
-  <si>
-    <t>ICLDrop</t>
-  </si>
-  <si>
     <t>NylahaDROP</t>
   </si>
   <si>
@@ -751,23 +719,239 @@
     <t>I.Craneoct18@mailinator.com</t>
   </si>
   <si>
-    <t>ju.Kentoct18@mailinator.com</t>
-  </si>
-  <si>
-    <t>c.Stevensoct18@mailinator.com</t>
-  </si>
-  <si>
     <t>Oct18Drop</t>
   </si>
   <si>
     <t>OctDeferal</t>
+  </si>
+  <si>
+    <t>Scholarship</t>
+  </si>
+  <si>
+    <t>200 Broadway Av</t>
+  </si>
+  <si>
+    <t>NEW CANBERRA</t>
+  </si>
+  <si>
+    <t>Western Australia</t>
+  </si>
+  <si>
+    <t>5024</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>MBBS Degree from Overseas Institution</t>
+  </si>
+  <si>
+    <t>MBBS Medicine</t>
+  </si>
+  <si>
+    <t>Medical Research Council Funding</t>
+  </si>
+  <si>
+    <t>Postgraduate Research</t>
+  </si>
+  <si>
+    <t>Business Analytics (MSc 1YFT) - Business school taught</t>
+  </si>
+  <si>
+    <t>Human Vaccinology (MRes 1YFT) - Postgraduate Taught</t>
+  </si>
+  <si>
+    <t>Advanced Chemical Engineering (MSc 1YFT) - Post graduate Taught</t>
+  </si>
+  <si>
+    <t>Management (MBA 1YFT) - Business school MBA</t>
+  </si>
+  <si>
+    <t>Medical Sciences with Humanities, Philosophy and Law BSc (1YFT - Intercalated) - Intercalated</t>
+  </si>
+  <si>
+    <t>Short course</t>
+  </si>
+  <si>
+    <t>Pre-Sessional English Programme (12 week) - Presesional</t>
+  </si>
+  <si>
+    <t>Mathematics Research (Occasional FT) - Visiting non degree</t>
+  </si>
+  <si>
+    <t>Mastering Lab Skills- Visting Non degree</t>
+  </si>
+  <si>
+    <t>c.Stevensoct18test@mailinator.com</t>
+  </si>
+  <si>
+    <t>ICLDropDEVL</t>
+  </si>
+  <si>
+    <t>Drop18devl</t>
+  </si>
+  <si>
+    <t>ju.Kentoct18DEVL@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Student - Create Account </t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Student - Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Student - Logout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Student – Complete Application </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DA WFE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login and Logout - Super User (crmrec1)  </t>
+  </si>
+  <si>
+    <t>Login and Logout - Registry User (crmrec2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login and Logout - - Department Recorder  (crmrec3) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login and Logout - Department Reviewer (crmrec4) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application - Offer Made </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application - Reject  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application - Reject at Source </t>
+  </si>
+  <si>
+    <t>DA CRM Recruit</t>
+  </si>
+  <si>
+    <t>TEST ENV</t>
+  </si>
+  <si>
+    <t>DEVL ENV</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>UG CRM Recruit</t>
+  </si>
+  <si>
+    <t>Undergraduate CRM Recruit Tests</t>
+  </si>
+  <si>
+    <t>Direct Addmissions Web front end and CRM Recruit Tests</t>
+  </si>
+  <si>
+    <t>DA</t>
+  </si>
+  <si>
+    <t>UG</t>
+  </si>
+  <si>
+    <t>TEST EVN</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>selected by default</t>
+  </si>
+  <si>
+    <t>s.sonnar@mailinator.com</t>
+  </si>
+  <si>
+    <t>05/09/2008 - NOT REQUIRED</t>
+  </si>
+  <si>
+    <t>Yes - NOT REQUIRED</t>
+  </si>
+  <si>
+    <t>Coventry - NOT REQUIRED</t>
+  </si>
+  <si>
+    <t>Chemistry Research (PhD) - NOT REQUIRED</t>
+  </si>
+  <si>
+    <t>NOT REQUIRED</t>
+  </si>
+  <si>
+    <t>IELTS (Academic)</t>
+  </si>
+  <si>
+    <t>IELTS Exam Date Taken</t>
+  </si>
+  <si>
+    <t>IELTS Test Report Form Number</t>
+  </si>
+  <si>
+    <t>000119</t>
+  </si>
+  <si>
+    <t>IELTS Score</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Non-Imperial</t>
+  </si>
+  <si>
+    <t>Name of Scholarship</t>
+  </si>
+  <si>
+    <t>Common Wealth Scholarship</t>
+  </si>
+  <si>
+    <t>Award Amount</t>
+  </si>
+  <si>
+    <t>Fees/Maintenance/Both</t>
+  </si>
+  <si>
+    <t>Award Status</t>
+  </si>
+  <si>
+    <t>If you do not have scholarship support, will you still be able to fund your studies?</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>25000</t>
+  </si>
+  <si>
+    <t>Confirmed</t>
+  </si>
+  <si>
+    <t>Asian - Chinese</t>
+  </si>
+  <si>
+    <t>d29.chemistry@mailinator.com</t>
+  </si>
+  <si>
+    <t>Doctoral29</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+  </numFmts>
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -850,8 +1034,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF1F497D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -893,8 +1107,68 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3300"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -1141,13 +1415,72 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1211,6 +1544,72 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="15" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="17" fontId="3" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="3" fillId="3" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent5" xfId="1" builtinId="45"/>
@@ -1221,6 +1620,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF3300"/>
+      <color rgb="FFA50021"/>
+      <color rgb="FFD60093"/>
+      <color rgb="FFFF6600"/>
       <color rgb="FFF1C5E5"/>
     </mruColors>
   </colors>
@@ -1757,7 +2160,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
@@ -1765,7 +2168,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
@@ -1792,7 +2195,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
@@ -1919,7 +2322,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1927,7 +2330,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -1967,7 +2370,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -2642,7 +3045,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'Drop Down Values'!$C$30:$C$31</xm:f>
+            <xm:f>'Drop Down Values'!$C$31:$C$32</xm:f>
           </x14:formula1>
           <xm:sqref>B17</xm:sqref>
         </x14:dataValidation>
@@ -2663,8 +3066,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2692,7 +3095,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>225</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -2700,7 +3103,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -2740,7 +3143,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>231</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -3397,7 +3800,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'Drop Down Values'!$C$30:$C$31</xm:f>
+            <xm:f>'Drop Down Values'!$C$31:$C$32</xm:f>
           </x14:formula1>
           <xm:sqref>B17</xm:sqref>
         </x14:dataValidation>
@@ -3436,8 +3839,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3465,7 +3868,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -3473,7 +3876,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -3513,7 +3916,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -4188,7 +4591,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'Drop Down Values'!$C$30:$C$31</xm:f>
+            <xm:f>'Drop Down Values'!$C$31:$C$32</xm:f>
           </x14:formula1>
           <xm:sqref>B17</xm:sqref>
         </x14:dataValidation>
@@ -4207,18 +4610,17 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:K101"/>
+  <dimension ref="A1:K106"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="89.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="6" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -4238,7 +4640,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>137</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -4246,7 +4648,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -4286,7 +4688,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>222</v>
+        <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -4294,7 +4696,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>13</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -4302,7 +4704,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>12</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -4353,32 +4755,38 @@
         <v>26</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>27</v>
+        <v>231</v>
       </c>
       <c r="C16" s="28" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="54" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+        <v>275</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B18" s="54" t="s">
+        <v>274</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>29</v>
       </c>
@@ -4386,7 +4794,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>30</v>
       </c>
@@ -4394,96 +4802,99 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+      <c r="D21" s="86" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>44</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>37</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>40</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B29" s="53" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B30" s="10" t="s">
-        <v>18</v>
+      <c r="B30" s="54" t="s">
+        <v>271</v>
       </c>
       <c r="C30" s="28"/>
     </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B31" s="54" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>42</v>
       </c>
@@ -4556,7 +4967,7 @@
         <v>59</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>69</v>
+        <v>228</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
@@ -4564,7 +4975,7 @@
         <v>60</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>70</v>
+        <v>229</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
@@ -4657,12 +5068,12 @@
         <v>82</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>83</v>
+        <v>276</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
-        <v>84</v>
+        <v>277</v>
       </c>
       <c r="B60" s="15" t="s">
         <v>80</v>
@@ -4670,18 +5081,18 @@
     </row>
     <row r="61" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
-        <v>85</v>
+        <v>278</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>102</v>
+        <v>279</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A62" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="B62" s="87" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -4694,222 +5105,264 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="B67" s="6"/>
+      <c r="B66" s="6"/>
+    </row>
+    <row r="67" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A67" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B67" s="12" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="68" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A68" s="7" t="s">
-        <v>106</v>
+        <v>222</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="B71" s="13" t="s">
-        <v>112</v>
+        <v>282</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A69" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="B69" s="12" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A70" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="B70" s="88" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A71" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="B71" s="12" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A72" s="7" t="s">
-        <v>114</v>
+        <v>287</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>119</v>
+        <v>291</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A73" s="7" t="s">
-        <v>115</v>
+        <v>288</v>
       </c>
       <c r="B73" s="12" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A74" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B74" s="12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="B77" s="13" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B76" s="13" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A77" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B77" s="12" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A78" s="7" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A79" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B79" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B82" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A83" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B83" s="12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A84" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B79" s="12" t="s">
+      <c r="B84" s="12" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="13" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="B84" s="13" t="s">
+      <c r="B89" s="13" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A85" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B85" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A86" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="B86" s="12" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A87" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="B87" s="12" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A88" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="B88" s="12" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A89" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="B89" s="12" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A90" s="7" t="s">
-        <v>154</v>
+        <v>20</v>
       </c>
       <c r="B90" s="12" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A91" s="7" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B91" s="12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="B94" s="13" t="s">
-        <v>112</v>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A92" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B92" s="12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A93" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B93" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A94" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B94" s="12" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A95" s="7" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="B95" s="12" t="s">
-        <v>21</v>
+        <v>157</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A96" s="7" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B96" s="12" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A97" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="B97" s="12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A98" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="B98" s="12" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A99" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="B99" s="12" t="s">
-        <v>166</v>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B99" s="13" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A100" s="7" t="s">
-        <v>154</v>
+        <v>20</v>
       </c>
       <c r="B100" s="12" t="s">
-        <v>165</v>
+        <v>21</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A101" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B101" s="12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A102" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B102" s="12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A103" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B103" s="12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A104" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B104" s="12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A105" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B105" s="12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A106" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="B101" s="12" t="s">
+      <c r="B106" s="12" t="s">
         <v>167</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="D21" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="14337" r:id="rId4" name="Control 1">
-          <controlPr defaultSize="0" r:id="rId5">
+        <control shapeId="14337" r:id="rId6" name="Control 1">
+          <controlPr defaultSize="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -4928,7 +5381,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="14337" r:id="rId4" name="Control 1"/>
+        <control shapeId="14337" r:id="rId6" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -4943,13 +5396,13 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'Drop Down Values'!$C$30:$C$31</xm:f>
+            <xm:f>'Drop Down Values'!$C$31:$C$32</xm:f>
           </x14:formula1>
           <xm:sqref>B17</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'Drop Down Values'!$C$22:$C$27</xm:f>
+            <xm:f>'Drop Down Values'!$C$22:$C$29</xm:f>
           </x14:formula1>
           <xm:sqref>B16</xm:sqref>
         </x14:dataValidation>
@@ -4979,10 +5432,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5158,18 +5611,24 @@
         <v>144</v>
       </c>
     </row>
-    <row r="29" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="2:3" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B30" s="31" t="s">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="55"/>
+      <c r="C28" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="2:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B31" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="C30" s="23" t="s">
+      <c r="C31" s="23" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="31" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="21"/>
-      <c r="C31" s="26" t="s">
+    <row r="32" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="21"/>
+      <c r="C32" s="26" t="s">
         <v>14</v>
       </c>
     </row>
@@ -5185,8 +5644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E11:P43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5198,14 +5657,14 @@
     <col min="9" max="9" width="25.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="33.42578125" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="41" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="30.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="81.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="30.85546875" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="70" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="11" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F11" s="50" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="G11" s="50"/>
       <c r="H11" s="50"/>
@@ -5233,10 +5692,10 @@
         <v>94</v>
       </c>
       <c r="I14" s="19" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="J14" s="19" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="5:12" x14ac:dyDescent="0.25">
@@ -5250,7 +5709,7 @@
         <v>95</v>
       </c>
       <c r="I15" s="42" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="J15" s="42" t="s">
         <v>51</v>
@@ -5280,7 +5739,7 @@
         <v>2516</v>
       </c>
     </row>
-    <row r="17" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F17" s="41" t="s">
         <v>100</v>
       </c>
@@ -5292,7 +5751,7 @@
       </c>
       <c r="I17" s="17"/>
     </row>
-    <row r="18" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F18" s="41" t="s">
         <v>97</v>
       </c>
@@ -5302,7 +5761,7 @@
       <c r="H18" s="17"/>
       <c r="I18" s="17"/>
     </row>
-    <row r="19" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F19" s="41"/>
       <c r="G19" s="17" t="s">
         <v>97</v>
@@ -5310,32 +5769,50 @@
       <c r="H19" s="17"/>
       <c r="I19" s="17"/>
     </row>
-    <row r="21" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F21" s="2"/>
     </row>
-    <row r="23" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:15" x14ac:dyDescent="0.25">
       <c r="N23" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="26" spans="6:14" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="26" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F27" s="18" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="28" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F28" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F29" s="20" t="s">
         <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="O31" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="O32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="O33" t="s">
+        <v>222</v>
+      </c>
+      <c r="P33" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="34" spans="5:16" x14ac:dyDescent="0.25">
@@ -5352,7 +5829,7 @@
       </c>
       <c r="K34" s="17"/>
       <c r="M34" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="N34" s="39" t="s">
         <v>136</v>
@@ -5375,7 +5852,7 @@
         <v>183</v>
       </c>
       <c r="K35" s="17" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="M35" t="s">
         <v>186</v>
@@ -5404,7 +5881,7 @@
         <v>182</v>
       </c>
       <c r="J36" s="17" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="K36" s="17"/>
     </row>
@@ -5419,10 +5896,10 @@
         <v>178</v>
       </c>
       <c r="I37" s="17" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="J37" s="45" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="K37" s="17" t="s">
         <v>185</v>
@@ -5442,16 +5919,16 @@
         <v>178</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="G38" s="17" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="I38" s="17" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="J38" s="17" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="K38" s="17"/>
       <c r="N38" t="s">
@@ -5461,7 +5938,7 @@
         <v>188</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>190</v>
+        <v>238</v>
       </c>
     </row>
     <row r="39" spans="5:16" x14ac:dyDescent="0.25">
@@ -5469,22 +5946,22 @@
         <v>178</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="G39" s="17" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="M39" t="s">
         <v>24</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>194</v>
+        <v>234</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>199</v>
+        <v>230</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>191</v>
+        <v>239</v>
       </c>
     </row>
     <row r="40" spans="5:16" x14ac:dyDescent="0.25">
@@ -5495,10 +5972,13 @@
         <v>23</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>195</v>
+        <v>233</v>
+      </c>
+      <c r="O40" s="2" t="s">
+        <v>191</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>192</v>
+        <v>240</v>
       </c>
     </row>
     <row r="41" spans="5:16" x14ac:dyDescent="0.25">
@@ -5512,17 +5992,20 @@
         <v>23</v>
       </c>
       <c r="N41" s="2" t="s">
-        <v>196</v>
+        <v>232</v>
+      </c>
+      <c r="O41" s="2" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="42" spans="5:16" x14ac:dyDescent="0.25">
       <c r="N42" s="2" t="s">
-        <v>197</v>
+        <v>235</v>
       </c>
     </row>
     <row r="43" spans="5:16" x14ac:dyDescent="0.25">
       <c r="N43" s="2" t="s">
-        <v>198</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -5540,7 +6023,7 @@
   <dimension ref="E6:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E7" sqref="E7:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5551,23 +6034,23 @@
   <sheetData>
     <row r="6" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
+        <v>202</v>
+      </c>
+      <c r="F6" t="s">
         <v>210</v>
-      </c>
-      <c r="F6" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="7" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E7" s="44" t="s">
+        <v>201</v>
+      </c>
+      <c r="F7" s="19" t="s">
         <v>209</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="8" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E8" s="44" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="F8" s="42" t="s">
         <v>51</v>
@@ -5583,18 +6066,617 @@
         <v>174</v>
       </c>
       <c r="F12" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="F13" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:P33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="58"/>
+    <col min="3" max="3" width="4.140625" style="58" customWidth="1"/>
+    <col min="4" max="4" width="48.7109375" style="58" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="59"/>
+    <col min="6" max="7" width="3.7109375" style="58" customWidth="1"/>
+    <col min="8" max="8" width="3.42578125" style="58" customWidth="1"/>
+    <col min="9" max="9" width="48.7109375" style="58" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="59"/>
+    <col min="11" max="11" width="4.140625" style="58" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="58"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="83" t="s">
+        <v>264</v>
+      </c>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="85"/>
+      <c r="M3" s="70" t="s">
+        <v>260</v>
+      </c>
+      <c r="N3" s="70"/>
+      <c r="O3" s="70"/>
+    </row>
+    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C4" s="60"/>
+      <c r="D4" s="76" t="s">
+        <v>259</v>
+      </c>
+      <c r="E4" s="76"/>
+      <c r="F4" s="77"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="76" t="s">
+        <v>260</v>
+      </c>
+      <c r="J4" s="76"/>
+      <c r="K4" s="61"/>
+      <c r="M4" s="71" t="s">
+        <v>268</v>
+      </c>
+      <c r="N4" s="71" t="s">
+        <v>246</v>
+      </c>
+      <c r="O4" s="71" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C5" s="60"/>
+      <c r="D5" s="80" t="s">
+        <v>250</v>
+      </c>
+      <c r="E5" s="80"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="80" t="s">
+        <v>250</v>
+      </c>
+      <c r="J5" s="80"/>
+      <c r="K5" s="61"/>
+      <c r="M5" s="71" t="s">
+        <v>265</v>
+      </c>
+      <c r="N5" s="72">
+        <v>12</v>
+      </c>
+      <c r="O5" s="73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C6" s="60"/>
+      <c r="D6" s="74" t="s">
+        <v>245</v>
+      </c>
+      <c r="E6" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="F6" s="61"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="74" t="s">
+        <v>245</v>
+      </c>
+      <c r="J6" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="K6" s="61"/>
+      <c r="M6" s="71" t="s">
+        <v>266</v>
+      </c>
+      <c r="N6" s="72">
+        <v>7</v>
+      </c>
+      <c r="O6" s="73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C7" s="60"/>
+      <c r="D7" s="74" t="s">
+        <v>247</v>
+      </c>
+      <c r="E7" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="F7" s="61"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="74" t="s">
+        <v>247</v>
+      </c>
+      <c r="J7" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="K7" s="61"/>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C8" s="60"/>
+      <c r="D8" s="74" t="s">
+        <v>248</v>
+      </c>
+      <c r="E8" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="F8" s="61"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="74" t="s">
+        <v>248</v>
+      </c>
+      <c r="J8" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="K8" s="61"/>
+    </row>
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C9" s="60"/>
+      <c r="D9" s="74" t="s">
+        <v>249</v>
+      </c>
+      <c r="E9" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="F9" s="61"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="60"/>
+      <c r="I9" s="74" t="s">
+        <v>249</v>
+      </c>
+      <c r="J9" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="K9" s="61"/>
+    </row>
+    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C10" s="60"/>
+      <c r="D10" s="74" t="s">
+        <v>249</v>
+      </c>
+      <c r="E10" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="F10" s="61"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="60"/>
+      <c r="I10" s="74" t="s">
+        <v>249</v>
+      </c>
+      <c r="J10" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="K10" s="61"/>
+    </row>
+    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C11" s="60"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="60"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="61"/>
+    </row>
+    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C12" s="60"/>
+      <c r="D12" s="80" t="s">
+        <v>258</v>
+      </c>
+      <c r="E12" s="80"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="78"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="80" t="s">
+        <v>258</v>
+      </c>
+      <c r="J12" s="80"/>
+      <c r="K12" s="61"/>
+    </row>
+    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C13" s="60"/>
+      <c r="D13" s="74" t="s">
+        <v>251</v>
+      </c>
+      <c r="E13" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="F13" s="61"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="60"/>
+      <c r="I13" s="74" t="s">
+        <v>251</v>
+      </c>
+      <c r="J13" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="K13" s="61"/>
+    </row>
+    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C14" s="60"/>
+      <c r="D14" s="74" t="s">
+        <v>252</v>
+      </c>
+      <c r="E14" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="F14" s="61"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="74" t="s">
+        <v>252</v>
+      </c>
+      <c r="J14" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="K14" s="61"/>
+    </row>
+    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C15" s="60"/>
+      <c r="D15" s="74" t="s">
+        <v>253</v>
+      </c>
+      <c r="E15" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="F15" s="61"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="60"/>
+      <c r="I15" s="74" t="s">
+        <v>253</v>
+      </c>
+      <c r="J15" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="K15" s="61"/>
+    </row>
+    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C16" s="60"/>
+      <c r="D16" s="74" t="s">
+        <v>254</v>
+      </c>
+      <c r="E16" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="F16" s="61"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="74" t="s">
+        <v>254</v>
+      </c>
+      <c r="J16" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="K16" s="61"/>
+      <c r="O16" s="64"/>
+      <c r="P16" s="65"/>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C17" s="60"/>
+      <c r="D17" s="74" t="s">
+        <v>255</v>
+      </c>
+      <c r="E17" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="F17" s="61"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="74" t="s">
+        <v>255</v>
+      </c>
+      <c r="J17" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="K17" s="61"/>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C18" s="60"/>
+      <c r="D18" s="74" t="s">
+        <v>256</v>
+      </c>
+      <c r="E18" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="F18" s="61"/>
+      <c r="G18" s="62"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="74" t="s">
+        <v>256</v>
+      </c>
+      <c r="J18" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="K18" s="61"/>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C19" s="60"/>
+      <c r="D19" s="74" t="s">
+        <v>257</v>
+      </c>
+      <c r="E19" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="F19" s="61"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="60"/>
+      <c r="I19" s="74" t="s">
+        <v>257</v>
+      </c>
+      <c r="J19" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="K19" s="61"/>
+    </row>
+    <row r="20" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="66"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="68"/>
+      <c r="F20" s="69"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="66"/>
+      <c r="I20" s="67"/>
+      <c r="J20" s="68"/>
+      <c r="K20" s="69"/>
+    </row>
+    <row r="22" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="83" t="s">
+        <v>263</v>
+      </c>
+      <c r="D23" s="84"/>
+      <c r="E23" s="84"/>
+      <c r="F23" s="84"/>
+      <c r="G23" s="84"/>
+      <c r="H23" s="84"/>
+      <c r="I23" s="84"/>
+      <c r="J23" s="84"/>
+      <c r="K23" s="85"/>
+      <c r="M23" s="70" t="s">
+        <v>267</v>
+      </c>
+      <c r="N23" s="70"/>
+      <c r="O23" s="70"/>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C24" s="60"/>
+      <c r="D24" s="76" t="s">
+        <v>259</v>
+      </c>
+      <c r="E24" s="76"/>
+      <c r="F24" s="77"/>
+      <c r="G24" s="81"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="82" t="s">
+        <v>260</v>
+      </c>
+      <c r="J24" s="82"/>
+      <c r="K24" s="61"/>
+      <c r="M24" s="71" t="s">
+        <v>268</v>
+      </c>
+      <c r="N24" s="71" t="s">
+        <v>246</v>
+      </c>
+      <c r="O24" s="71" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C25" s="60"/>
+      <c r="D25" s="80" t="s">
+        <v>262</v>
+      </c>
+      <c r="E25" s="80"/>
+      <c r="F25" s="77"/>
+      <c r="G25" s="81"/>
+      <c r="H25" s="79"/>
+      <c r="I25" s="80" t="s">
+        <v>262</v>
+      </c>
+      <c r="J25" s="80"/>
+      <c r="K25" s="61"/>
+      <c r="M25" s="71" t="s">
+        <v>265</v>
+      </c>
+      <c r="N25" s="72">
+        <v>12</v>
+      </c>
+      <c r="O25" s="73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C26" s="60"/>
+      <c r="D26" s="74" t="s">
+        <v>251</v>
+      </c>
+      <c r="E26" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="F26" s="61"/>
+      <c r="H26" s="60"/>
+      <c r="I26" s="74" t="s">
+        <v>251</v>
+      </c>
+      <c r="J26" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="K26" s="61"/>
+      <c r="M26" s="71" t="s">
+        <v>266</v>
+      </c>
+      <c r="N26" s="72">
+        <v>4</v>
+      </c>
+      <c r="O26" s="73">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C27" s="60"/>
+      <c r="D27" s="74" t="s">
+        <v>252</v>
+      </c>
+      <c r="E27" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="F27" s="61"/>
+      <c r="H27" s="60"/>
+      <c r="I27" s="74" t="s">
+        <v>252</v>
+      </c>
+      <c r="J27" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="K27" s="61"/>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C28" s="60"/>
+      <c r="D28" s="74" t="s">
+        <v>253</v>
+      </c>
+      <c r="E28" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="F28" s="61"/>
+      <c r="H28" s="60"/>
+      <c r="I28" s="74" t="s">
+        <v>253</v>
+      </c>
+      <c r="J28" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="K28" s="61"/>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C29" s="60"/>
+      <c r="D29" s="74" t="s">
+        <v>254</v>
+      </c>
+      <c r="E29" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="F29" s="61"/>
+      <c r="H29" s="60"/>
+      <c r="I29" s="74" t="s">
+        <v>254</v>
+      </c>
+      <c r="J29" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="K29" s="61"/>
+    </row>
+    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C30" s="60"/>
+      <c r="D30" s="75" t="s">
+        <v>255</v>
+      </c>
+      <c r="E30" s="57" t="s">
+        <v>261</v>
+      </c>
+      <c r="F30" s="61"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="74" t="s">
+        <v>255</v>
+      </c>
+      <c r="J30" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="K30" s="61"/>
+    </row>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C31" s="60"/>
+      <c r="D31" s="75" t="s">
+        <v>256</v>
+      </c>
+      <c r="E31" s="57" t="s">
+        <v>261</v>
+      </c>
+      <c r="F31" s="61"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="74" t="s">
+        <v>256</v>
+      </c>
+      <c r="J31" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="K31" s="61"/>
+    </row>
+    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C32" s="60"/>
+      <c r="D32" s="75" t="s">
+        <v>257</v>
+      </c>
+      <c r="E32" s="57" t="s">
+        <v>261</v>
+      </c>
+      <c r="F32" s="61"/>
+      <c r="H32" s="60"/>
+      <c r="I32" s="74" t="s">
+        <v>257</v>
+      </c>
+      <c r="J32" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="K32" s="61"/>
+    </row>
+    <row r="33" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="66"/>
+      <c r="D33" s="67"/>
+      <c r="E33" s="68"/>
+      <c r="F33" s="69"/>
+      <c r="H33" s="66"/>
+      <c r="I33" s="67"/>
+      <c r="J33" s="68"/>
+      <c r="K33" s="69"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="C23:K23"/>
+    <mergeCell ref="C3:K3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="I4:J4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Application - Doctoral Chemistry Research PDH - Completed End to End
</commit_message>
<xml_diff>
--- a/src/test/java/BaseFramework/Data/DA.xlsx
+++ b/src/test/java/BaseFramework/Data/DA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14445" windowHeight="8160" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14445" windowHeight="8160" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Create Account" sheetId="1" r:id="rId1"/>
@@ -938,10 +938,10 @@
     <t>Asian - Chinese</t>
   </si>
   <si>
-    <t>d29.chemistry@mailinator.com</t>
-  </si>
-  <si>
-    <t>Doctoral29</t>
+    <t>Doctoral37</t>
+  </si>
+  <si>
+    <t>d37.chemistry@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -3066,8 +3066,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3839,8 +3839,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4613,7 +4613,7 @@
   <dimension ref="A1:K106"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4640,7 +4640,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -4688,7 +4688,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Moved Recruit Folders in under Main folders.
</commit_message>
<xml_diff>
--- a/src/test/java/BaseFramework/Data/DA.xlsx
+++ b/src/test/java/BaseFramework/Data/DA.xlsx
@@ -938,10 +938,10 @@
     <t>Asian - Chinese</t>
   </si>
   <si>
-    <t>Doctoral37</t>
-  </si>
-  <si>
-    <t>d37.chemistry@mailinator.com</t>
+    <t>Doctoral38</t>
+  </si>
+  <si>
+    <t>d38.chemistry@mailinator.com</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Data Generator PGT_Create_Account Files Added
</commit_message>
<xml_diff>
--- a/src/test/java/BaseFramework/Data/DA.xlsx
+++ b/src/test/java/BaseFramework/Data/DA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14445" windowHeight="8160" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14445" windowHeight="8160" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Create Account" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="302">
   <si>
     <t>First Name</t>
   </si>
@@ -695,9 +695,6 @@
     <t>Assgine , Steps Required</t>
   </si>
   <si>
-    <t>Doctoral_ChemistryResearch_PHD_Programme_StepDefs</t>
-  </si>
-  <si>
     <t>Chemistry</t>
   </si>
   <si>
@@ -770,9 +767,6 @@
     <t>Medical Sciences with Humanities, Philosophy and Law BSc (1YFT - Intercalated) - Intercalated</t>
   </si>
   <si>
-    <t>Short course</t>
-  </si>
-  <si>
     <t>Pre-Sessional English Programme (12 week) - Presesional</t>
   </si>
   <si>
@@ -869,9 +863,6 @@
     <t>selected by default</t>
   </si>
   <si>
-    <t>s.sonnar@mailinator.com</t>
-  </si>
-  <si>
     <t>05/09/2008 - NOT REQUIRED</t>
   </si>
   <si>
@@ -938,10 +929,40 @@
     <t>Asian - Chinese</t>
   </si>
   <si>
-    <t>Doctoral38</t>
-  </si>
-  <si>
-    <t>d38.chemistry@mailinator.com</t>
+    <t>Doctoral39</t>
+  </si>
+  <si>
+    <t>d39.chemistry@mailinator.com</t>
+  </si>
+  <si>
+    <t>Course Type</t>
+  </si>
+  <si>
+    <t>Academice Programme</t>
+  </si>
+  <si>
+    <t>IETLS</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Criminal</t>
+  </si>
+  <si>
+    <t>ScholarShip</t>
+  </si>
+  <si>
+    <t>Disability</t>
+  </si>
+  <si>
+    <t>Select course type - Postgraduate Research</t>
+  </si>
+  <si>
+    <t>Select course type - Postgraduate Taught</t>
+  </si>
+  <si>
+    <t>Select course type - Short course</t>
   </si>
 </sst>
 </file>
@@ -1480,7 +1501,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1533,15 +1554,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="15" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="17" fontId="3" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1571,9 +1583,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1585,17 +1594,26 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="3" fillId="3" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1607,9 +1625,21 @@
     <xf numFmtId="0" fontId="13" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="6" fontId="3" fillId="3" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent5" xfId="1" builtinId="45"/>
@@ -2160,7 +2190,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
@@ -2168,7 +2198,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
@@ -2194,8 +2224,8 @@
       <c r="A8" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="51" t="s">
-        <v>218</v>
+      <c r="B8" s="48" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
@@ -2322,7 +2352,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -2330,7 +2360,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -2369,8 +2399,8 @@
       <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="51" t="s">
-        <v>219</v>
+      <c r="B6" s="48" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -3095,7 +3125,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -3103,7 +3133,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -3142,8 +3172,8 @@
       <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="51" t="s">
-        <v>244</v>
+      <c r="B6" s="48" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -3868,15 +3898,15 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="52" t="s">
-        <v>220</v>
+      <c r="B3" s="49" t="s">
+        <v>219</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -3915,8 +3945,8 @@
       <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="51" t="s">
-        <v>241</v>
+      <c r="B6" s="48" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -4612,8 +4642,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:K106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4640,7 +4670,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -4648,7 +4678,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -4687,8 +4717,8 @@
       <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="51" t="s">
-        <v>294</v>
+      <c r="B6" s="48" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -4706,6 +4736,9 @@
       <c r="B8" s="10" t="s">
         <v>191</v>
       </c>
+      <c r="D8" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
@@ -4755,7 +4788,7 @@
         <v>26</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C16" s="28" t="s">
         <v>139</v>
@@ -4765,25 +4798,25 @@
       <c r="A17" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="51" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B18" s="54" t="s">
-        <v>274</v>
+      <c r="B18" s="51" t="s">
+        <v>271</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
@@ -4807,18 +4840,16 @@
         <v>32</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="D21" s="86" t="s">
-        <v>270</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="D21" s="76"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
@@ -4826,7 +4857,7 @@
         <v>44</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
@@ -4834,7 +4865,7 @@
         <v>37</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
@@ -4842,7 +4873,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
@@ -4850,7 +4881,7 @@
         <v>39</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
@@ -4858,7 +4889,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
@@ -4866,23 +4897,23 @@
         <v>41</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="53" t="s">
-        <v>273</v>
+      <c r="B29" s="50" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B30" s="54" t="s">
-        <v>271</v>
+      <c r="B30" s="51" t="s">
+        <v>268</v>
       </c>
       <c r="C30" s="28"/>
     </row>
@@ -4890,8 +4921,8 @@
       <c r="A31" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="54" t="s">
-        <v>272</v>
+      <c r="B31" s="51" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
@@ -4967,7 +4998,7 @@
         <v>59</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
@@ -4975,7 +5006,7 @@
         <v>60</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
@@ -5068,12 +5099,12 @@
         <v>82</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B60" s="15" t="s">
         <v>80</v>
@@ -5081,18 +5112,18 @@
     </row>
     <row r="61" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="B62" s="87" t="s">
-        <v>281</v>
+        <v>277</v>
+      </c>
+      <c r="B62" s="77" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -5114,52 +5145,52 @@
         <v>106</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A68" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A69" s="7" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A70" s="7" t="s">
-        <v>285</v>
-      </c>
-      <c r="B70" s="88" t="s">
-        <v>290</v>
+        <v>282</v>
+      </c>
+      <c r="B70" s="78" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="B71" s="12" t="s">
         <v>286</v>
-      </c>
-      <c r="B71" s="12" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A72" s="7" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A73" s="7" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B73" s="12" t="s">
         <v>52</v>
@@ -5178,7 +5209,7 @@
         <v>114</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
@@ -5352,17 +5383,16 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1"/>
-    <hyperlink ref="D21" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-  <drawing r:id="rId4"/>
-  <legacyDrawing r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="14337" r:id="rId6" name="Control 1">
-          <controlPr defaultSize="0" r:id="rId7">
+        <control shapeId="14337" r:id="rId5" name="Control 1">
+          <controlPr defaultSize="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -5381,7 +5411,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="14337" r:id="rId6" name="Control 1"/>
+        <control shapeId="14337" r:id="rId5" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -5446,15 +5476,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="79" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5612,9 +5642,9 @@
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="55"/>
+      <c r="B28" s="52"/>
       <c r="C28" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5642,46 +5672,49 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E11:P43"/>
+  <dimension ref="B11:P49"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+    <sheetView topLeftCell="L23" workbookViewId="0">
+      <selection activeCell="O43" sqref="O43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="20.7109375" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="25.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="33.42578125" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="81.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="44.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="70" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="11" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="F11" s="50" t="s">
+    <row r="11" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="F11" s="81" t="s">
         <v>207</v>
       </c>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="50"/>
-    </row>
-    <row r="12" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="G11" s="81"/>
+      <c r="H11" s="81"/>
+      <c r="I11" s="81"/>
+      <c r="J11" s="81"/>
+    </row>
+    <row r="12" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="13" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="14" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F14" s="40" t="s">
         <v>87</v>
       </c>
@@ -5697,8 +5730,11 @@
       <c r="J14" s="19" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="15" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="O14" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="15" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F15" s="41" t="s">
         <v>89</v>
       </c>
@@ -5715,7 +5751,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>185</v>
       </c>
@@ -5739,7 +5775,7 @@
         <v>2516</v>
       </c>
     </row>
-    <row r="17" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F17" s="41" t="s">
         <v>100</v>
       </c>
@@ -5751,7 +5787,7 @@
       </c>
       <c r="I17" s="17"/>
     </row>
-    <row r="18" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F18" s="41" t="s">
         <v>97</v>
       </c>
@@ -5761,7 +5797,7 @@
       <c r="H18" s="17"/>
       <c r="I18" s="17"/>
     </row>
-    <row r="19" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F19" s="41"/>
       <c r="G19" s="17" t="s">
         <v>97</v>
@@ -5769,58 +5805,38 @@
       <c r="H19" s="17"/>
       <c r="I19" s="17"/>
     </row>
-    <row r="21" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F21" s="2"/>
     </row>
-    <row r="23" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="N23" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="26" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F26" t="s">
+    <row r="22" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="N22" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F27" s="18" t="s">
+    <row r="23" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="N23" s="18" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="28" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F28" t="s">
+    <row r="24" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="N24" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F29" s="20" t="s">
+    <row r="25" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="N25" s="20" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="31" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="O31" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="32" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="O32" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="33" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="O33" t="s">
-        <v>222</v>
-      </c>
-      <c r="P33" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="34" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E34" s="49" t="s">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="P33" s="2"/>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E34" s="80" t="s">
         <v>173</v>
       </c>
-      <c r="F34" s="49"/>
-      <c r="G34" s="49"/>
+      <c r="F34" s="80"/>
+      <c r="G34" s="80"/>
       <c r="I34" s="17" t="s">
         <v>179</v>
       </c>
@@ -5832,16 +5848,16 @@
         <v>190</v>
       </c>
       <c r="N34" s="39" t="s">
-        <v>136</v>
+        <v>300</v>
       </c>
       <c r="O34" s="39" t="s">
-        <v>136</v>
+        <v>299</v>
       </c>
       <c r="P34" s="39" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="35" spans="5:16" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E35" s="17"/>
       <c r="F35" s="17"/>
       <c r="G35" s="17"/>
@@ -5867,7 +5883,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="36" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E36" s="17" t="s">
         <v>175</v>
       </c>
@@ -5885,7 +5901,7 @@
       </c>
       <c r="K36" s="17"/>
     </row>
-    <row r="37" spans="5:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="E37" s="17" t="s">
         <v>176</v>
       </c>
@@ -5914,7 +5930,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E38" s="17" t="s">
         <v>178</v>
       </c>
@@ -5938,10 +5954,10 @@
         <v>188</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="39" spans="5:16" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E39" s="17" t="s">
         <v>178</v>
       </c>
@@ -5955,16 +5971,16 @@
         <v>24</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="40" spans="5:16" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E40" s="17"/>
       <c r="F40" s="17"/>
       <c r="G40" s="17"/>
@@ -5972,16 +5988,16 @@
         <v>23</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="O40" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="O40" s="93" t="s">
         <v>191</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="41" spans="5:16" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E41" s="17"/>
       <c r="F41" s="17"/>
       <c r="G41" s="17"/>
@@ -5992,20 +6008,72 @@
         <v>23</v>
       </c>
       <c r="N41" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="O41" s="2" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="42" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="O41" s="2"/>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
       <c r="N42" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N43" s="2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="43" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="N43" s="2" t="s">
-        <v>236</v>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B47" s="89" t="s">
+        <v>292</v>
+      </c>
+      <c r="C47" s="89" t="s">
+        <v>293</v>
+      </c>
+      <c r="D47" s="89" t="s">
+        <v>88</v>
+      </c>
+      <c r="E47" s="89" t="s">
+        <v>294</v>
+      </c>
+      <c r="F47" s="92" t="s">
+        <v>296</v>
+      </c>
+      <c r="G47" s="92" t="s">
+        <v>297</v>
+      </c>
+      <c r="H47" s="92" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B48" s="90" t="s">
+        <v>137</v>
+      </c>
+      <c r="C48" s="90" t="s">
+        <v>191</v>
+      </c>
+      <c r="D48" s="90" t="s">
+        <v>91</v>
+      </c>
+      <c r="E48" s="91" t="s">
+        <v>295</v>
+      </c>
+      <c r="F48" s="91" t="s">
+        <v>52</v>
+      </c>
+      <c r="G48" s="91" t="s">
+        <v>52</v>
+      </c>
+      <c r="H48" s="91" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -6092,572 +6160,572 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="58"/>
-    <col min="3" max="3" width="4.140625" style="58" customWidth="1"/>
-    <col min="4" max="4" width="48.7109375" style="58" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="59"/>
-    <col min="6" max="7" width="3.7109375" style="58" customWidth="1"/>
-    <col min="8" max="8" width="3.42578125" style="58" customWidth="1"/>
-    <col min="9" max="9" width="48.7109375" style="58" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="59"/>
-    <col min="11" max="11" width="4.140625" style="58" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="58"/>
+    <col min="1" max="2" width="9.140625" style="55"/>
+    <col min="3" max="3" width="4.140625" style="55" customWidth="1"/>
+    <col min="4" max="4" width="48.7109375" style="55" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="56"/>
+    <col min="6" max="7" width="3.7109375" style="55" customWidth="1"/>
+    <col min="8" max="8" width="3.42578125" style="55" customWidth="1"/>
+    <col min="9" max="9" width="48.7109375" style="55" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="56"/>
+    <col min="11" max="11" width="4.140625" style="55" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="55"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="83" t="s">
+      <c r="C3" s="84" t="s">
+        <v>262</v>
+      </c>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="86"/>
+      <c r="M3" s="87" t="s">
+        <v>258</v>
+      </c>
+      <c r="N3" s="87"/>
+      <c r="O3" s="87"/>
+    </row>
+    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C4" s="57"/>
+      <c r="D4" s="88" t="s">
+        <v>257</v>
+      </c>
+      <c r="E4" s="88"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="88" t="s">
+        <v>258</v>
+      </c>
+      <c r="J4" s="88"/>
+      <c r="K4" s="58"/>
+      <c r="M4" s="67" t="s">
+        <v>266</v>
+      </c>
+      <c r="N4" s="67" t="s">
+        <v>244</v>
+      </c>
+      <c r="O4" s="67" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C5" s="57"/>
+      <c r="D5" s="83" t="s">
+        <v>248</v>
+      </c>
+      <c r="E5" s="83"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="83" t="s">
+        <v>248</v>
+      </c>
+      <c r="J5" s="83"/>
+      <c r="K5" s="58"/>
+      <c r="M5" s="67" t="s">
+        <v>263</v>
+      </c>
+      <c r="N5" s="68">
+        <v>12</v>
+      </c>
+      <c r="O5" s="69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C6" s="57"/>
+      <c r="D6" s="70" t="s">
+        <v>243</v>
+      </c>
+      <c r="E6" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F6" s="58"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="70" t="s">
+        <v>243</v>
+      </c>
+      <c r="J6" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K6" s="58"/>
+      <c r="M6" s="67" t="s">
         <v>264</v>
       </c>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="84"/>
-      <c r="K3" s="85"/>
-      <c r="M3" s="70" t="s">
-        <v>260</v>
-      </c>
-      <c r="N3" s="70"/>
-      <c r="O3" s="70"/>
-    </row>
-    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C4" s="60"/>
-      <c r="D4" s="76" t="s">
-        <v>259</v>
-      </c>
-      <c r="E4" s="76"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="76" t="s">
-        <v>260</v>
-      </c>
-      <c r="J4" s="76"/>
-      <c r="K4" s="61"/>
-      <c r="M4" s="71" t="s">
-        <v>268</v>
-      </c>
-      <c r="N4" s="71" t="s">
+      <c r="N6" s="68">
+        <v>7</v>
+      </c>
+      <c r="O6" s="69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C7" s="57"/>
+      <c r="D7" s="70" t="s">
+        <v>245</v>
+      </c>
+      <c r="E7" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F7" s="58"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="70" t="s">
+        <v>245</v>
+      </c>
+      <c r="J7" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K7" s="58"/>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C8" s="57"/>
+      <c r="D8" s="70" t="s">
         <v>246</v>
       </c>
-      <c r="O4" s="71" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C5" s="60"/>
-      <c r="D5" s="80" t="s">
+      <c r="E8" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F8" s="58"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="70" t="s">
+        <v>246</v>
+      </c>
+      <c r="J8" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K8" s="58"/>
+    </row>
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C9" s="57"/>
+      <c r="D9" s="70" t="s">
+        <v>247</v>
+      </c>
+      <c r="E9" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F9" s="58"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="70" t="s">
+        <v>247</v>
+      </c>
+      <c r="J9" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K9" s="58"/>
+    </row>
+    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C10" s="57"/>
+      <c r="D10" s="70" t="s">
+        <v>247</v>
+      </c>
+      <c r="E10" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F10" s="58"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="70" t="s">
+        <v>247</v>
+      </c>
+      <c r="J10" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K10" s="58"/>
+    </row>
+    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C11" s="57"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="58"/>
+    </row>
+    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C12" s="57"/>
+      <c r="D12" s="83" t="s">
+        <v>256</v>
+      </c>
+      <c r="E12" s="83"/>
+      <c r="F12" s="72"/>
+      <c r="G12" s="73"/>
+      <c r="H12" s="74"/>
+      <c r="I12" s="83" t="s">
+        <v>256</v>
+      </c>
+      <c r="J12" s="83"/>
+      <c r="K12" s="58"/>
+    </row>
+    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C13" s="57"/>
+      <c r="D13" s="70" t="s">
+        <v>249</v>
+      </c>
+      <c r="E13" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F13" s="58"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="70" t="s">
+        <v>249</v>
+      </c>
+      <c r="J13" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K13" s="58"/>
+    </row>
+    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C14" s="57"/>
+      <c r="D14" s="70" t="s">
         <v>250</v>
       </c>
-      <c r="E5" s="80"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="79"/>
-      <c r="I5" s="80" t="s">
+      <c r="E14" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F14" s="58"/>
+      <c r="G14" s="59"/>
+      <c r="H14" s="57"/>
+      <c r="I14" s="70" t="s">
         <v>250</v>
       </c>
-      <c r="J5" s="80"/>
-      <c r="K5" s="61"/>
-      <c r="M5" s="71" t="s">
-        <v>265</v>
-      </c>
-      <c r="N5" s="72">
-        <v>12</v>
-      </c>
-      <c r="O5" s="73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C6" s="60"/>
-      <c r="D6" s="74" t="s">
-        <v>245</v>
-      </c>
-      <c r="E6" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F6" s="61"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="74" t="s">
-        <v>245</v>
-      </c>
-      <c r="J6" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K6" s="61"/>
-      <c r="M6" s="71" t="s">
-        <v>266</v>
-      </c>
-      <c r="N6" s="72">
-        <v>7</v>
-      </c>
-      <c r="O6" s="73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C7" s="60"/>
-      <c r="D7" s="74" t="s">
-        <v>247</v>
-      </c>
-      <c r="E7" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F7" s="61"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="74" t="s">
-        <v>247</v>
-      </c>
-      <c r="J7" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K7" s="61"/>
-    </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C8" s="60"/>
-      <c r="D8" s="74" t="s">
-        <v>248</v>
-      </c>
-      <c r="E8" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F8" s="61"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="74" t="s">
-        <v>248</v>
-      </c>
-      <c r="J8" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K8" s="61"/>
-    </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C9" s="60"/>
-      <c r="D9" s="74" t="s">
-        <v>249</v>
-      </c>
-      <c r="E9" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F9" s="61"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="74" t="s">
-        <v>249</v>
-      </c>
-      <c r="J9" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K9" s="61"/>
-    </row>
-    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C10" s="60"/>
-      <c r="D10" s="74" t="s">
-        <v>249</v>
-      </c>
-      <c r="E10" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F10" s="61"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="74" t="s">
-        <v>249</v>
-      </c>
-      <c r="J10" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K10" s="61"/>
-    </row>
-    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C11" s="60"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="62"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="62"/>
-      <c r="J11" s="63"/>
-      <c r="K11" s="61"/>
-    </row>
-    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C12" s="60"/>
-      <c r="D12" s="80" t="s">
-        <v>258</v>
-      </c>
-      <c r="E12" s="80"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="78"/>
-      <c r="H12" s="79"/>
-      <c r="I12" s="80" t="s">
-        <v>258</v>
-      </c>
-      <c r="J12" s="80"/>
-      <c r="K12" s="61"/>
-    </row>
-    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C13" s="60"/>
-      <c r="D13" s="74" t="s">
+      <c r="J14" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K14" s="58"/>
+    </row>
+    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C15" s="57"/>
+      <c r="D15" s="70" t="s">
         <v>251</v>
       </c>
-      <c r="E13" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F13" s="61"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="74" t="s">
+      <c r="E15" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F15" s="58"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="70" t="s">
         <v>251</v>
       </c>
-      <c r="J13" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K13" s="61"/>
-    </row>
-    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C14" s="60"/>
-      <c r="D14" s="74" t="s">
+      <c r="J15" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K15" s="58"/>
+    </row>
+    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C16" s="57"/>
+      <c r="D16" s="70" t="s">
         <v>252</v>
       </c>
-      <c r="E14" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F14" s="61"/>
-      <c r="G14" s="62"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="74" t="s">
+      <c r="E16" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F16" s="58"/>
+      <c r="G16" s="59"/>
+      <c r="H16" s="57"/>
+      <c r="I16" s="70" t="s">
         <v>252</v>
       </c>
-      <c r="J14" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K14" s="61"/>
-    </row>
-    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C15" s="60"/>
-      <c r="D15" s="74" t="s">
+      <c r="J16" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K16" s="58"/>
+      <c r="O16" s="61"/>
+      <c r="P16" s="62"/>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C17" s="57"/>
+      <c r="D17" s="70" t="s">
         <v>253</v>
       </c>
-      <c r="E15" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F15" s="61"/>
-      <c r="G15" s="62"/>
-      <c r="H15" s="60"/>
-      <c r="I15" s="74" t="s">
+      <c r="E17" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F17" s="58"/>
+      <c r="G17" s="59"/>
+      <c r="H17" s="57"/>
+      <c r="I17" s="70" t="s">
         <v>253</v>
       </c>
-      <c r="J15" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K15" s="61"/>
-    </row>
-    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C16" s="60"/>
-      <c r="D16" s="74" t="s">
+      <c r="J17" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K17" s="58"/>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C18" s="57"/>
+      <c r="D18" s="70" t="s">
         <v>254</v>
       </c>
-      <c r="E16" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F16" s="61"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="74" t="s">
+      <c r="E18" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F18" s="58"/>
+      <c r="G18" s="59"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="70" t="s">
         <v>254</v>
       </c>
-      <c r="J16" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K16" s="61"/>
-      <c r="O16" s="64"/>
-      <c r="P16" s="65"/>
-    </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C17" s="60"/>
-      <c r="D17" s="74" t="s">
+      <c r="J18" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K18" s="58"/>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C19" s="57"/>
+      <c r="D19" s="70" t="s">
         <v>255</v>
       </c>
-      <c r="E17" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F17" s="61"/>
-      <c r="G17" s="62"/>
-      <c r="H17" s="60"/>
-      <c r="I17" s="74" t="s">
+      <c r="E19" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F19" s="58"/>
+      <c r="G19" s="59"/>
+      <c r="H19" s="57"/>
+      <c r="I19" s="70" t="s">
         <v>255</v>
       </c>
-      <c r="J17" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K17" s="61"/>
-    </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C18" s="60"/>
-      <c r="D18" s="74" t="s">
-        <v>256</v>
-      </c>
-      <c r="E18" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F18" s="61"/>
-      <c r="G18" s="62"/>
-      <c r="H18" s="60"/>
-      <c r="I18" s="74" t="s">
-        <v>256</v>
-      </c>
-      <c r="J18" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K18" s="61"/>
-    </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C19" s="60"/>
-      <c r="D19" s="74" t="s">
-        <v>257</v>
-      </c>
-      <c r="E19" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F19" s="61"/>
-      <c r="G19" s="62"/>
-      <c r="H19" s="60"/>
-      <c r="I19" s="74" t="s">
-        <v>257</v>
-      </c>
-      <c r="J19" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K19" s="61"/>
+      <c r="J19" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K19" s="58"/>
     </row>
     <row r="20" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="66"/>
-      <c r="D20" s="67"/>
-      <c r="E20" s="68"/>
-      <c r="F20" s="69"/>
-      <c r="G20" s="62"/>
-      <c r="H20" s="66"/>
-      <c r="I20" s="67"/>
-      <c r="J20" s="68"/>
-      <c r="K20" s="69"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="65"/>
+      <c r="F20" s="66"/>
+      <c r="G20" s="59"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="64"/>
+      <c r="J20" s="65"/>
+      <c r="K20" s="66"/>
     </row>
     <row r="22" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="83" t="s">
+      <c r="C23" s="84" t="s">
+        <v>261</v>
+      </c>
+      <c r="D23" s="85"/>
+      <c r="E23" s="85"/>
+      <c r="F23" s="85"/>
+      <c r="G23" s="85"/>
+      <c r="H23" s="85"/>
+      <c r="I23" s="85"/>
+      <c r="J23" s="85"/>
+      <c r="K23" s="86"/>
+      <c r="M23" s="87" t="s">
+        <v>265</v>
+      </c>
+      <c r="N23" s="87"/>
+      <c r="O23" s="87"/>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C24" s="57"/>
+      <c r="D24" s="88" t="s">
+        <v>257</v>
+      </c>
+      <c r="E24" s="88"/>
+      <c r="F24" s="72"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="74"/>
+      <c r="I24" s="82" t="s">
+        <v>258</v>
+      </c>
+      <c r="J24" s="82"/>
+      <c r="K24" s="58"/>
+      <c r="M24" s="67" t="s">
+        <v>266</v>
+      </c>
+      <c r="N24" s="67" t="s">
+        <v>244</v>
+      </c>
+      <c r="O24" s="67" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C25" s="57"/>
+      <c r="D25" s="83" t="s">
+        <v>260</v>
+      </c>
+      <c r="E25" s="83"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="75"/>
+      <c r="H25" s="74"/>
+      <c r="I25" s="83" t="s">
+        <v>260</v>
+      </c>
+      <c r="J25" s="83"/>
+      <c r="K25" s="58"/>
+      <c r="M25" s="67" t="s">
         <v>263</v>
       </c>
-      <c r="D23" s="84"/>
-      <c r="E23" s="84"/>
-      <c r="F23" s="84"/>
-      <c r="G23" s="84"/>
-      <c r="H23" s="84"/>
-      <c r="I23" s="84"/>
-      <c r="J23" s="84"/>
-      <c r="K23" s="85"/>
-      <c r="M23" s="70" t="s">
-        <v>267</v>
-      </c>
-      <c r="N23" s="70"/>
-      <c r="O23" s="70"/>
-    </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C24" s="60"/>
-      <c r="D24" s="76" t="s">
+      <c r="N25" s="68">
+        <v>12</v>
+      </c>
+      <c r="O25" s="69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C26" s="57"/>
+      <c r="D26" s="70" t="s">
+        <v>249</v>
+      </c>
+      <c r="E26" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F26" s="58"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="70" t="s">
+        <v>249</v>
+      </c>
+      <c r="J26" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K26" s="58"/>
+      <c r="M26" s="67" t="s">
+        <v>264</v>
+      </c>
+      <c r="N26" s="68">
+        <v>4</v>
+      </c>
+      <c r="O26" s="69">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C27" s="57"/>
+      <c r="D27" s="70" t="s">
+        <v>250</v>
+      </c>
+      <c r="E27" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F27" s="58"/>
+      <c r="H27" s="57"/>
+      <c r="I27" s="70" t="s">
+        <v>250</v>
+      </c>
+      <c r="J27" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K27" s="58"/>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C28" s="57"/>
+      <c r="D28" s="70" t="s">
+        <v>251</v>
+      </c>
+      <c r="E28" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F28" s="58"/>
+      <c r="H28" s="57"/>
+      <c r="I28" s="70" t="s">
+        <v>251</v>
+      </c>
+      <c r="J28" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K28" s="58"/>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C29" s="57"/>
+      <c r="D29" s="70" t="s">
+        <v>252</v>
+      </c>
+      <c r="E29" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F29" s="58"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="70" t="s">
+        <v>252</v>
+      </c>
+      <c r="J29" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K29" s="58"/>
+    </row>
+    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C30" s="57"/>
+      <c r="D30" s="71" t="s">
+        <v>253</v>
+      </c>
+      <c r="E30" s="54" t="s">
         <v>259</v>
       </c>
-      <c r="E24" s="76"/>
-      <c r="F24" s="77"/>
-      <c r="G24" s="81"/>
-      <c r="H24" s="79"/>
-      <c r="I24" s="82" t="s">
-        <v>260</v>
-      </c>
-      <c r="J24" s="82"/>
-      <c r="K24" s="61"/>
-      <c r="M24" s="71" t="s">
-        <v>268</v>
-      </c>
-      <c r="N24" s="71" t="s">
-        <v>246</v>
-      </c>
-      <c r="O24" s="71" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C25" s="60"/>
-      <c r="D25" s="80" t="s">
-        <v>262</v>
-      </c>
-      <c r="E25" s="80"/>
-      <c r="F25" s="77"/>
-      <c r="G25" s="81"/>
-      <c r="H25" s="79"/>
-      <c r="I25" s="80" t="s">
-        <v>262</v>
-      </c>
-      <c r="J25" s="80"/>
-      <c r="K25" s="61"/>
-      <c r="M25" s="71" t="s">
-        <v>265</v>
-      </c>
-      <c r="N25" s="72">
-        <v>12</v>
-      </c>
-      <c r="O25" s="73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C26" s="60"/>
-      <c r="D26" s="74" t="s">
-        <v>251</v>
-      </c>
-      <c r="E26" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F26" s="61"/>
-      <c r="H26" s="60"/>
-      <c r="I26" s="74" t="s">
-        <v>251</v>
-      </c>
-      <c r="J26" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K26" s="61"/>
-      <c r="M26" s="71" t="s">
-        <v>266</v>
-      </c>
-      <c r="N26" s="72">
-        <v>4</v>
-      </c>
-      <c r="O26" s="73">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C27" s="60"/>
-      <c r="D27" s="74" t="s">
-        <v>252</v>
-      </c>
-      <c r="E27" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F27" s="61"/>
-      <c r="H27" s="60"/>
-      <c r="I27" s="74" t="s">
-        <v>252</v>
-      </c>
-      <c r="J27" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K27" s="61"/>
-    </row>
-    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C28" s="60"/>
-      <c r="D28" s="74" t="s">
+      <c r="F30" s="58"/>
+      <c r="H30" s="57"/>
+      <c r="I30" s="70" t="s">
         <v>253</v>
       </c>
-      <c r="E28" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F28" s="61"/>
-      <c r="H28" s="60"/>
-      <c r="I28" s="74" t="s">
-        <v>253</v>
-      </c>
-      <c r="J28" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K28" s="61"/>
-    </row>
-    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C29" s="60"/>
-      <c r="D29" s="74" t="s">
+      <c r="J30" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K30" s="58"/>
+    </row>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C31" s="57"/>
+      <c r="D31" s="71" t="s">
         <v>254</v>
       </c>
-      <c r="E29" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F29" s="61"/>
-      <c r="H29" s="60"/>
-      <c r="I29" s="74" t="s">
+      <c r="E31" s="54" t="s">
+        <v>259</v>
+      </c>
+      <c r="F31" s="58"/>
+      <c r="H31" s="57"/>
+      <c r="I31" s="70" t="s">
         <v>254</v>
       </c>
-      <c r="J29" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K29" s="61"/>
-    </row>
-    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C30" s="60"/>
-      <c r="D30" s="75" t="s">
+      <c r="J31" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K31" s="58"/>
+    </row>
+    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C32" s="57"/>
+      <c r="D32" s="71" t="s">
         <v>255</v>
       </c>
-      <c r="E30" s="57" t="s">
-        <v>261</v>
-      </c>
-      <c r="F30" s="61"/>
-      <c r="H30" s="60"/>
-      <c r="I30" s="74" t="s">
+      <c r="E32" s="54" t="s">
+        <v>259</v>
+      </c>
+      <c r="F32" s="58"/>
+      <c r="H32" s="57"/>
+      <c r="I32" s="70" t="s">
         <v>255</v>
       </c>
-      <c r="J30" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K30" s="61"/>
-    </row>
-    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C31" s="60"/>
-      <c r="D31" s="75" t="s">
-        <v>256</v>
-      </c>
-      <c r="E31" s="57" t="s">
-        <v>261</v>
-      </c>
-      <c r="F31" s="61"/>
-      <c r="H31" s="60"/>
-      <c r="I31" s="74" t="s">
-        <v>256</v>
-      </c>
-      <c r="J31" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K31" s="61"/>
-    </row>
-    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C32" s="60"/>
-      <c r="D32" s="75" t="s">
-        <v>257</v>
-      </c>
-      <c r="E32" s="57" t="s">
-        <v>261</v>
-      </c>
-      <c r="F32" s="61"/>
-      <c r="H32" s="60"/>
-      <c r="I32" s="74" t="s">
-        <v>257</v>
-      </c>
-      <c r="J32" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K32" s="61"/>
+      <c r="J32" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K32" s="58"/>
     </row>
     <row r="33" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="66"/>
-      <c r="D33" s="67"/>
-      <c r="E33" s="68"/>
-      <c r="F33" s="69"/>
-      <c r="H33" s="66"/>
-      <c r="I33" s="67"/>
-      <c r="J33" s="68"/>
-      <c r="K33" s="69"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="65"/>
+      <c r="F33" s="66"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="64"/>
+      <c r="J33" s="65"/>
+      <c r="K33" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>

<commit_message>
Updated Hooks and Cucucmber Runner.
</commit_message>
<xml_diff>
--- a/src/test/java/BaseFramework/Data/DA.xlsx
+++ b/src/test/java/BaseFramework/Data/DA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14445" windowHeight="8160" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14445" windowHeight="8160" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Create Account" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="302">
   <si>
     <t>First Name</t>
   </si>
@@ -695,9 +695,6 @@
     <t>Assgine , Steps Required</t>
   </si>
   <si>
-    <t>Doctoral_ChemistryResearch_PHD_Programme_StepDefs</t>
-  </si>
-  <si>
     <t>Chemistry</t>
   </si>
   <si>
@@ -770,9 +767,6 @@
     <t>Medical Sciences with Humanities, Philosophy and Law BSc (1YFT - Intercalated) - Intercalated</t>
   </si>
   <si>
-    <t>Short course</t>
-  </si>
-  <si>
     <t>Pre-Sessional English Programme (12 week) - Presesional</t>
   </si>
   <si>
@@ -869,9 +863,6 @@
     <t>selected by default</t>
   </si>
   <si>
-    <t>s.sonnar@mailinator.com</t>
-  </si>
-  <si>
     <t>05/09/2008 - NOT REQUIRED</t>
   </si>
   <si>
@@ -938,10 +929,40 @@
     <t>Asian - Chinese</t>
   </si>
   <si>
-    <t>Doctoral38</t>
-  </si>
-  <si>
-    <t>d38.chemistry@mailinator.com</t>
+    <t>Doctoral39</t>
+  </si>
+  <si>
+    <t>d39.chemistry@mailinator.com</t>
+  </si>
+  <si>
+    <t>Course Type</t>
+  </si>
+  <si>
+    <t>Academice Programme</t>
+  </si>
+  <si>
+    <t>IETLS</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Criminal</t>
+  </si>
+  <si>
+    <t>ScholarShip</t>
+  </si>
+  <si>
+    <t>Disability</t>
+  </si>
+  <si>
+    <t>Select course type - Postgraduate Research</t>
+  </si>
+  <si>
+    <t>Select course type - Postgraduate Taught</t>
+  </si>
+  <si>
+    <t>Select course type - Short course</t>
   </si>
 </sst>
 </file>
@@ -1480,7 +1501,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1533,15 +1554,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="15" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="17" fontId="3" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1571,9 +1583,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1585,17 +1594,26 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="3" fillId="3" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1607,9 +1625,21 @@
     <xf numFmtId="0" fontId="13" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="6" fontId="3" fillId="3" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent5" xfId="1" builtinId="45"/>
@@ -2160,7 +2190,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
@@ -2168,7 +2198,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
@@ -2194,8 +2224,8 @@
       <c r="A8" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="51" t="s">
-        <v>218</v>
+      <c r="B8" s="48" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
@@ -2322,7 +2352,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -2330,7 +2360,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -2369,8 +2399,8 @@
       <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="51" t="s">
-        <v>219</v>
+      <c r="B6" s="48" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -3095,7 +3125,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -3103,7 +3133,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -3142,8 +3172,8 @@
       <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="51" t="s">
-        <v>244</v>
+      <c r="B6" s="48" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -3868,15 +3898,15 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="52" t="s">
-        <v>220</v>
+      <c r="B3" s="49" t="s">
+        <v>219</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -3915,8 +3945,8 @@
       <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="51" t="s">
-        <v>241</v>
+      <c r="B6" s="48" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -4612,8 +4642,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:K106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4640,7 +4670,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -4648,7 +4678,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -4687,8 +4717,8 @@
       <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="51" t="s">
-        <v>294</v>
+      <c r="B6" s="48" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -4706,6 +4736,9 @@
       <c r="B8" s="10" t="s">
         <v>191</v>
       </c>
+      <c r="D8" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
@@ -4755,7 +4788,7 @@
         <v>26</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C16" s="28" t="s">
         <v>139</v>
@@ -4765,25 +4798,25 @@
       <c r="A17" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="51" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B18" s="54" t="s">
-        <v>274</v>
+      <c r="B18" s="51" t="s">
+        <v>271</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
@@ -4807,18 +4840,16 @@
         <v>32</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="D21" s="86" t="s">
-        <v>270</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="D21" s="76"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
@@ -4826,7 +4857,7 @@
         <v>44</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
@@ -4834,7 +4865,7 @@
         <v>37</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
@@ -4842,7 +4873,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
@@ -4850,7 +4881,7 @@
         <v>39</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
@@ -4858,7 +4889,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
@@ -4866,23 +4897,23 @@
         <v>41</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="53" t="s">
-        <v>273</v>
+      <c r="B29" s="50" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B30" s="54" t="s">
-        <v>271</v>
+      <c r="B30" s="51" t="s">
+        <v>268</v>
       </c>
       <c r="C30" s="28"/>
     </row>
@@ -4890,8 +4921,8 @@
       <c r="A31" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="54" t="s">
-        <v>272</v>
+      <c r="B31" s="51" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
@@ -4967,7 +4998,7 @@
         <v>59</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
@@ -4975,7 +5006,7 @@
         <v>60</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
@@ -5068,12 +5099,12 @@
         <v>82</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B60" s="15" t="s">
         <v>80</v>
@@ -5081,18 +5112,18 @@
     </row>
     <row r="61" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="B62" s="87" t="s">
-        <v>281</v>
+        <v>277</v>
+      </c>
+      <c r="B62" s="77" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -5114,52 +5145,52 @@
         <v>106</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A68" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A69" s="7" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A70" s="7" t="s">
-        <v>285</v>
-      </c>
-      <c r="B70" s="88" t="s">
-        <v>290</v>
+        <v>282</v>
+      </c>
+      <c r="B70" s="78" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="B71" s="12" t="s">
         <v>286</v>
-      </c>
-      <c r="B71" s="12" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A72" s="7" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A73" s="7" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B73" s="12" t="s">
         <v>52</v>
@@ -5178,7 +5209,7 @@
         <v>114</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
@@ -5352,17 +5383,16 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1"/>
-    <hyperlink ref="D21" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-  <drawing r:id="rId4"/>
-  <legacyDrawing r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="14337" r:id="rId6" name="Control 1">
-          <controlPr defaultSize="0" r:id="rId7">
+        <control shapeId="14337" r:id="rId5" name="Control 1">
+          <controlPr defaultSize="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -5381,7 +5411,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="14337" r:id="rId6" name="Control 1"/>
+        <control shapeId="14337" r:id="rId5" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -5446,15 +5476,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="79" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5612,9 +5642,9 @@
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="55"/>
+      <c r="B28" s="52"/>
       <c r="C28" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5642,46 +5672,49 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E11:P43"/>
+  <dimension ref="B11:P49"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+    <sheetView topLeftCell="L23" workbookViewId="0">
+      <selection activeCell="O43" sqref="O43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="20.7109375" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="25.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="33.42578125" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="81.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="44.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="70" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="11" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="F11" s="50" t="s">
+    <row r="11" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="F11" s="81" t="s">
         <v>207</v>
       </c>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="50"/>
-    </row>
-    <row r="12" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="G11" s="81"/>
+      <c r="H11" s="81"/>
+      <c r="I11" s="81"/>
+      <c r="J11" s="81"/>
+    </row>
+    <row r="12" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="13" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="14" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F14" s="40" t="s">
         <v>87</v>
       </c>
@@ -5697,8 +5730,11 @@
       <c r="J14" s="19" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="15" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="O14" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="15" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F15" s="41" t="s">
         <v>89</v>
       </c>
@@ -5715,7 +5751,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>185</v>
       </c>
@@ -5739,7 +5775,7 @@
         <v>2516</v>
       </c>
     </row>
-    <row r="17" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F17" s="41" t="s">
         <v>100</v>
       </c>
@@ -5751,7 +5787,7 @@
       </c>
       <c r="I17" s="17"/>
     </row>
-    <row r="18" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F18" s="41" t="s">
         <v>97</v>
       </c>
@@ -5761,7 +5797,7 @@
       <c r="H18" s="17"/>
       <c r="I18" s="17"/>
     </row>
-    <row r="19" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F19" s="41"/>
       <c r="G19" s="17" t="s">
         <v>97</v>
@@ -5769,58 +5805,38 @@
       <c r="H19" s="17"/>
       <c r="I19" s="17"/>
     </row>
-    <row r="21" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F21" s="2"/>
     </row>
-    <row r="23" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="N23" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="26" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F26" t="s">
+    <row r="22" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="N22" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F27" s="18" t="s">
+    <row r="23" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="N23" s="18" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="28" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F28" t="s">
+    <row r="24" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="N24" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F29" s="20" t="s">
+    <row r="25" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="N25" s="20" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="31" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="O31" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="32" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="O32" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="33" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="O33" t="s">
-        <v>222</v>
-      </c>
-      <c r="P33" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="34" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E34" s="49" t="s">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="P33" s="2"/>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E34" s="80" t="s">
         <v>173</v>
       </c>
-      <c r="F34" s="49"/>
-      <c r="G34" s="49"/>
+      <c r="F34" s="80"/>
+      <c r="G34" s="80"/>
       <c r="I34" s="17" t="s">
         <v>179</v>
       </c>
@@ -5832,16 +5848,16 @@
         <v>190</v>
       </c>
       <c r="N34" s="39" t="s">
-        <v>136</v>
+        <v>300</v>
       </c>
       <c r="O34" s="39" t="s">
-        <v>136</v>
+        <v>299</v>
       </c>
       <c r="P34" s="39" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="35" spans="5:16" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E35" s="17"/>
       <c r="F35" s="17"/>
       <c r="G35" s="17"/>
@@ -5867,7 +5883,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="36" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E36" s="17" t="s">
         <v>175</v>
       </c>
@@ -5885,7 +5901,7 @@
       </c>
       <c r="K36" s="17"/>
     </row>
-    <row r="37" spans="5:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="E37" s="17" t="s">
         <v>176</v>
       </c>
@@ -5914,7 +5930,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E38" s="17" t="s">
         <v>178</v>
       </c>
@@ -5938,10 +5954,10 @@
         <v>188</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="39" spans="5:16" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E39" s="17" t="s">
         <v>178</v>
       </c>
@@ -5955,16 +5971,16 @@
         <v>24</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="40" spans="5:16" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E40" s="17"/>
       <c r="F40" s="17"/>
       <c r="G40" s="17"/>
@@ -5972,16 +5988,16 @@
         <v>23</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="O40" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="O40" s="93" t="s">
         <v>191</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="41" spans="5:16" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E41" s="17"/>
       <c r="F41" s="17"/>
       <c r="G41" s="17"/>
@@ -5992,20 +6008,72 @@
         <v>23</v>
       </c>
       <c r="N41" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="O41" s="2" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="42" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="O41" s="2"/>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
       <c r="N42" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N43" s="2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="43" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="N43" s="2" t="s">
-        <v>236</v>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B47" s="89" t="s">
+        <v>292</v>
+      </c>
+      <c r="C47" s="89" t="s">
+        <v>293</v>
+      </c>
+      <c r="D47" s="89" t="s">
+        <v>88</v>
+      </c>
+      <c r="E47" s="89" t="s">
+        <v>294</v>
+      </c>
+      <c r="F47" s="92" t="s">
+        <v>296</v>
+      </c>
+      <c r="G47" s="92" t="s">
+        <v>297</v>
+      </c>
+      <c r="H47" s="92" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B48" s="90" t="s">
+        <v>137</v>
+      </c>
+      <c r="C48" s="90" t="s">
+        <v>191</v>
+      </c>
+      <c r="D48" s="90" t="s">
+        <v>91</v>
+      </c>
+      <c r="E48" s="91" t="s">
+        <v>295</v>
+      </c>
+      <c r="F48" s="91" t="s">
+        <v>52</v>
+      </c>
+      <c r="G48" s="91" t="s">
+        <v>52</v>
+      </c>
+      <c r="H48" s="91" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -6092,572 +6160,572 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="58"/>
-    <col min="3" max="3" width="4.140625" style="58" customWidth="1"/>
-    <col min="4" max="4" width="48.7109375" style="58" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="59"/>
-    <col min="6" max="7" width="3.7109375" style="58" customWidth="1"/>
-    <col min="8" max="8" width="3.42578125" style="58" customWidth="1"/>
-    <col min="9" max="9" width="48.7109375" style="58" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="59"/>
-    <col min="11" max="11" width="4.140625" style="58" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="58"/>
+    <col min="1" max="2" width="9.140625" style="55"/>
+    <col min="3" max="3" width="4.140625" style="55" customWidth="1"/>
+    <col min="4" max="4" width="48.7109375" style="55" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="56"/>
+    <col min="6" max="7" width="3.7109375" style="55" customWidth="1"/>
+    <col min="8" max="8" width="3.42578125" style="55" customWidth="1"/>
+    <col min="9" max="9" width="48.7109375" style="55" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="56"/>
+    <col min="11" max="11" width="4.140625" style="55" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="55"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="83" t="s">
+      <c r="C3" s="84" t="s">
+        <v>262</v>
+      </c>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="86"/>
+      <c r="M3" s="87" t="s">
+        <v>258</v>
+      </c>
+      <c r="N3" s="87"/>
+      <c r="O3" s="87"/>
+    </row>
+    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C4" s="57"/>
+      <c r="D4" s="88" t="s">
+        <v>257</v>
+      </c>
+      <c r="E4" s="88"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="88" t="s">
+        <v>258</v>
+      </c>
+      <c r="J4" s="88"/>
+      <c r="K4" s="58"/>
+      <c r="M4" s="67" t="s">
+        <v>266</v>
+      </c>
+      <c r="N4" s="67" t="s">
+        <v>244</v>
+      </c>
+      <c r="O4" s="67" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C5" s="57"/>
+      <c r="D5" s="83" t="s">
+        <v>248</v>
+      </c>
+      <c r="E5" s="83"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="83" t="s">
+        <v>248</v>
+      </c>
+      <c r="J5" s="83"/>
+      <c r="K5" s="58"/>
+      <c r="M5" s="67" t="s">
+        <v>263</v>
+      </c>
+      <c r="N5" s="68">
+        <v>12</v>
+      </c>
+      <c r="O5" s="69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C6" s="57"/>
+      <c r="D6" s="70" t="s">
+        <v>243</v>
+      </c>
+      <c r="E6" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F6" s="58"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="70" t="s">
+        <v>243</v>
+      </c>
+      <c r="J6" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K6" s="58"/>
+      <c r="M6" s="67" t="s">
         <v>264</v>
       </c>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="84"/>
-      <c r="K3" s="85"/>
-      <c r="M3" s="70" t="s">
-        <v>260</v>
-      </c>
-      <c r="N3" s="70"/>
-      <c r="O3" s="70"/>
-    </row>
-    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C4" s="60"/>
-      <c r="D4" s="76" t="s">
-        <v>259</v>
-      </c>
-      <c r="E4" s="76"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="76" t="s">
-        <v>260</v>
-      </c>
-      <c r="J4" s="76"/>
-      <c r="K4" s="61"/>
-      <c r="M4" s="71" t="s">
-        <v>268</v>
-      </c>
-      <c r="N4" s="71" t="s">
+      <c r="N6" s="68">
+        <v>7</v>
+      </c>
+      <c r="O6" s="69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C7" s="57"/>
+      <c r="D7" s="70" t="s">
+        <v>245</v>
+      </c>
+      <c r="E7" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F7" s="58"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="70" t="s">
+        <v>245</v>
+      </c>
+      <c r="J7" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K7" s="58"/>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C8" s="57"/>
+      <c r="D8" s="70" t="s">
         <v>246</v>
       </c>
-      <c r="O4" s="71" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C5" s="60"/>
-      <c r="D5" s="80" t="s">
+      <c r="E8" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F8" s="58"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="70" t="s">
+        <v>246</v>
+      </c>
+      <c r="J8" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K8" s="58"/>
+    </row>
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C9" s="57"/>
+      <c r="D9" s="70" t="s">
+        <v>247</v>
+      </c>
+      <c r="E9" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F9" s="58"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="70" t="s">
+        <v>247</v>
+      </c>
+      <c r="J9" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K9" s="58"/>
+    </row>
+    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C10" s="57"/>
+      <c r="D10" s="70" t="s">
+        <v>247</v>
+      </c>
+      <c r="E10" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F10" s="58"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="70" t="s">
+        <v>247</v>
+      </c>
+      <c r="J10" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K10" s="58"/>
+    </row>
+    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C11" s="57"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="58"/>
+    </row>
+    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C12" s="57"/>
+      <c r="D12" s="83" t="s">
+        <v>256</v>
+      </c>
+      <c r="E12" s="83"/>
+      <c r="F12" s="72"/>
+      <c r="G12" s="73"/>
+      <c r="H12" s="74"/>
+      <c r="I12" s="83" t="s">
+        <v>256</v>
+      </c>
+      <c r="J12" s="83"/>
+      <c r="K12" s="58"/>
+    </row>
+    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C13" s="57"/>
+      <c r="D13" s="70" t="s">
+        <v>249</v>
+      </c>
+      <c r="E13" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F13" s="58"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="70" t="s">
+        <v>249</v>
+      </c>
+      <c r="J13" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K13" s="58"/>
+    </row>
+    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C14" s="57"/>
+      <c r="D14" s="70" t="s">
         <v>250</v>
       </c>
-      <c r="E5" s="80"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="79"/>
-      <c r="I5" s="80" t="s">
+      <c r="E14" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F14" s="58"/>
+      <c r="G14" s="59"/>
+      <c r="H14" s="57"/>
+      <c r="I14" s="70" t="s">
         <v>250</v>
       </c>
-      <c r="J5" s="80"/>
-      <c r="K5" s="61"/>
-      <c r="M5" s="71" t="s">
-        <v>265</v>
-      </c>
-      <c r="N5" s="72">
-        <v>12</v>
-      </c>
-      <c r="O5" s="73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C6" s="60"/>
-      <c r="D6" s="74" t="s">
-        <v>245</v>
-      </c>
-      <c r="E6" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F6" s="61"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="74" t="s">
-        <v>245</v>
-      </c>
-      <c r="J6" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K6" s="61"/>
-      <c r="M6" s="71" t="s">
-        <v>266</v>
-      </c>
-      <c r="N6" s="72">
-        <v>7</v>
-      </c>
-      <c r="O6" s="73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C7" s="60"/>
-      <c r="D7" s="74" t="s">
-        <v>247</v>
-      </c>
-      <c r="E7" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F7" s="61"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="74" t="s">
-        <v>247</v>
-      </c>
-      <c r="J7" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K7" s="61"/>
-    </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C8" s="60"/>
-      <c r="D8" s="74" t="s">
-        <v>248</v>
-      </c>
-      <c r="E8" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F8" s="61"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="74" t="s">
-        <v>248</v>
-      </c>
-      <c r="J8" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K8" s="61"/>
-    </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C9" s="60"/>
-      <c r="D9" s="74" t="s">
-        <v>249</v>
-      </c>
-      <c r="E9" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F9" s="61"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="74" t="s">
-        <v>249</v>
-      </c>
-      <c r="J9" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K9" s="61"/>
-    </row>
-    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C10" s="60"/>
-      <c r="D10" s="74" t="s">
-        <v>249</v>
-      </c>
-      <c r="E10" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F10" s="61"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="74" t="s">
-        <v>249</v>
-      </c>
-      <c r="J10" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K10" s="61"/>
-    </row>
-    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C11" s="60"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="62"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="62"/>
-      <c r="J11" s="63"/>
-      <c r="K11" s="61"/>
-    </row>
-    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C12" s="60"/>
-      <c r="D12" s="80" t="s">
-        <v>258</v>
-      </c>
-      <c r="E12" s="80"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="78"/>
-      <c r="H12" s="79"/>
-      <c r="I12" s="80" t="s">
-        <v>258</v>
-      </c>
-      <c r="J12" s="80"/>
-      <c r="K12" s="61"/>
-    </row>
-    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C13" s="60"/>
-      <c r="D13" s="74" t="s">
+      <c r="J14" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K14" s="58"/>
+    </row>
+    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C15" s="57"/>
+      <c r="D15" s="70" t="s">
         <v>251</v>
       </c>
-      <c r="E13" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F13" s="61"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="74" t="s">
+      <c r="E15" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F15" s="58"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="70" t="s">
         <v>251</v>
       </c>
-      <c r="J13" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K13" s="61"/>
-    </row>
-    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C14" s="60"/>
-      <c r="D14" s="74" t="s">
+      <c r="J15" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K15" s="58"/>
+    </row>
+    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C16" s="57"/>
+      <c r="D16" s="70" t="s">
         <v>252</v>
       </c>
-      <c r="E14" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F14" s="61"/>
-      <c r="G14" s="62"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="74" t="s">
+      <c r="E16" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F16" s="58"/>
+      <c r="G16" s="59"/>
+      <c r="H16" s="57"/>
+      <c r="I16" s="70" t="s">
         <v>252</v>
       </c>
-      <c r="J14" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K14" s="61"/>
-    </row>
-    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C15" s="60"/>
-      <c r="D15" s="74" t="s">
+      <c r="J16" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K16" s="58"/>
+      <c r="O16" s="61"/>
+      <c r="P16" s="62"/>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C17" s="57"/>
+      <c r="D17" s="70" t="s">
         <v>253</v>
       </c>
-      <c r="E15" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F15" s="61"/>
-      <c r="G15" s="62"/>
-      <c r="H15" s="60"/>
-      <c r="I15" s="74" t="s">
+      <c r="E17" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F17" s="58"/>
+      <c r="G17" s="59"/>
+      <c r="H17" s="57"/>
+      <c r="I17" s="70" t="s">
         <v>253</v>
       </c>
-      <c r="J15" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K15" s="61"/>
-    </row>
-    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C16" s="60"/>
-      <c r="D16" s="74" t="s">
+      <c r="J17" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K17" s="58"/>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C18" s="57"/>
+      <c r="D18" s="70" t="s">
         <v>254</v>
       </c>
-      <c r="E16" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F16" s="61"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="74" t="s">
+      <c r="E18" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F18" s="58"/>
+      <c r="G18" s="59"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="70" t="s">
         <v>254</v>
       </c>
-      <c r="J16" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K16" s="61"/>
-      <c r="O16" s="64"/>
-      <c r="P16" s="65"/>
-    </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C17" s="60"/>
-      <c r="D17" s="74" t="s">
+      <c r="J18" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K18" s="58"/>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C19" s="57"/>
+      <c r="D19" s="70" t="s">
         <v>255</v>
       </c>
-      <c r="E17" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F17" s="61"/>
-      <c r="G17" s="62"/>
-      <c r="H17" s="60"/>
-      <c r="I17" s="74" t="s">
+      <c r="E19" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F19" s="58"/>
+      <c r="G19" s="59"/>
+      <c r="H19" s="57"/>
+      <c r="I19" s="70" t="s">
         <v>255</v>
       </c>
-      <c r="J17" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K17" s="61"/>
-    </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C18" s="60"/>
-      <c r="D18" s="74" t="s">
-        <v>256</v>
-      </c>
-      <c r="E18" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F18" s="61"/>
-      <c r="G18" s="62"/>
-      <c r="H18" s="60"/>
-      <c r="I18" s="74" t="s">
-        <v>256</v>
-      </c>
-      <c r="J18" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K18" s="61"/>
-    </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C19" s="60"/>
-      <c r="D19" s="74" t="s">
-        <v>257</v>
-      </c>
-      <c r="E19" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F19" s="61"/>
-      <c r="G19" s="62"/>
-      <c r="H19" s="60"/>
-      <c r="I19" s="74" t="s">
-        <v>257</v>
-      </c>
-      <c r="J19" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K19" s="61"/>
+      <c r="J19" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K19" s="58"/>
     </row>
     <row r="20" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="66"/>
-      <c r="D20" s="67"/>
-      <c r="E20" s="68"/>
-      <c r="F20" s="69"/>
-      <c r="G20" s="62"/>
-      <c r="H20" s="66"/>
-      <c r="I20" s="67"/>
-      <c r="J20" s="68"/>
-      <c r="K20" s="69"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="65"/>
+      <c r="F20" s="66"/>
+      <c r="G20" s="59"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="64"/>
+      <c r="J20" s="65"/>
+      <c r="K20" s="66"/>
     </row>
     <row r="22" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="83" t="s">
+      <c r="C23" s="84" t="s">
+        <v>261</v>
+      </c>
+      <c r="D23" s="85"/>
+      <c r="E23" s="85"/>
+      <c r="F23" s="85"/>
+      <c r="G23" s="85"/>
+      <c r="H23" s="85"/>
+      <c r="I23" s="85"/>
+      <c r="J23" s="85"/>
+      <c r="K23" s="86"/>
+      <c r="M23" s="87" t="s">
+        <v>265</v>
+      </c>
+      <c r="N23" s="87"/>
+      <c r="O23" s="87"/>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C24" s="57"/>
+      <c r="D24" s="88" t="s">
+        <v>257</v>
+      </c>
+      <c r="E24" s="88"/>
+      <c r="F24" s="72"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="74"/>
+      <c r="I24" s="82" t="s">
+        <v>258</v>
+      </c>
+      <c r="J24" s="82"/>
+      <c r="K24" s="58"/>
+      <c r="M24" s="67" t="s">
+        <v>266</v>
+      </c>
+      <c r="N24" s="67" t="s">
+        <v>244</v>
+      </c>
+      <c r="O24" s="67" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C25" s="57"/>
+      <c r="D25" s="83" t="s">
+        <v>260</v>
+      </c>
+      <c r="E25" s="83"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="75"/>
+      <c r="H25" s="74"/>
+      <c r="I25" s="83" t="s">
+        <v>260</v>
+      </c>
+      <c r="J25" s="83"/>
+      <c r="K25" s="58"/>
+      <c r="M25" s="67" t="s">
         <v>263</v>
       </c>
-      <c r="D23" s="84"/>
-      <c r="E23" s="84"/>
-      <c r="F23" s="84"/>
-      <c r="G23" s="84"/>
-      <c r="H23" s="84"/>
-      <c r="I23" s="84"/>
-      <c r="J23" s="84"/>
-      <c r="K23" s="85"/>
-      <c r="M23" s="70" t="s">
-        <v>267</v>
-      </c>
-      <c r="N23" s="70"/>
-      <c r="O23" s="70"/>
-    </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C24" s="60"/>
-      <c r="D24" s="76" t="s">
+      <c r="N25" s="68">
+        <v>12</v>
+      </c>
+      <c r="O25" s="69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C26" s="57"/>
+      <c r="D26" s="70" t="s">
+        <v>249</v>
+      </c>
+      <c r="E26" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F26" s="58"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="70" t="s">
+        <v>249</v>
+      </c>
+      <c r="J26" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K26" s="58"/>
+      <c r="M26" s="67" t="s">
+        <v>264</v>
+      </c>
+      <c r="N26" s="68">
+        <v>4</v>
+      </c>
+      <c r="O26" s="69">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C27" s="57"/>
+      <c r="D27" s="70" t="s">
+        <v>250</v>
+      </c>
+      <c r="E27" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F27" s="58"/>
+      <c r="H27" s="57"/>
+      <c r="I27" s="70" t="s">
+        <v>250</v>
+      </c>
+      <c r="J27" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K27" s="58"/>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C28" s="57"/>
+      <c r="D28" s="70" t="s">
+        <v>251</v>
+      </c>
+      <c r="E28" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F28" s="58"/>
+      <c r="H28" s="57"/>
+      <c r="I28" s="70" t="s">
+        <v>251</v>
+      </c>
+      <c r="J28" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K28" s="58"/>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C29" s="57"/>
+      <c r="D29" s="70" t="s">
+        <v>252</v>
+      </c>
+      <c r="E29" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="F29" s="58"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="70" t="s">
+        <v>252</v>
+      </c>
+      <c r="J29" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K29" s="58"/>
+    </row>
+    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C30" s="57"/>
+      <c r="D30" s="71" t="s">
+        <v>253</v>
+      </c>
+      <c r="E30" s="54" t="s">
         <v>259</v>
       </c>
-      <c r="E24" s="76"/>
-      <c r="F24" s="77"/>
-      <c r="G24" s="81"/>
-      <c r="H24" s="79"/>
-      <c r="I24" s="82" t="s">
-        <v>260</v>
-      </c>
-      <c r="J24" s="82"/>
-      <c r="K24" s="61"/>
-      <c r="M24" s="71" t="s">
-        <v>268</v>
-      </c>
-      <c r="N24" s="71" t="s">
-        <v>246</v>
-      </c>
-      <c r="O24" s="71" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C25" s="60"/>
-      <c r="D25" s="80" t="s">
-        <v>262</v>
-      </c>
-      <c r="E25" s="80"/>
-      <c r="F25" s="77"/>
-      <c r="G25" s="81"/>
-      <c r="H25" s="79"/>
-      <c r="I25" s="80" t="s">
-        <v>262</v>
-      </c>
-      <c r="J25" s="80"/>
-      <c r="K25" s="61"/>
-      <c r="M25" s="71" t="s">
-        <v>265</v>
-      </c>
-      <c r="N25" s="72">
-        <v>12</v>
-      </c>
-      <c r="O25" s="73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C26" s="60"/>
-      <c r="D26" s="74" t="s">
-        <v>251</v>
-      </c>
-      <c r="E26" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F26" s="61"/>
-      <c r="H26" s="60"/>
-      <c r="I26" s="74" t="s">
-        <v>251</v>
-      </c>
-      <c r="J26" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K26" s="61"/>
-      <c r="M26" s="71" t="s">
-        <v>266</v>
-      </c>
-      <c r="N26" s="72">
-        <v>4</v>
-      </c>
-      <c r="O26" s="73">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C27" s="60"/>
-      <c r="D27" s="74" t="s">
-        <v>252</v>
-      </c>
-      <c r="E27" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F27" s="61"/>
-      <c r="H27" s="60"/>
-      <c r="I27" s="74" t="s">
-        <v>252</v>
-      </c>
-      <c r="J27" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K27" s="61"/>
-    </row>
-    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C28" s="60"/>
-      <c r="D28" s="74" t="s">
+      <c r="F30" s="58"/>
+      <c r="H30" s="57"/>
+      <c r="I30" s="70" t="s">
         <v>253</v>
       </c>
-      <c r="E28" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F28" s="61"/>
-      <c r="H28" s="60"/>
-      <c r="I28" s="74" t="s">
-        <v>253</v>
-      </c>
-      <c r="J28" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K28" s="61"/>
-    </row>
-    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C29" s="60"/>
-      <c r="D29" s="74" t="s">
+      <c r="J30" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K30" s="58"/>
+    </row>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C31" s="57"/>
+      <c r="D31" s="71" t="s">
         <v>254</v>
       </c>
-      <c r="E29" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F29" s="61"/>
-      <c r="H29" s="60"/>
-      <c r="I29" s="74" t="s">
+      <c r="E31" s="54" t="s">
+        <v>259</v>
+      </c>
+      <c r="F31" s="58"/>
+      <c r="H31" s="57"/>
+      <c r="I31" s="70" t="s">
         <v>254</v>
       </c>
-      <c r="J29" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K29" s="61"/>
-    </row>
-    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C30" s="60"/>
-      <c r="D30" s="75" t="s">
+      <c r="J31" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K31" s="58"/>
+    </row>
+    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C32" s="57"/>
+      <c r="D32" s="71" t="s">
         <v>255</v>
       </c>
-      <c r="E30" s="57" t="s">
-        <v>261</v>
-      </c>
-      <c r="F30" s="61"/>
-      <c r="H30" s="60"/>
-      <c r="I30" s="74" t="s">
+      <c r="E32" s="54" t="s">
+        <v>259</v>
+      </c>
+      <c r="F32" s="58"/>
+      <c r="H32" s="57"/>
+      <c r="I32" s="70" t="s">
         <v>255</v>
       </c>
-      <c r="J30" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K30" s="61"/>
-    </row>
-    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C31" s="60"/>
-      <c r="D31" s="75" t="s">
-        <v>256</v>
-      </c>
-      <c r="E31" s="57" t="s">
-        <v>261</v>
-      </c>
-      <c r="F31" s="61"/>
-      <c r="H31" s="60"/>
-      <c r="I31" s="74" t="s">
-        <v>256</v>
-      </c>
-      <c r="J31" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K31" s="61"/>
-    </row>
-    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C32" s="60"/>
-      <c r="D32" s="75" t="s">
-        <v>257</v>
-      </c>
-      <c r="E32" s="57" t="s">
-        <v>261</v>
-      </c>
-      <c r="F32" s="61"/>
-      <c r="H32" s="60"/>
-      <c r="I32" s="74" t="s">
-        <v>257</v>
-      </c>
-      <c r="J32" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="K32" s="61"/>
+      <c r="J32" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="K32" s="58"/>
     </row>
     <row r="33" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="66"/>
-      <c r="D33" s="67"/>
-      <c r="E33" s="68"/>
-      <c r="F33" s="69"/>
-      <c r="H33" s="66"/>
-      <c r="I33" s="67"/>
-      <c r="J33" s="68"/>
-      <c r="K33" s="69"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="65"/>
+      <c r="F33" s="66"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="64"/>
+      <c r="J33" s="65"/>
+      <c r="K33" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>

<commit_message>
Running th failing test
</commit_message>
<xml_diff>
--- a/src/test/java/BaseFramework/Data/DA.xlsx
+++ b/src/test/java/BaseFramework/Data/DA.xlsx
@@ -956,13 +956,13 @@
     <t>Select course type - Short course</t>
   </si>
   <si>
-    <t>GitTest</t>
-  </si>
-  <si>
     <t>Pjohny</t>
   </si>
   <si>
-    <t>git.pjohny@mailinator.com</t>
+    <t>GitI2</t>
+  </si>
+  <si>
+    <t>gitI2.pjohny@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -2190,7 +2190,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
@@ -2198,7 +2198,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Running th failing test_2
</commit_message>
<xml_diff>
--- a/src/test/java/BaseFramework/Data/DA.xlsx
+++ b/src/test/java/BaseFramework/Data/DA.xlsx
@@ -956,13 +956,13 @@
     <t>Select course type - Short course</t>
   </si>
   <si>
-    <t>Pjohny</t>
-  </si>
-  <si>
-    <t>GitI2</t>
-  </si>
-  <si>
-    <t>gitI2.pjohny@mailinator.com</t>
+    <t>Johnty</t>
+  </si>
+  <si>
+    <t>Rodes</t>
+  </si>
+  <si>
+    <t>johnty.rodes@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -2190,7 +2190,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
@@ -2198,7 +2198,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Correcting the error in excel file
</commit_message>
<xml_diff>
--- a/src/test/java/BaseFramework/Data/DA.xlsx
+++ b/src/test/java/BaseFramework/Data/DA.xlsx
@@ -956,13 +956,13 @@
     <t>Select course type - Short course</t>
   </si>
   <si>
-    <t>Pjohny</t>
-  </si>
-  <si>
-    <t>GitI2</t>
-  </si>
-  <si>
-    <t>gitI2.pjohny@mailinator.com</t>
+    <t>Johnty</t>
+  </si>
+  <si>
+    <t>Rodes</t>
+  </si>
+  <si>
+    <t>johnty.rodes@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -2190,7 +2190,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
@@ -2198,7 +2198,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Changed Create Account Feature Scenario Titles.
</commit_message>
<xml_diff>
--- a/src/test/java/BaseFramework/Data/DA.xlsx
+++ b/src/test/java/BaseFramework/Data/DA.xlsx
@@ -956,13 +956,13 @@
     <t>Select course type - Short course</t>
   </si>
   <si>
-    <t>Johnty</t>
-  </si>
-  <si>
-    <t>Rodes</t>
-  </si>
-  <si>
-    <t>johnty.rodes@mailinator.com</t>
+    <t>Shaun</t>
+  </si>
+  <si>
+    <t>Pollocks</t>
+  </si>
+  <si>
+    <t>s.pollocks@mailinator.com</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Added new Program - MRC
</commit_message>
<xml_diff>
--- a/src/test/java/BaseFramework/Data/DA.xlsx
+++ b/src/test/java/BaseFramework/Data/DA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14445" windowHeight="8160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14445" windowHeight="8160" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Create Account" sheetId="1" r:id="rId1"/>
@@ -2157,8 +2157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2324,7 +2324,7 @@
   <dimension ref="A1:K101"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B16" sqref="B16:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3097,7 +3097,7 @@
   <dimension ref="A1:K101"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5674,8 +5674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B11:P49"/>
   <sheetViews>
-    <sheetView topLeftCell="L23" workbookViewId="0">
-      <selection activeCell="O40" sqref="O40"/>
+    <sheetView tabSelected="1" topLeftCell="L23" workbookViewId="0">
+      <selection activeCell="N42" sqref="N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
MBA Programme - Page development - Payments Workflow.
</commit_message>
<xml_diff>
--- a/src/test/java/BaseFramework/Data/DA.xlsx
+++ b/src/test/java/BaseFramework/Data/DA.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1424" uniqueCount="375">
   <si>
     <t>First Name</t>
   </si>
@@ -950,13 +950,7 @@
     <t xml:space="preserve">DA </t>
   </si>
   <si>
-    <t>MBA</t>
-  </si>
-  <si>
     <t>Management (MBA 1YFT)</t>
-  </si>
-  <si>
-    <t>Sam</t>
   </si>
   <si>
     <t xml:space="preserve"> Student - Create Account with existing email address</t>
@@ -1086,9 +1080,6 @@
     <t>List your second choice organisation(s) and role</t>
   </si>
   <si>
-    <t>samsonite.mba@mailinator.com</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
@@ -1140,41 +1131,67 @@
     <t>Criterion 2</t>
   </si>
   <si>
-    <t>Peer review of unit materials by unit/course coordinator
-For relevant items in the student survey, average or above average scores for all units taught e.g.
-• Appropriate teaching techniques are used by the teacher to enhance my learning.
-• The teacher is well prepared.
-• The teacher effectively used learning technologies to support my learning - Total 342</t>
-  </si>
-  <si>
-    <t>Deep knowledge of the discipline area
-Well planned learning activities designed to develop the students learning
-Scholarly/informed approach to learning design
-Thorough knowledge of the unit material and its contribution in the course
-Effective and appropriate use of learning technologies
-Effective unit/ course coordination - Total 320 Character</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Planned learning activities designed to develop the students’ learning                
-Sound knowledge of the unit content and material
-Unit outline that clearly details learning outcomes, teaching and learning activities and assessment Preparation of unit materials - 264 words
-</t>
-  </si>
-  <si>
-    <t>Deep knowledge of the discipline area
-Innovation in the design of teaching, including use of learning technologies    
-Effective preparation and management of tutors and teaching teams</t>
-  </si>
-  <si>
     <t>Hedge Funds</t>
   </si>
   <si>
     <t>United States of America</t>
   </si>
   <si>
-    <t>Thorough knowledge of the unit material and its contribution in the course
-Effective and appropriate use of learning technologies
-Effective unit/ course coordination</t>
+    <t>Payments</t>
+  </si>
+  <si>
+    <t>Card Number</t>
+  </si>
+  <si>
+    <t>Card Security Code</t>
+  </si>
+  <si>
+    <t>574</t>
+  </si>
+  <si>
+    <t>Expiry Date Month</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>Expiry Date Year</t>
+  </si>
+  <si>
+    <t>2041</t>
+  </si>
+  <si>
+    <t>Shami</t>
+  </si>
+  <si>
+    <t>Bam</t>
+  </si>
+  <si>
+    <t>shamibam.mba@mailinator.com</t>
+  </si>
+  <si>
+    <t>Deep knowledge of the discipline area Innovation in the design of teaching, including use of learning technologies Effective preparation and management of tutors and teaching teams</t>
+  </si>
+  <si>
+    <t>Peer review of unit materials by unit/course coordinator For relevant items in the student survey.</t>
+  </si>
+  <si>
+    <t>Planned learning activities designed to develop the students’ learning.</t>
+  </si>
+  <si>
+    <t>Deep knowledge of the discipline area Well planned learning activities designed to develop.</t>
+  </si>
+  <si>
+    <t>Thorough knowledge of the unit material and its contribution in the course</t>
+  </si>
+  <si>
+    <t>Card Holder Name</t>
+  </si>
+  <si>
+    <t>Sam MBA</t>
+  </si>
+  <si>
+    <t>4263970000005262</t>
   </si>
 </sst>
 </file>
@@ -3906,7 +3923,7 @@
         <v>246</v>
       </c>
       <c r="P4" s="90" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="5" spans="3:16" x14ac:dyDescent="0.25">
@@ -3924,7 +3941,7 @@
       <c r="J5" s="95"/>
       <c r="K5" s="57"/>
       <c r="M5" s="89" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="N5" s="91">
         <v>3</v>
@@ -3956,7 +3973,7 @@
       </c>
       <c r="K6" s="57"/>
       <c r="M6" s="89" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="N6" s="91">
         <v>7</v>
@@ -3972,7 +3989,7 @@
     <row r="7" spans="3:16" ht="26.25" x14ac:dyDescent="0.25">
       <c r="C7" s="56"/>
       <c r="D7" s="69" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E7" s="52" t="s">
         <v>231</v>
@@ -3981,14 +3998,14 @@
       <c r="G7" s="58"/>
       <c r="H7" s="56"/>
       <c r="I7" s="83" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="J7" s="93" t="s">
         <v>246</v>
       </c>
       <c r="K7" s="57"/>
       <c r="M7" s="89" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="N7" s="91">
         <v>7</v>
@@ -4079,7 +4096,7 @@
     <row r="12" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C12" s="56"/>
       <c r="D12" s="86" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E12" s="85" t="s">
         <v>231</v>
@@ -4088,7 +4105,7 @@
       <c r="G12" s="58"/>
       <c r="H12" s="56"/>
       <c r="I12" s="83" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J12" s="93" t="s">
         <v>246</v>
@@ -4098,7 +4115,7 @@
     <row r="13" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C13" s="56"/>
       <c r="D13" s="86" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E13" s="85" t="s">
         <v>231</v>
@@ -4107,7 +4124,7 @@
       <c r="G13" s="58"/>
       <c r="H13" s="56"/>
       <c r="I13" s="83" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="J13" s="93" t="s">
         <v>246</v>
@@ -4329,7 +4346,7 @@
         <v>246</v>
       </c>
       <c r="P27" s="90" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="28" spans="3:16" x14ac:dyDescent="0.25">
@@ -4347,7 +4364,7 @@
       <c r="J28" s="95"/>
       <c r="K28" s="57"/>
       <c r="M28" s="89" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="N28" s="91">
         <v>8</v>
@@ -4378,7 +4395,7 @@
       </c>
       <c r="K29" s="57"/>
       <c r="M29" s="89" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="N29" s="91">
         <v>7</v>
@@ -5182,7 +5199,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="88" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
@@ -5190,7 +5207,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
@@ -5217,7 +5234,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="88" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
@@ -5341,7 +5358,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -5349,7 +5366,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -5389,7 +5406,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="87" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -6114,7 +6131,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -6122,7 +6139,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -6162,7 +6179,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="87" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -6887,7 +6904,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -6895,7 +6912,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -6935,7 +6952,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="87" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -7659,7 +7676,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -7667,7 +7684,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -7707,7 +7724,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="87" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -8459,16 +8476,16 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:K131"/>
+  <dimension ref="A1:K140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E94" sqref="E94"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="89.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="55.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="99.7109375" customWidth="1" collapsed="1"/>
     <col min="3" max="4" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="6" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -8489,7 +8506,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>296</v>
+        <v>364</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -8497,7 +8514,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>294</v>
+        <v>365</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -8537,7 +8554,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="110" t="s">
-        <v>339</v>
+        <v>366</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -8553,7 +8570,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D8" t="s">
         <v>127</v>
@@ -8955,133 +8972,133 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B66" s="14"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="107" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B67" s="107"/>
     </row>
     <row r="68" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="108" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B68" s="109" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="108" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B69" s="109" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="108" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B70" s="109" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="108" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B71" s="109" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="108" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B72" s="109" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="107" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B73" s="107"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="108" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B74" s="109" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="108" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B75" s="109" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="108" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B76" s="109" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="108" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B77" s="109" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B78" s="14"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="108" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B79" s="109" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="108" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B80" s="109" t="s">
+        <v>346</v>
+      </c>
+      <c r="C80" t="s">
         <v>349</v>
       </c>
-      <c r="C80" t="s">
-        <v>352</v>
-      </c>
       <c r="D80" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="108" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B81" s="109" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="108" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B82" s="109" t="s">
         <v>46</v>
@@ -9089,66 +9106,66 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="108" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B83" s="109" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="114" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" ht="84" x14ac:dyDescent="0.25">
-      <c r="A84" s="114" t="s">
-        <v>354</v>
-      </c>
       <c r="B84" s="115" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="108" x14ac:dyDescent="0.25">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A85" s="114" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B85" s="115" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="114" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B86" s="115" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="60.75" x14ac:dyDescent="0.25">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A87" s="108" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B87" s="113" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="108" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B88" s="109" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="108" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B89" s="109" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="114" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B90" s="115" t="s">
-        <v>363</v>
+        <v>371</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -9273,131 +9290,179 @@
         <v>67</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="B114" s="13" t="s">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="B112" s="13" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A113" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="B113" s="12" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A114" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="B114" s="12" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A115" s="7" t="s">
-        <v>20</v>
+        <v>358</v>
       </c>
       <c r="B115" s="12" t="s">
-        <v>132</v>
+        <v>359</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A116" s="7" t="s">
-        <v>150</v>
+        <v>360</v>
       </c>
       <c r="B116" s="12" t="s">
-        <v>156</v>
+        <v>361</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A117" s="7" t="s">
-        <v>151</v>
+        <v>362</v>
       </c>
       <c r="B117" s="12" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A118" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="B118" s="12" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A119" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="B119" s="12" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A120" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="B120" s="12" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A121" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="B121" s="12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="13" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="B124" s="13" t="s">
+      <c r="B123" s="13" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A124" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B124" s="12" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A125" s="7" t="s">
-        <v>20</v>
+        <v>150</v>
       </c>
       <c r="B125" s="12" t="s">
-        <v>21</v>
+        <v>156</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A126" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B126" s="12" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A127" s="7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B127" s="12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A128" s="7" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B128" s="12" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A129" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B129" s="12" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A130" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B130" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B133" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A134" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B134" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A135" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B135" s="12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A136" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B136" s="12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A137" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B137" s="12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A138" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B138" s="12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A139" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="B130" s="12" t="s">
+      <c r="B139" s="12" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A131" s="7" t="s">
+    <row r="140" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A140" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="B131" s="12" t="s">
+      <c r="B140" s="12" t="s">
         <v>167</v>
       </c>
     </row>
@@ -9435,7 +9500,7 @@
   </controls>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Drop Down Values'!$C$11:$C$13</xm:f>

</xml_diff>

<commit_message>
MBA Programme - With Promo Code - End To End Complete.
</commit_message>
<xml_diff>
--- a/src/test/java/BaseFramework/Data/DA.xlsx
+++ b/src/test/java/BaseFramework/Data/DA.xlsx
@@ -27,7 +27,6 @@
     <sheet name="Sheet4" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1424" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="380">
   <si>
     <t>First Name</t>
   </si>
@@ -1161,15 +1160,6 @@
     <t>2041</t>
   </si>
   <si>
-    <t>Shami</t>
-  </si>
-  <si>
-    <t>Bam</t>
-  </si>
-  <si>
-    <t>shamibam.mba@mailinator.com</t>
-  </si>
-  <si>
     <t>Deep knowledge of the discipline area Innovation in the design of teaching, including use of learning technologies Effective preparation and management of tutors and teaching teams</t>
   </si>
   <si>
@@ -1192,6 +1182,30 @@
   </si>
   <si>
     <t>4263970000005262</t>
+  </si>
+  <si>
+    <t>Discount Code</t>
+  </si>
+  <si>
+    <t>EARLYBIRD</t>
+  </si>
+  <si>
+    <t>05/09/2000</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>green.dan@mailinator.com</t>
+  </si>
+  <si>
+    <t>Fname</t>
+  </si>
+  <si>
+    <t>Lname</t>
   </si>
 </sst>
 </file>
@@ -1908,6 +1922,21 @@
     <xf numFmtId="0" fontId="14" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1946,21 +1975,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2557,36 +2571,36 @@
   <sheetData>
     <row r="2" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="96" t="s">
+      <c r="C3" s="105" t="s">
         <v>249</v>
       </c>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="98"/>
-      <c r="M3" s="99" t="s">
+      <c r="D3" s="106"/>
+      <c r="E3" s="106"/>
+      <c r="F3" s="106"/>
+      <c r="G3" s="106"/>
+      <c r="H3" s="106"/>
+      <c r="I3" s="106"/>
+      <c r="J3" s="106"/>
+      <c r="K3" s="107"/>
+      <c r="M3" s="108" t="s">
         <v>245</v>
       </c>
-      <c r="N3" s="99"/>
-      <c r="O3" s="99"/>
+      <c r="N3" s="108"/>
+      <c r="O3" s="108"/>
     </row>
     <row r="4" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C4" s="56"/>
-      <c r="D4" s="100" t="s">
+      <c r="D4" s="109" t="s">
         <v>244</v>
       </c>
-      <c r="E4" s="100"/>
+      <c r="E4" s="109"/>
       <c r="F4" s="71"/>
       <c r="G4" s="72"/>
       <c r="H4" s="73"/>
-      <c r="I4" s="100" t="s">
+      <c r="I4" s="109" t="s">
         <v>245</v>
       </c>
-      <c r="J4" s="100"/>
+      <c r="J4" s="109"/>
       <c r="K4" s="57"/>
       <c r="M4" s="66" t="s">
         <v>253</v>
@@ -2600,17 +2614,17 @@
     </row>
     <row r="5" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C5" s="56"/>
-      <c r="D5" s="95" t="s">
+      <c r="D5" s="104" t="s">
         <v>235</v>
       </c>
-      <c r="E5" s="95"/>
+      <c r="E5" s="104"/>
       <c r="F5" s="71"/>
       <c r="G5" s="72"/>
       <c r="H5" s="73"/>
-      <c r="I5" s="95" t="s">
+      <c r="I5" s="104" t="s">
         <v>235</v>
       </c>
-      <c r="J5" s="95"/>
+      <c r="J5" s="104"/>
       <c r="K5" s="57"/>
       <c r="M5" s="66" t="s">
         <v>250</v>
@@ -2739,17 +2753,17 @@
     </row>
     <row r="12" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C12" s="56"/>
-      <c r="D12" s="95" t="s">
+      <c r="D12" s="104" t="s">
         <v>243</v>
       </c>
-      <c r="E12" s="95"/>
+      <c r="E12" s="104"/>
       <c r="F12" s="71"/>
       <c r="G12" s="72"/>
       <c r="H12" s="73"/>
-      <c r="I12" s="95" t="s">
+      <c r="I12" s="104" t="s">
         <v>243</v>
       </c>
-      <c r="J12" s="95"/>
+      <c r="J12" s="104"/>
       <c r="K12" s="57"/>
     </row>
     <row r="13" spans="3:16" x14ac:dyDescent="0.25">
@@ -2900,36 +2914,36 @@
     </row>
     <row r="22" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="96" t="s">
+      <c r="C23" s="105" t="s">
         <v>248</v>
       </c>
-      <c r="D23" s="97"/>
-      <c r="E23" s="97"/>
-      <c r="F23" s="97"/>
-      <c r="G23" s="97"/>
-      <c r="H23" s="97"/>
-      <c r="I23" s="97"/>
-      <c r="J23" s="97"/>
-      <c r="K23" s="98"/>
-      <c r="M23" s="99" t="s">
+      <c r="D23" s="106"/>
+      <c r="E23" s="106"/>
+      <c r="F23" s="106"/>
+      <c r="G23" s="106"/>
+      <c r="H23" s="106"/>
+      <c r="I23" s="106"/>
+      <c r="J23" s="106"/>
+      <c r="K23" s="107"/>
+      <c r="M23" s="108" t="s">
         <v>252</v>
       </c>
-      <c r="N23" s="99"/>
-      <c r="O23" s="99"/>
+      <c r="N23" s="108"/>
+      <c r="O23" s="108"/>
     </row>
     <row r="24" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C24" s="56"/>
-      <c r="D24" s="100" t="s">
+      <c r="D24" s="109" t="s">
         <v>244</v>
       </c>
-      <c r="E24" s="100"/>
+      <c r="E24" s="109"/>
       <c r="F24" s="71"/>
       <c r="G24" s="74"/>
       <c r="H24" s="73"/>
-      <c r="I24" s="94" t="s">
+      <c r="I24" s="103" t="s">
         <v>245</v>
       </c>
-      <c r="J24" s="94"/>
+      <c r="J24" s="103"/>
       <c r="K24" s="57"/>
       <c r="M24" s="66" t="s">
         <v>253</v>
@@ -2943,17 +2957,17 @@
     </row>
     <row r="25" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C25" s="56"/>
-      <c r="D25" s="95" t="s">
+      <c r="D25" s="104" t="s">
         <v>247</v>
       </c>
-      <c r="E25" s="95"/>
+      <c r="E25" s="104"/>
       <c r="F25" s="71"/>
       <c r="G25" s="74"/>
       <c r="H25" s="73"/>
-      <c r="I25" s="95" t="s">
+      <c r="I25" s="104" t="s">
         <v>247</v>
       </c>
-      <c r="J25" s="95"/>
+      <c r="J25" s="104"/>
       <c r="K25" s="57"/>
       <c r="M25" s="66" t="s">
         <v>250</v>
@@ -3148,15 +3162,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="113" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
-      <c r="E1" s="104"/>
-      <c r="F1" s="104"/>
-      <c r="G1" s="104"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -3368,13 +3382,13 @@
   </cols>
   <sheetData>
     <row r="11" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="F11" s="106" t="s">
+      <c r="F11" s="115" t="s">
         <v>207</v>
       </c>
-      <c r="G11" s="106"/>
-      <c r="H11" s="106"/>
-      <c r="I11" s="106"/>
-      <c r="J11" s="106"/>
+      <c r="G11" s="115"/>
+      <c r="H11" s="115"/>
+      <c r="I11" s="115"/>
+      <c r="J11" s="115"/>
     </row>
     <row r="12" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
@@ -3504,11 +3518,11 @@
       <c r="P33" s="2"/>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E34" s="105" t="s">
+      <c r="E34" s="114" t="s">
         <v>173</v>
       </c>
-      <c r="F34" s="105"/>
-      <c r="G34" s="105"/>
+      <c r="F34" s="114"/>
+      <c r="G34" s="114"/>
       <c r="I34" s="17" t="s">
         <v>179</v>
       </c>
@@ -3881,37 +3895,37 @@
   <sheetData>
     <row r="2" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="96" t="s">
+      <c r="C3" s="105" t="s">
         <v>292</v>
       </c>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="98"/>
-      <c r="M3" s="101" t="s">
+      <c r="D3" s="106"/>
+      <c r="E3" s="106"/>
+      <c r="F3" s="106"/>
+      <c r="G3" s="106"/>
+      <c r="H3" s="106"/>
+      <c r="I3" s="106"/>
+      <c r="J3" s="106"/>
+      <c r="K3" s="107"/>
+      <c r="M3" s="110" t="s">
         <v>245</v>
       </c>
-      <c r="N3" s="102"/>
-      <c r="O3" s="102"/>
-      <c r="P3" s="103"/>
+      <c r="N3" s="111"/>
+      <c r="O3" s="111"/>
+      <c r="P3" s="112"/>
     </row>
     <row r="4" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C4" s="56"/>
-      <c r="D4" s="100" t="s">
+      <c r="D4" s="109" t="s">
         <v>244</v>
       </c>
-      <c r="E4" s="100"/>
+      <c r="E4" s="109"/>
       <c r="F4" s="71"/>
       <c r="G4" s="72"/>
       <c r="H4" s="73"/>
-      <c r="I4" s="100" t="s">
+      <c r="I4" s="109" t="s">
         <v>245</v>
       </c>
-      <c r="J4" s="100"/>
+      <c r="J4" s="109"/>
       <c r="K4" s="57"/>
       <c r="M4" s="89" t="s">
         <v>253</v>
@@ -3928,17 +3942,17 @@
     </row>
     <row r="5" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C5" s="56"/>
-      <c r="D5" s="95" t="s">
+      <c r="D5" s="104" t="s">
         <v>235</v>
       </c>
-      <c r="E5" s="95"/>
+      <c r="E5" s="104"/>
       <c r="F5" s="71"/>
       <c r="G5" s="72"/>
       <c r="H5" s="73"/>
-      <c r="I5" s="95" t="s">
+      <c r="I5" s="104" t="s">
         <v>235</v>
       </c>
-      <c r="J5" s="95"/>
+      <c r="J5" s="104"/>
       <c r="K5" s="57"/>
       <c r="M5" s="89" t="s">
         <v>308</v>
@@ -4144,17 +4158,17 @@
     </row>
     <row r="15" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C15" s="56"/>
-      <c r="D15" s="95" t="s">
+      <c r="D15" s="104" t="s">
         <v>243</v>
       </c>
-      <c r="E15" s="95"/>
+      <c r="E15" s="104"/>
       <c r="F15" s="71"/>
       <c r="G15" s="72"/>
       <c r="H15" s="73"/>
-      <c r="I15" s="95" t="s">
+      <c r="I15" s="104" t="s">
         <v>243</v>
       </c>
-      <c r="J15" s="95"/>
+      <c r="J15" s="104"/>
       <c r="K15" s="57"/>
     </row>
     <row r="16" spans="3:16" x14ac:dyDescent="0.25">
@@ -4304,37 +4318,37 @@
     </row>
     <row r="25" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="96" t="s">
+      <c r="C26" s="105" t="s">
         <v>248</v>
       </c>
-      <c r="D26" s="97"/>
-      <c r="E26" s="97"/>
-      <c r="F26" s="97"/>
-      <c r="G26" s="97"/>
-      <c r="H26" s="97"/>
-      <c r="I26" s="97"/>
-      <c r="J26" s="97"/>
-      <c r="K26" s="98"/>
-      <c r="M26" s="99" t="s">
+      <c r="D26" s="106"/>
+      <c r="E26" s="106"/>
+      <c r="F26" s="106"/>
+      <c r="G26" s="106"/>
+      <c r="H26" s="106"/>
+      <c r="I26" s="106"/>
+      <c r="J26" s="106"/>
+      <c r="K26" s="107"/>
+      <c r="M26" s="108" t="s">
         <v>252</v>
       </c>
-      <c r="N26" s="99"/>
-      <c r="O26" s="99"/>
-      <c r="P26" s="99"/>
+      <c r="N26" s="108"/>
+      <c r="O26" s="108"/>
+      <c r="P26" s="108"/>
     </row>
     <row r="27" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C27" s="56"/>
-      <c r="D27" s="100" t="s">
+      <c r="D27" s="109" t="s">
         <v>244</v>
       </c>
-      <c r="E27" s="100"/>
+      <c r="E27" s="109"/>
       <c r="F27" s="71"/>
       <c r="G27" s="74"/>
       <c r="H27" s="73"/>
-      <c r="I27" s="94" t="s">
+      <c r="I27" s="103" t="s">
         <v>245</v>
       </c>
-      <c r="J27" s="94"/>
+      <c r="J27" s="103"/>
       <c r="K27" s="57"/>
       <c r="M27" s="89" t="s">
         <v>253</v>
@@ -4351,17 +4365,17 @@
     </row>
     <row r="28" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C28" s="56"/>
-      <c r="D28" s="95" t="s">
+      <c r="D28" s="104" t="s">
         <v>247</v>
       </c>
-      <c r="E28" s="95"/>
+      <c r="E28" s="104"/>
       <c r="F28" s="71"/>
       <c r="G28" s="74"/>
       <c r="H28" s="73"/>
-      <c r="I28" s="95" t="s">
+      <c r="I28" s="104" t="s">
         <v>247</v>
       </c>
-      <c r="J28" s="95"/>
+      <c r="J28" s="104"/>
       <c r="K28" s="57"/>
       <c r="M28" s="89" t="s">
         <v>308</v>
@@ -4587,36 +4601,36 @@
   <sheetData>
     <row r="2" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="96" t="s">
+      <c r="C3" s="105" t="s">
         <v>292</v>
       </c>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="98"/>
-      <c r="M3" s="99" t="s">
+      <c r="D3" s="106"/>
+      <c r="E3" s="106"/>
+      <c r="F3" s="106"/>
+      <c r="G3" s="106"/>
+      <c r="H3" s="106"/>
+      <c r="I3" s="106"/>
+      <c r="J3" s="106"/>
+      <c r="K3" s="107"/>
+      <c r="M3" s="108" t="s">
         <v>245</v>
       </c>
-      <c r="N3" s="99"/>
-      <c r="O3" s="99"/>
+      <c r="N3" s="108"/>
+      <c r="O3" s="108"/>
     </row>
     <row r="4" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C4" s="56"/>
-      <c r="D4" s="100" t="s">
+      <c r="D4" s="109" t="s">
         <v>244</v>
       </c>
-      <c r="E4" s="100"/>
+      <c r="E4" s="109"/>
       <c r="F4" s="71"/>
       <c r="G4" s="72"/>
       <c r="H4" s="73"/>
-      <c r="I4" s="100" t="s">
+      <c r="I4" s="109" t="s">
         <v>245</v>
       </c>
-      <c r="J4" s="100"/>
+      <c r="J4" s="109"/>
       <c r="K4" s="57"/>
       <c r="M4" s="66" t="s">
         <v>253</v>
@@ -4630,17 +4644,17 @@
     </row>
     <row r="5" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C5" s="56"/>
-      <c r="D5" s="95" t="s">
+      <c r="D5" s="104" t="s">
         <v>235</v>
       </c>
-      <c r="E5" s="95"/>
+      <c r="E5" s="104"/>
       <c r="F5" s="71"/>
       <c r="G5" s="72"/>
       <c r="H5" s="73"/>
-      <c r="I5" s="95" t="s">
+      <c r="I5" s="104" t="s">
         <v>235</v>
       </c>
-      <c r="J5" s="95"/>
+      <c r="J5" s="104"/>
       <c r="K5" s="57"/>
       <c r="M5" s="66" t="s">
         <v>293</v>
@@ -4769,17 +4783,17 @@
     </row>
     <row r="12" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C12" s="56"/>
-      <c r="D12" s="95" t="s">
+      <c r="D12" s="104" t="s">
         <v>243</v>
       </c>
-      <c r="E12" s="95"/>
+      <c r="E12" s="104"/>
       <c r="F12" s="71"/>
       <c r="G12" s="72"/>
       <c r="H12" s="73"/>
-      <c r="I12" s="95" t="s">
+      <c r="I12" s="104" t="s">
         <v>243</v>
       </c>
-      <c r="J12" s="95"/>
+      <c r="J12" s="104"/>
       <c r="K12" s="57"/>
     </row>
     <row r="13" spans="3:16" x14ac:dyDescent="0.25">
@@ -4930,36 +4944,36 @@
     </row>
     <row r="22" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="96" t="s">
+      <c r="C23" s="105" t="s">
         <v>248</v>
       </c>
-      <c r="D23" s="97"/>
-      <c r="E23" s="97"/>
-      <c r="F23" s="97"/>
-      <c r="G23" s="97"/>
-      <c r="H23" s="97"/>
-      <c r="I23" s="97"/>
-      <c r="J23" s="97"/>
-      <c r="K23" s="98"/>
-      <c r="M23" s="99" t="s">
+      <c r="D23" s="106"/>
+      <c r="E23" s="106"/>
+      <c r="F23" s="106"/>
+      <c r="G23" s="106"/>
+      <c r="H23" s="106"/>
+      <c r="I23" s="106"/>
+      <c r="J23" s="106"/>
+      <c r="K23" s="107"/>
+      <c r="M23" s="108" t="s">
         <v>252</v>
       </c>
-      <c r="N23" s="99"/>
-      <c r="O23" s="99"/>
+      <c r="N23" s="108"/>
+      <c r="O23" s="108"/>
     </row>
     <row r="24" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C24" s="56"/>
-      <c r="D24" s="100" t="s">
+      <c r="D24" s="109" t="s">
         <v>244</v>
       </c>
-      <c r="E24" s="100"/>
+      <c r="E24" s="109"/>
       <c r="F24" s="71"/>
       <c r="G24" s="74"/>
       <c r="H24" s="73"/>
-      <c r="I24" s="94" t="s">
+      <c r="I24" s="103" t="s">
         <v>245</v>
       </c>
-      <c r="J24" s="94"/>
+      <c r="J24" s="103"/>
       <c r="K24" s="57"/>
       <c r="M24" s="66" t="s">
         <v>253</v>
@@ -4973,17 +4987,17 @@
     </row>
     <row r="25" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C25" s="56"/>
-      <c r="D25" s="95" t="s">
+      <c r="D25" s="104" t="s">
         <v>247</v>
       </c>
-      <c r="E25" s="95"/>
+      <c r="E25" s="104"/>
       <c r="F25" s="71"/>
       <c r="G25" s="74"/>
       <c r="H25" s="73"/>
-      <c r="I25" s="95" t="s">
+      <c r="I25" s="104" t="s">
         <v>247</v>
       </c>
-      <c r="J25" s="95"/>
+      <c r="J25" s="104"/>
       <c r="K25" s="57"/>
       <c r="M25" s="66" t="s">
         <v>250</v>
@@ -5142,11 +5156,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="C23:K23"/>
     <mergeCell ref="M23:O23"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="I24:J24"/>
@@ -5156,6 +5165,11 @@
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="I5:J5"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="C23:K23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8478,8 +8492,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:K140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B111" sqref="B111"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8506,7 +8520,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>364</v>
+        <v>375</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -8514,7 +8528,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>365</v>
+        <v>376</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -8527,8 +8541,8 @@
       <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>18</v>
+      <c r="B4" s="12" t="s">
+        <v>374</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>22</v>
@@ -8542,7 +8556,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C5" s="28" t="s">
         <v>139</v>
@@ -8553,8 +8567,8 @@
       <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="110" t="s">
-        <v>366</v>
+      <c r="B6" s="97" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -8610,6 +8624,20 @@
       <c r="B12" s="8" t="s">
         <v>17</v>
       </c>
+      <c r="E12" t="s">
+        <v>378</v>
+      </c>
+      <c r="F12" s="46" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>379</v>
+      </c>
+      <c r="F13" s="46" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
@@ -8977,86 +9005,86 @@
       <c r="B66" s="14"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="107" t="s">
+      <c r="A67" s="94" t="s">
         <v>322</v>
       </c>
-      <c r="B67" s="107"/>
+      <c r="B67" s="94"/>
     </row>
     <row r="68" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="108" t="s">
+      <c r="A68" s="95" t="s">
         <v>319</v>
       </c>
-      <c r="B68" s="109" t="s">
+      <c r="B68" s="96" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="108" t="s">
+      <c r="A69" s="95" t="s">
         <v>320</v>
       </c>
-      <c r="B69" s="109" t="s">
+      <c r="B69" s="96" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="108" t="s">
+      <c r="A70" s="95" t="s">
         <v>323</v>
       </c>
-      <c r="B70" s="109" t="s">
+      <c r="B70" s="96" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="108" t="s">
+      <c r="A71" s="95" t="s">
         <v>321</v>
       </c>
-      <c r="B71" s="109" t="s">
+      <c r="B71" s="96" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="108" t="s">
+      <c r="A72" s="95" t="s">
         <v>341</v>
       </c>
-      <c r="B72" s="109" t="s">
+      <c r="B72" s="96" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="107" t="s">
+      <c r="A73" s="94" t="s">
         <v>324</v>
       </c>
-      <c r="B73" s="107"/>
+      <c r="B73" s="94"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="108" t="s">
+      <c r="A74" s="95" t="s">
         <v>319</v>
       </c>
-      <c r="B74" s="109" t="s">
+      <c r="B74" s="96" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="108" t="s">
+      <c r="A75" s="95" t="s">
         <v>320</v>
       </c>
-      <c r="B75" s="109" t="s">
+      <c r="B75" s="96" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="108" t="s">
+      <c r="A76" s="95" t="s">
         <v>325</v>
       </c>
-      <c r="B76" s="109" t="s">
+      <c r="B76" s="96" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="108" t="s">
+      <c r="A77" s="95" t="s">
         <v>326</v>
       </c>
-      <c r="B77" s="109" t="s">
+      <c r="B77" s="96" t="s">
         <v>346</v>
       </c>
     </row>
@@ -9067,18 +9095,18 @@
       <c r="B78" s="14"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="108" t="s">
+      <c r="A79" s="95" t="s">
         <v>328</v>
       </c>
-      <c r="B79" s="109" t="s">
+      <c r="B79" s="96" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="108" t="s">
+      <c r="A80" s="95" t="s">
         <v>329</v>
       </c>
-      <c r="B80" s="109" t="s">
+      <c r="B80" s="96" t="s">
         <v>346</v>
       </c>
       <c r="C80" t="s">
@@ -9089,83 +9117,83 @@
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="108" t="s">
+      <c r="A81" s="95" t="s">
         <v>330</v>
       </c>
-      <c r="B81" s="109" t="s">
+      <c r="B81" s="96" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="108" t="s">
+      <c r="A82" s="95" t="s">
         <v>331</v>
       </c>
-      <c r="B82" s="109" t="s">
+      <c r="B82" s="96" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="108" t="s">
+      <c r="A83" s="95" t="s">
         <v>332</v>
       </c>
-      <c r="B83" s="109" t="s">
+      <c r="B83" s="96" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="114" t="s">
+      <c r="A84" s="101" t="s">
         <v>351</v>
       </c>
-      <c r="B84" s="115" t="s">
-        <v>369</v>
+      <c r="B84" s="102" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="24" x14ac:dyDescent="0.25">
-      <c r="A85" s="114" t="s">
+      <c r="A85" s="101" t="s">
         <v>353</v>
       </c>
-      <c r="B85" s="115" t="s">
+      <c r="B85" s="102" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="101" t="s">
+        <v>352</v>
+      </c>
+      <c r="B86" s="102" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="95" t="s">
+        <v>333</v>
+      </c>
+      <c r="B87" s="100" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="95" t="s">
+        <v>334</v>
+      </c>
+      <c r="B88" s="96" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="95" t="s">
+        <v>335</v>
+      </c>
+      <c r="B89" s="96" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="101" t="s">
+        <v>336</v>
+      </c>
+      <c r="B90" s="102" t="s">
         <v>368</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="114" t="s">
-        <v>352</v>
-      </c>
-      <c r="B86" s="115" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A87" s="108" t="s">
-        <v>333</v>
-      </c>
-      <c r="B87" s="113" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="108" t="s">
-        <v>334</v>
-      </c>
-      <c r="B88" s="109" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="108" t="s">
-        <v>335</v>
-      </c>
-      <c r="B89" s="109" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="114" t="s">
-        <v>336</v>
-      </c>
-      <c r="B90" s="115" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -9231,8 +9259,8 @@
       </c>
     </row>
     <row r="99" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A99" s="111"/>
-      <c r="B99" s="112"/>
+      <c r="A99" s="98"/>
+      <c r="B99" s="99"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="13" t="s">
@@ -9300,10 +9328,10 @@
     </row>
     <row r="113" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A113" s="7" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B113" s="12" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
@@ -9311,7 +9339,7 @@
         <v>357</v>
       </c>
       <c r="B114" s="12" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
@@ -9336,6 +9364,14 @@
       </c>
       <c r="B117" s="12" t="s">
         <v>363</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A118" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="B118" s="12" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Short Course - End To End Complete.
</commit_message>
<xml_diff>
--- a/src/test/java/BaseFramework/Data/DA.xlsx
+++ b/src/test/java/BaseFramework/Data/DA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11775" windowHeight="8160" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11775" windowHeight="8160" firstSheet="7" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Result Summary" sheetId="11" r:id="rId1"/>
@@ -21,10 +21,11 @@
     <sheet name="Withdraw_Application" sheetId="8" r:id="rId7"/>
     <sheet name="Doctoral_Chem_Research_PHD" sheetId="10" r:id="rId8"/>
     <sheet name="Management_MBA" sheetId="13" r:id="rId9"/>
-    <sheet name="Drop Down Values" sheetId="6" r:id="rId10"/>
-    <sheet name="Requirments Sheet" sheetId="3" r:id="rId11"/>
-    <sheet name="Sheet3" sheetId="9" r:id="rId12"/>
-    <sheet name="Sheet4" sheetId="14" r:id="rId13"/>
+    <sheet name="ShortCourse" sheetId="16" r:id="rId10"/>
+    <sheet name="Drop Down Values" sheetId="6" r:id="rId11"/>
+    <sheet name="Requirments Sheet" sheetId="3" r:id="rId12"/>
+    <sheet name="Sheet3" sheetId="9" r:id="rId13"/>
+    <sheet name="Sheet4" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1538" uniqueCount="396">
   <si>
     <t>First Name</t>
   </si>
@@ -1206,6 +1207,54 @@
   </si>
   <si>
     <t>Lname</t>
+  </si>
+  <si>
+    <t>shortcourse@mailinator.com</t>
+  </si>
+  <si>
+    <t>Visiting</t>
+  </si>
+  <si>
+    <t>Global innovation Design (Occasional)</t>
+  </si>
+  <si>
+    <t>Global innovation Design (Occasional) - NOT REQUIRED</t>
+  </si>
+  <si>
+    <t>Please select the framework under which you are applying</t>
+  </si>
+  <si>
+    <t>Please indicate your intended study plans for this period of short term study</t>
+  </si>
+  <si>
+    <t>Proposed start date</t>
+  </si>
+  <si>
+    <t>Proposed end date</t>
+  </si>
+  <si>
+    <t>Erasmus Study (Exchange)</t>
+  </si>
+  <si>
+    <t>Modules, including projects (from Imperial College’s curriculum)</t>
+  </si>
+  <si>
+    <t>07/01/2019</t>
+  </si>
+  <si>
+    <t>30/11/2019</t>
+  </si>
+  <si>
+    <t>English Language</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Angus</t>
+  </si>
+  <si>
+    <t>angus.georgia@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -1785,7 +1834,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1976,6 +2025,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent5" xfId="1" builtinId="45"/>
@@ -2023,6 +2073,10 @@
 </file>
 
 <file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D11A-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX6.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D11A-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
 </file>
 
@@ -2257,6 +2311,58 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s21505"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>40</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>457200</xdr:colOff>
+          <xdr:row>41</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="30721" name="Control 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s30721"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3147,11 +3253,521 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet6"/>
+  <dimension ref="A1:F54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="89.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="99.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>393</v>
+      </c>
+      <c r="C2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>394</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>374</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="97" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>382</v>
+      </c>
+      <c r="D8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>378</v>
+      </c>
+      <c r="F12" s="46" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>379</v>
+      </c>
+      <c r="F13" s="46" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B17" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>259</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B18" s="50" t="s">
+        <v>383</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="B22" s="116" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="B23" s="116" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="D25" s="75"/>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="49" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="50" t="s">
+        <v>255</v>
+      </c>
+      <c r="C34" s="28"/>
+    </row>
+    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="50" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="13" t="s">
+        <v>392</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A44" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A46" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="B47" s="76" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A52" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A53" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A54" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <controls>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="30721" r:id="rId4" name="Control 1">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>40</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>457200</xdr:colOff>
+                <xdr:row>41</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="30721" r:id="rId4" name="Control 1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </controls>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$G$3:$G$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>F4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$C$31:$C$32</xm:f>
+          </x14:formula1>
+          <xm:sqref>B17</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$C$22:$C$29</xm:f>
+          </x14:formula1>
+          <xm:sqref>B16</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$C$15:$C$16</xm:f>
+          </x14:formula1>
+          <xm:sqref>B10</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$C$3:$C$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$C$11:$C$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>B5</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3333,6 +3949,11 @@
         <v>221</v>
       </c>
     </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="2" t="s">
+        <v>381</v>
+      </c>
+    </row>
     <row r="30" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="2:3" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B31" s="31" t="s">
@@ -3353,10 +3974,11 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B11:P49"/>
   <sheetViews>
@@ -3772,7 +4394,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E6:F13"/>
   <sheetViews>
@@ -3836,7 +4458,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="O18:O20"/>
   <sheetViews>
@@ -5343,8 +5965,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8492,7 +9114,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:K140"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F12" sqref="F12:F13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Short Course Data - End To End Complete.
</commit_message>
<xml_diff>
--- a/src/test/java/BaseFramework/Data/DA.xlsx
+++ b/src/test/java/BaseFramework/Data/DA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11775" windowHeight="8160" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11775" windowHeight="7830" firstSheet="6" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Result Summary" sheetId="11" r:id="rId1"/>
@@ -22,10 +22,11 @@
     <sheet name="Doctoral_Chem_Research_PHD" sheetId="10" r:id="rId8"/>
     <sheet name="Management_MBA" sheetId="13" r:id="rId9"/>
     <sheet name="ShortCourse" sheetId="16" r:id="rId10"/>
-    <sheet name="Drop Down Values" sheetId="6" r:id="rId11"/>
-    <sheet name="Requirments Sheet" sheetId="3" r:id="rId12"/>
-    <sheet name="Sheet3" sheetId="9" r:id="rId13"/>
-    <sheet name="Sheet4" sheetId="14" r:id="rId14"/>
+    <sheet name="ShortCourse Data" sheetId="17" r:id="rId11"/>
+    <sheet name="Drop Down Values" sheetId="6" r:id="rId12"/>
+    <sheet name="Requirments Sheet" sheetId="3" r:id="rId13"/>
+    <sheet name="Sheet3" sheetId="9" r:id="rId14"/>
+    <sheet name="Sheet4" sheetId="14" r:id="rId15"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1561" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1734" uniqueCount="457">
   <si>
     <t>First Name</t>
   </si>
@@ -956,15 +957,6 @@
     <t xml:space="preserve"> Student - Create Account with existing email address</t>
   </si>
   <si>
-    <t>doc.nov01tst@mailinator.com</t>
-  </si>
-  <si>
-    <t>TST</t>
-  </si>
-  <si>
-    <t>DOCRES_nov1</t>
-  </si>
-  <si>
     <t>refTst</t>
   </si>
   <si>
@@ -983,13 +975,7 @@
     <t>Defer_nov1tst</t>
   </si>
   <si>
-    <t>tstnov01</t>
-  </si>
-  <si>
     <t>envtest</t>
-  </si>
-  <si>
-    <t>testnove1@mailinator.com</t>
   </si>
   <si>
     <t>DA - WFE</t>
@@ -1299,6 +1285,162 @@
   </si>
   <si>
     <t>English Language Upload button missing  Defect</t>
+  </si>
+  <si>
+    <t>novSixteen</t>
+  </si>
+  <si>
+    <t>devl</t>
+  </si>
+  <si>
+    <t>sixteen.nov@mailinator.com</t>
+  </si>
+  <si>
+    <t>tstnov01_123</t>
+  </si>
+  <si>
+    <t>testnove123@mailinator.com</t>
+  </si>
+  <si>
+    <t>School of Public Health Taught Programmes (Occasional FT)</t>
+  </si>
+  <si>
+    <t>Devl2</t>
+  </si>
+  <si>
+    <t>med2.devl2@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Med2 </t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Autumn 2019-2020 - School of Public Health Taught Programmes (Occasional FT)</t>
+  </si>
+  <si>
+    <t>Prgramme and Entry Term</t>
+  </si>
+  <si>
+    <t>Med1</t>
+  </si>
+  <si>
+    <t>Devl1</t>
+  </si>
+  <si>
+    <t>med1.devl1@mailinator.com</t>
+  </si>
+  <si>
+    <t>Med3</t>
+  </si>
+  <si>
+    <t>Devl3</t>
+  </si>
+  <si>
+    <t>med3.devl3@mailinator.com</t>
+  </si>
+  <si>
+    <t>Med4</t>
+  </si>
+  <si>
+    <t>Devl4</t>
+  </si>
+  <si>
+    <t>Med5</t>
+  </si>
+  <si>
+    <t>Devl5</t>
+  </si>
+  <si>
+    <t>Med6</t>
+  </si>
+  <si>
+    <t>Devl6</t>
+  </si>
+  <si>
+    <t>Med7</t>
+  </si>
+  <si>
+    <t>Devl7</t>
+  </si>
+  <si>
+    <t>Med8</t>
+  </si>
+  <si>
+    <t>Devl8</t>
+  </si>
+  <si>
+    <t>Med9</t>
+  </si>
+  <si>
+    <t>Devl9</t>
+  </si>
+  <si>
+    <t>Med10</t>
+  </si>
+  <si>
+    <t>Devl10</t>
+  </si>
+  <si>
+    <t>Med11</t>
+  </si>
+  <si>
+    <t>Devl11</t>
+  </si>
+  <si>
+    <t>Med12</t>
+  </si>
+  <si>
+    <t>Devl12</t>
+  </si>
+  <si>
+    <t>Med13</t>
+  </si>
+  <si>
+    <t>Devl13</t>
+  </si>
+  <si>
+    <t>Med14</t>
+  </si>
+  <si>
+    <t>Devl14</t>
+  </si>
+  <si>
+    <t>Med15</t>
+  </si>
+  <si>
+    <t>Devl15</t>
+  </si>
+  <si>
+    <t>Med16</t>
+  </si>
+  <si>
+    <t>Devl16</t>
+  </si>
+  <si>
+    <t>Med17</t>
+  </si>
+  <si>
+    <t>Devl17</t>
+  </si>
+  <si>
+    <t>Med18</t>
+  </si>
+  <si>
+    <t>Devl18</t>
+  </si>
+  <si>
+    <t>Med19</t>
+  </si>
+  <si>
+    <t>Devl19</t>
+  </si>
+  <si>
+    <t>Med20</t>
+  </si>
+  <si>
+    <t>Devl20</t>
   </si>
 </sst>
 </file>
@@ -1308,7 +1450,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1427,8 +1569,16 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="22">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1551,6 +1701,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2776A"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1917,7 +2073,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2133,6 +2289,14 @@
     <xf numFmtId="0" fontId="12" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="8" xfId="2" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent5" xfId="1" builtinId="45"/>
@@ -2184,6 +2348,10 @@
 </file>
 
 <file path=xl/activeX/activeX6.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D11A-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX7.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D11A-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
 </file>
 
@@ -2470,6 +2638,58 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s30721"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>40</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>457200</xdr:colOff>
+          <xdr:row>41</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="31745" name="Control 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s31745"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3365,7 +3585,7 @@
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3392,10 +3612,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="C2" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -3403,7 +3623,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -3417,7 +3637,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>22</v>
@@ -3443,7 +3663,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="97" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -3459,7 +3679,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="D8" t="s">
         <v>127</v>
@@ -3500,18 +3720,18 @@
         <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="F12" s="46" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="F13" s="46" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -3527,7 +3747,7 @@
         <v>26</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="C16" s="28" t="s">
         <v>139</v>
@@ -3552,7 +3772,7 @@
         <v>126</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="C18" s="28" t="s">
         <v>254</v>
@@ -3568,34 +3788,34 @@
     </row>
     <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="B22" s="116" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="B23" s="116" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
@@ -3714,7 +3934,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="B42" s="13" t="s">
         <v>112</v>
@@ -3870,6 +4090,800 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet7"/>
+  <dimension ref="A1:G54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="89.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="99.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="64.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>455</v>
+      </c>
+      <c r="C2" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>456</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>368</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="97" t="str">
+        <f>CONCATENATE(B2,".",B3,"@mailinator.com")</f>
+        <v>Med20.Devl20@mailinator.com</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>410</v>
+      </c>
+      <c r="D8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>371</v>
+      </c>
+      <c r="F12" s="46" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>372</v>
+      </c>
+      <c r="F13" s="46" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B17" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>259</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B18" s="50" t="s">
+        <v>410</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="B22" s="116" t="s">
+        <v>383</v>
+      </c>
+      <c r="D22" s="89" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="89" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="89" t="s">
+        <v>414</v>
+      </c>
+      <c r="G22" s="89" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="B23" s="116" t="s">
+        <v>384</v>
+      </c>
+      <c r="D23" s="130" t="s">
+        <v>417</v>
+      </c>
+      <c r="E23" s="130" t="s">
+        <v>418</v>
+      </c>
+      <c r="F23" s="131" t="s">
+        <v>419</v>
+      </c>
+      <c r="G23" s="132" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="130" t="s">
+        <v>413</v>
+      </c>
+      <c r="E24" s="130" t="s">
+        <v>411</v>
+      </c>
+      <c r="F24" s="131" t="s">
+        <v>412</v>
+      </c>
+      <c r="G24" s="132" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="D25" s="130" t="s">
+        <v>420</v>
+      </c>
+      <c r="E25" s="130" t="s">
+        <v>421</v>
+      </c>
+      <c r="F25" s="131" t="s">
+        <v>422</v>
+      </c>
+      <c r="G25" s="132" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="D26" s="130" t="s">
+        <v>423</v>
+      </c>
+      <c r="E26" s="130" t="s">
+        <v>424</v>
+      </c>
+      <c r="F26" s="131" t="str">
+        <f>CONCATENATE(D26,".",E26,"@mailinator.com")</f>
+        <v>Med4.Devl4@mailinator.com</v>
+      </c>
+      <c r="G26" s="132" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="D27" s="130" t="s">
+        <v>425</v>
+      </c>
+      <c r="E27" s="130" t="s">
+        <v>426</v>
+      </c>
+      <c r="F27" s="131" t="str">
+        <f>CONCATENATE(D27,".",E27,"@mailinator.com")</f>
+        <v>Med5.Devl5@mailinator.com</v>
+      </c>
+      <c r="G27" s="132" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="D28" s="130" t="s">
+        <v>427</v>
+      </c>
+      <c r="E28" s="130" t="s">
+        <v>428</v>
+      </c>
+      <c r="F28" s="131" t="str">
+        <f>CONCATENATE(D28,".",E28,"@mailinator.com")</f>
+        <v>Med6.Devl6@mailinator.com</v>
+      </c>
+      <c r="G28" s="132" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="D29" s="130" t="s">
+        <v>429</v>
+      </c>
+      <c r="E29" s="130" t="s">
+        <v>430</v>
+      </c>
+      <c r="F29" s="131" t="str">
+        <f>CONCATENATE(D29,".",E29,"@mailinator.com")</f>
+        <v>Med7.Devl7@mailinator.com</v>
+      </c>
+      <c r="G29" s="132" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="D30" s="130" t="s">
+        <v>431</v>
+      </c>
+      <c r="E30" s="130" t="s">
+        <v>432</v>
+      </c>
+      <c r="F30" s="131" t="str">
+        <f>CONCATENATE(D30,".",E30,"@mailinator.com")</f>
+        <v>Med8.Devl8@mailinator.com</v>
+      </c>
+      <c r="G30" s="132" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="D31" s="130" t="s">
+        <v>433</v>
+      </c>
+      <c r="E31" s="130" t="s">
+        <v>434</v>
+      </c>
+      <c r="F31" s="131" t="str">
+        <f>CONCATENATE(D31,".",E31,"@mailinator.com")</f>
+        <v>Med9.Devl9@mailinator.com</v>
+      </c>
+      <c r="G31" s="132" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="D32" s="130" t="s">
+        <v>435</v>
+      </c>
+      <c r="E32" s="130" t="s">
+        <v>436</v>
+      </c>
+      <c r="F32" s="131" t="str">
+        <f>CONCATENATE(D32,".",E32,"@mailinator.com")</f>
+        <v>Med10.Devl10@mailinator.com</v>
+      </c>
+      <c r="G32" s="132" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="49" t="s">
+        <v>257</v>
+      </c>
+      <c r="D33" s="130" t="s">
+        <v>437</v>
+      </c>
+      <c r="E33" s="130" t="s">
+        <v>438</v>
+      </c>
+      <c r="F33" s="131" t="str">
+        <f>CONCATENATE(D33,".",E33,"@mailinator.com")</f>
+        <v>Med11.Devl11@mailinator.com</v>
+      </c>
+      <c r="G33" s="132" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="50" t="s">
+        <v>255</v>
+      </c>
+      <c r="C34" s="28"/>
+      <c r="D34" s="130" t="s">
+        <v>439</v>
+      </c>
+      <c r="E34" s="130" t="s">
+        <v>440</v>
+      </c>
+      <c r="F34" s="131" t="str">
+        <f>CONCATENATE(D34,".",E34,"@mailinator.com")</f>
+        <v>Med12.Devl12@mailinator.com</v>
+      </c>
+      <c r="G34" s="132" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="50" t="s">
+        <v>256</v>
+      </c>
+      <c r="D35" s="130" t="s">
+        <v>441</v>
+      </c>
+      <c r="E35" s="130" t="s">
+        <v>442</v>
+      </c>
+      <c r="F35" s="131" t="str">
+        <f>CONCATENATE(D35,".",E35,"@mailinator.com")</f>
+        <v>Med13.Devl13@mailinator.com</v>
+      </c>
+      <c r="G35" s="132" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" s="130" t="s">
+        <v>443</v>
+      </c>
+      <c r="E36" s="130" t="s">
+        <v>444</v>
+      </c>
+      <c r="F36" s="131" t="str">
+        <f>CONCATENATE(D36,".",E36,"@mailinator.com")</f>
+        <v>Med14.Devl14@mailinator.com</v>
+      </c>
+      <c r="G36" s="132" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" s="130" t="s">
+        <v>445</v>
+      </c>
+      <c r="E37" s="130" t="s">
+        <v>446</v>
+      </c>
+      <c r="F37" s="131" t="str">
+        <f>CONCATENATE(D37,".",E37,"@mailinator.com")</f>
+        <v>Med15.Devl15@mailinator.com</v>
+      </c>
+      <c r="G37" s="132" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D38" s="130" t="s">
+        <v>447</v>
+      </c>
+      <c r="E38" s="130" t="s">
+        <v>448</v>
+      </c>
+      <c r="F38" s="131" t="str">
+        <f>CONCATENATE(D38,".",E38,"@mailinator.com")</f>
+        <v>Med16.Devl16@mailinator.com</v>
+      </c>
+      <c r="G38" s="132" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D39" s="130" t="s">
+        <v>449</v>
+      </c>
+      <c r="E39" s="130" t="s">
+        <v>450</v>
+      </c>
+      <c r="F39" s="131" t="str">
+        <f>CONCATENATE(D39,".",E39,"@mailinator.com")</f>
+        <v>Med17.Devl17@mailinator.com</v>
+      </c>
+      <c r="G39" s="132" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D40" s="130" t="s">
+        <v>451</v>
+      </c>
+      <c r="E40" s="130" t="s">
+        <v>452</v>
+      </c>
+      <c r="F40" s="131" t="str">
+        <f>CONCATENATE(D40,".",E40,"@mailinator.com")</f>
+        <v>Med18.Devl18@mailinator.com</v>
+      </c>
+      <c r="G40" s="132" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D41" s="130" t="s">
+        <v>453</v>
+      </c>
+      <c r="E41" s="130" t="s">
+        <v>454</v>
+      </c>
+      <c r="F41" s="131" t="str">
+        <f>CONCATENATE(D41,".",E41,"@mailinator.com")</f>
+        <v>Med19.Devl19@mailinator.com</v>
+      </c>
+      <c r="G41" s="132" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="13" t="s">
+        <v>385</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D42" s="130" t="s">
+        <v>455</v>
+      </c>
+      <c r="E42" s="130" t="s">
+        <v>456</v>
+      </c>
+      <c r="F42" s="131" t="str">
+        <f>CONCATENATE(D42,".",E42,"@mailinator.com")</f>
+        <v>Med20.Devl20@mailinator.com</v>
+      </c>
+      <c r="G42" s="132" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A44" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A46" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="B47" s="76" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A52" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A53" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A54" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F24" r:id="rId1"/>
+    <hyperlink ref="F23" r:id="rId2"/>
+    <hyperlink ref="F25" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <drawing r:id="rId5"/>
+  <legacyDrawing r:id="rId6"/>
+  <controls>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="31745" r:id="rId7" name="Control 1">
+          <controlPr defaultSize="0" r:id="rId8">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>40</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>457200</xdr:colOff>
+                <xdr:row>41</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="31745" r:id="rId7" name="Control 1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </controls>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$C$11:$C$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>B5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$C$3:$C$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$C$15:$C$16</xm:f>
+          </x14:formula1>
+          <xm:sqref>B10</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$C$22:$C$29</xm:f>
+          </x14:formula1>
+          <xm:sqref>B16</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$C$31:$C$32</xm:f>
+          </x14:formula1>
+          <xm:sqref>B17</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$G$3:$G$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>F4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
@@ -4058,7 +5072,7 @@
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C29" s="2" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4085,7 +5099,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B11:P49"/>
   <sheetViews>
@@ -4501,12 +5515,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E6:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:E8"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4565,7 +5579,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="O18:O20"/>
   <sheetViews>
@@ -4600,8 +5614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:T40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4628,7 +5642,7 @@
     <row r="2" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="105" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="D3" s="106"/>
       <c r="E3" s="106"/>
@@ -4648,10 +5662,10 @@
         <v>51</v>
       </c>
       <c r="S3" s="66" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="T3" s="66" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
     </row>
     <row r="4" spans="3:20" x14ac:dyDescent="0.25">
@@ -4678,16 +5692,16 @@
         <v>246</v>
       </c>
       <c r="P4" s="90" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="R4" s="126">
         <v>1</v>
       </c>
       <c r="S4" s="126" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="T4" s="127" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
     </row>
     <row r="5" spans="3:20" x14ac:dyDescent="0.25">
@@ -4709,7 +5723,7 @@
       <c r="J5" s="104"/>
       <c r="K5" s="57"/>
       <c r="M5" s="89" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="N5" s="91">
         <v>3</v>
@@ -4725,10 +5739,10 @@
         <v>2</v>
       </c>
       <c r="S5" s="126" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="T5" s="127" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="6" spans="3:20" x14ac:dyDescent="0.25">
@@ -4754,7 +5768,7 @@
       </c>
       <c r="K6" s="57"/>
       <c r="M6" s="89" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="N6" s="91">
         <v>7</v>
@@ -4770,10 +5784,10 @@
         <v>3</v>
       </c>
       <c r="S6" s="126" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="T6" s="127" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
     </row>
     <row r="7" spans="3:20" ht="26.25" x14ac:dyDescent="0.25">
@@ -4792,14 +5806,14 @@
         <v>2</v>
       </c>
       <c r="I7" s="83" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="J7" s="93" t="s">
         <v>246</v>
       </c>
       <c r="K7" s="57"/>
       <c r="M7" s="89" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="N7" s="91">
         <v>7</v>
@@ -4908,7 +5922,7 @@
         <v>7</v>
       </c>
       <c r="D12" s="86" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="E12" s="85" t="s">
         <v>231</v>
@@ -4919,7 +5933,7 @@
         <v>7</v>
       </c>
       <c r="I12" s="83" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="J12" s="93" t="s">
         <v>246</v>
@@ -4931,7 +5945,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="86" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="E13" s="85" t="s">
         <v>231</v>
@@ -4942,7 +5956,7 @@
         <v>8</v>
       </c>
       <c r="I13" s="83" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="J13" s="93" t="s">
         <v>246</v>
@@ -4954,7 +5968,7 @@
         <v>9</v>
       </c>
       <c r="D14" s="86" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E14" s="85" t="s">
         <v>231</v>
@@ -4965,7 +5979,7 @@
         <v>9</v>
       </c>
       <c r="I14" s="83" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="J14" s="93" t="s">
         <v>246</v>
@@ -4977,7 +5991,7 @@
         <v>10</v>
       </c>
       <c r="D15" s="86" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E15" s="85" t="s">
         <v>231</v>
@@ -4988,7 +6002,7 @@
         <v>10</v>
       </c>
       <c r="I15" s="83" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="J15" s="93" t="s">
         <v>246</v>
@@ -5242,7 +6256,7 @@
         <v>246</v>
       </c>
       <c r="P29" s="90" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
     </row>
     <row r="30" spans="3:16" x14ac:dyDescent="0.25">
@@ -5264,7 +6278,7 @@
       <c r="J30" s="104"/>
       <c r="K30" s="57"/>
       <c r="M30" s="89" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="N30" s="91">
         <v>8</v>
@@ -5299,7 +6313,7 @@
       </c>
       <c r="K31" s="57"/>
       <c r="M31" s="89" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="N31" s="91">
         <v>7</v>
@@ -6107,7 +7121,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B13"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6139,7 +7153,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="88" t="s">
-        <v>305</v>
+        <v>408</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
@@ -6147,7 +7161,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
@@ -6174,7 +7188,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="88" t="s">
-        <v>307</v>
+        <v>409</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
@@ -6269,8 +7283,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6298,7 +7312,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -6306,7 +7320,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -6346,7 +7360,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="87" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -7071,7 +8085,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -7079,7 +8093,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -7119,7 +8133,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="87" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -7844,7 +8858,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -7852,7 +8866,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -7892,7 +8906,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="87" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -8589,7 +9603,7 @@
   <dimension ref="A1:K106"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D24" sqref="D24:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8615,8 +9629,8 @@
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="46" t="s">
-        <v>298</v>
+      <c r="B2" s="97" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -8624,7 +9638,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>297</v>
+        <v>406</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -8663,8 +9677,8 @@
       <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="87" t="s">
-        <v>296</v>
+      <c r="B6" s="129" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -9335,7 +10349,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId1" display="doc.nov01tst@mailinator.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -9446,7 +10460,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -9454,7 +10468,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -9468,7 +10482,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>22</v>
@@ -9494,7 +10508,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="97" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -9551,18 +10565,18 @@
         <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="F12" s="46" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="F13" s="46" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -9926,133 +10940,133 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="B66" s="14"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="94" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B67" s="94"/>
     </row>
     <row r="68" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="95" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="B68" s="96" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="95" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="B69" s="96" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="95" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="B70" s="96" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="95" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="B71" s="96" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="95" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="B72" s="96" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="94" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B73" s="94"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="95" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="B74" s="96" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="95" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="B75" s="96" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="95" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="B76" s="96" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="95" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="B77" s="96" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="B78" s="14"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="95" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="B79" s="96" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="95" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B80" s="96" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="C80" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="D80" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="95" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="B81" s="96" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="95" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="B82" s="96" t="s">
         <v>46</v>
@@ -10060,55 +11074,55 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="95" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="B83" s="96" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="101" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="B84" s="102" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A85" s="101" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="B85" s="102" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="101" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="B86" s="102" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A87" s="95" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="B87" s="100" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="95" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B88" s="96" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="95" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="B89" s="11" t="s">
         <v>217</v>
@@ -10116,10 +11130,10 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="101" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="B90" s="102" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -10246,7 +11260,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="13" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="B112" s="13" t="s">
         <v>112</v>
@@ -10254,50 +11268,50 @@
     </row>
     <row r="113" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A113" s="7" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="B113" s="12" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A114" s="7" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="B114" s="12" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A115" s="7" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="B115" s="12" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A116" s="7" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="B116" s="12" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A117" s="7" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="B117" s="12" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A118" s="7" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="B118" s="12" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Removed bug from OfferMade_StepDefs File
</commit_message>
<xml_diff>
--- a/src/test/java/BaseFramework/Data/DA.xlsx
+++ b/src/test/java/BaseFramework/Data/DA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11775" windowHeight="7830" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11775" windowHeight="7830" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Result Summary" sheetId="11" r:id="rId1"/>
@@ -18,15 +18,16 @@
     <sheet name="Create Account" sheetId="1" r:id="rId4"/>
     <sheet name="Complete_Application_PGT" sheetId="2" r:id="rId5"/>
     <sheet name="RequestDeferral_Application" sheetId="7" r:id="rId6"/>
-    <sheet name="Withdraw_Application" sheetId="8" r:id="rId7"/>
-    <sheet name="Doctoral_Chem_Research_PHD" sheetId="10" r:id="rId8"/>
-    <sheet name="Management_MBA" sheetId="13" r:id="rId9"/>
-    <sheet name="ShortCourse" sheetId="16" r:id="rId10"/>
-    <sheet name="ShortCourse Data" sheetId="17" r:id="rId11"/>
-    <sheet name="Drop Down Values" sheetId="6" r:id="rId12"/>
-    <sheet name="Requirments Sheet" sheetId="3" r:id="rId13"/>
-    <sheet name="Sheet3" sheetId="9" r:id="rId14"/>
-    <sheet name="Sheet4" sheetId="14" r:id="rId15"/>
+    <sheet name="Sheet1" sheetId="18" r:id="rId7"/>
+    <sheet name="Withdraw_Application" sheetId="8" r:id="rId8"/>
+    <sheet name="Doctoral_Chem_Research_PHD" sheetId="10" r:id="rId9"/>
+    <sheet name="Management_MBA" sheetId="13" r:id="rId10"/>
+    <sheet name="ShortCourse" sheetId="16" r:id="rId11"/>
+    <sheet name="ShortCourse Data" sheetId="17" r:id="rId12"/>
+    <sheet name="Drop Down Values" sheetId="6" r:id="rId13"/>
+    <sheet name="Requirments Sheet" sheetId="3" r:id="rId14"/>
+    <sheet name="Sheet3" sheetId="9" r:id="rId15"/>
+    <sheet name="Sheet4" sheetId="14" r:id="rId16"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1727" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1738" uniqueCount="458">
   <si>
     <t>First Name</t>
   </si>
@@ -1421,6 +1422,30 @@
   <si>
     <t>Createaccount</t>
   </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Minimum 3 UG test records should be present in TEST and DEVL env</t>
+  </si>
+  <si>
+    <t>When refresh happens, all the existing data from TEST and DEVL are overwritten by PROD data</t>
+  </si>
+  <si>
+    <t>Therefore, to run our test suite on TEST and DEVL evn, we need to have UG data</t>
+  </si>
+  <si>
+    <t>Refer to file .docx, send these records to SMEs team and request them to run the sync between Banner and UCAS on both the ENV (Test/Devl) to have these records ready for testing in CRM.</t>
+  </si>
+  <si>
+    <t>MBA application fee when payment is done by Debit or Credit Card</t>
+  </si>
+  <si>
+    <t>TEST ENV - WPM should point to TEST WPM Link</t>
+  </si>
+  <si>
+    <t>DEVL ENV - WPM should point to DEVL WPM Link</t>
+  </si>
 </sst>
 </file>
 
@@ -1429,7 +1454,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1552,6 +1577,21 @@
       <u/>
       <sz val="9"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2046,7 +2086,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2267,6 +2307,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3552,6 +3607,1099 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:K140"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="89.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="99.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>384</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="96" t="str">
+        <f>CONCATENATE(B2,".",B3,"@mailinator.com")</f>
+        <v>Sam.Sonite@mailinator.com</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="D8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>366</v>
+      </c>
+      <c r="F12" s="46" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>367</v>
+      </c>
+      <c r="F13" s="46" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B17" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>259</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B18" s="50" t="s">
+        <v>258</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="D21" s="75"/>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="49" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="50" t="s">
+        <v>255</v>
+      </c>
+      <c r="C30" s="28"/>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="50" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C37" s="28"/>
+      <c r="K37" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A44" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A46" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A48" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A49" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A50" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A51" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A54" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A58" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A59" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A60" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="B60" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A61" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="B61" s="12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A62" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="B62" s="76" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B65" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="B66" s="14"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="93" t="s">
+        <v>312</v>
+      </c>
+      <c r="B67" s="93"/>
+    </row>
+    <row r="68" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="94" t="s">
+        <v>309</v>
+      </c>
+      <c r="B68" s="95" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="94" t="s">
+        <v>310</v>
+      </c>
+      <c r="B69" s="95" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="94" t="s">
+        <v>313</v>
+      </c>
+      <c r="B70" s="95" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="94" t="s">
+        <v>311</v>
+      </c>
+      <c r="B71" s="95" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="94" t="s">
+        <v>331</v>
+      </c>
+      <c r="B72" s="95" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="93" t="s">
+        <v>314</v>
+      </c>
+      <c r="B73" s="93"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="94" t="s">
+        <v>309</v>
+      </c>
+      <c r="B74" s="95" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="94" t="s">
+        <v>310</v>
+      </c>
+      <c r="B75" s="95" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="94" t="s">
+        <v>315</v>
+      </c>
+      <c r="B76" s="95" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="94" t="s">
+        <v>316</v>
+      </c>
+      <c r="B77" s="95" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="B78" s="14"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="94" t="s">
+        <v>318</v>
+      </c>
+      <c r="B79" s="95" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="94" t="s">
+        <v>319</v>
+      </c>
+      <c r="B80" s="95" t="s">
+        <v>336</v>
+      </c>
+      <c r="C80" t="s">
+        <v>339</v>
+      </c>
+      <c r="D80" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="94" t="s">
+        <v>320</v>
+      </c>
+      <c r="B81" s="95" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="94" t="s">
+        <v>321</v>
+      </c>
+      <c r="B82" s="95" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="94" t="s">
+        <v>322</v>
+      </c>
+      <c r="B83" s="95" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="100" t="s">
+        <v>341</v>
+      </c>
+      <c r="B84" s="101" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="24" x14ac:dyDescent="0.25">
+      <c r="A85" s="100" t="s">
+        <v>343</v>
+      </c>
+      <c r="B85" s="101" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="100" t="s">
+        <v>342</v>
+      </c>
+      <c r="B86" s="101" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="94" t="s">
+        <v>323</v>
+      </c>
+      <c r="B87" s="99" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="94" t="s">
+        <v>324</v>
+      </c>
+      <c r="B88" s="95" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="94" t="s">
+        <v>325</v>
+      </c>
+      <c r="B89" s="11" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="100" t="s">
+        <v>326</v>
+      </c>
+      <c r="B90" s="101" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="B91" s="14"/>
+    </row>
+    <row r="92" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A92" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B92" s="12" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A93" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="B93" s="12" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A94" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="B94" s="12" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A95" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="B95" s="77" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A96" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="B96" s="12" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A97" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="B97" s="12" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A98" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="B98" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A99" s="97"/>
+      <c r="B99" s="98"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B101" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A102" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B102" s="12" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A103" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B103" s="12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A104" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B104" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B107" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A108" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B108" s="12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A109" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B109" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="B112" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A113" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="B113" s="12" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A114" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="B114" s="12" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A115" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B115" s="12" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A116" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="B116" s="12" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A117" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="B117" s="12" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A118" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="B118" s="12" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B123" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A124" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B124" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A125" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B125" s="12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A126" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B126" s="12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A127" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B127" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A128" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B128" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A129" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B129" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A130" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B130" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B133" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A134" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B134" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A135" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B135" s="12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A136" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B136" s="12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A137" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B137" s="12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A138" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B138" s="12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A139" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B139" s="12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A140" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B140" s="12" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <controls>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="21505" r:id="rId4" name="Control 1">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>51</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>457200</xdr:colOff>
+                <xdr:row>52</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="21505" r:id="rId4" name="Control 1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </controls>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$C$11:$C$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>B5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$C$3:$C$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$C$15:$C$16</xm:f>
+          </x14:formula1>
+          <xm:sqref>B10</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$C$22:$C$29</xm:f>
+          </x14:formula1>
+          <xm:sqref>B16</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$C$31:$C$32</xm:f>
+          </x14:formula1>
+          <xm:sqref>B17</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$G$3:$G$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>F4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:F54"/>
   <sheetViews>
@@ -4061,7 +5209,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:G54"/>
@@ -4855,7 +6003,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
@@ -5071,7 +6219,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B11:P49"/>
   <sheetViews>
@@ -5487,7 +6635,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E6:F13"/>
   <sheetViews>
@@ -5551,7 +6699,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="O18:O20"/>
   <sheetViews>
@@ -7068,11 +8216,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="C23:K23"/>
     <mergeCell ref="M23:O23"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="I24:J24"/>
@@ -7082,6 +8225,11 @@
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="I5:J5"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="C23:K23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7092,7 +8240,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -7256,8 +8404,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8794,6 +9942,99 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="G13:H24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="6" width="9.140625" style="131"/>
+    <col min="7" max="7" width="2.85546875" style="131" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="74.28515625" style="131" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="131"/>
+  </cols>
+  <sheetData>
+    <row r="13" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G13" s="135" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="135" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="14" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G14" s="132">
+        <v>1</v>
+      </c>
+      <c r="H14" s="133" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="15" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G15" s="132">
+        <v>2</v>
+      </c>
+      <c r="H15" s="134" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="16" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G16" s="132">
+        <v>3</v>
+      </c>
+      <c r="H16" s="133" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="G17" s="132">
+        <v>4</v>
+      </c>
+      <c r="H17" s="133" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="21" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G21" s="135" t="s">
+        <v>51</v>
+      </c>
+      <c r="H21" s="135" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="22" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G22" s="132">
+        <v>1</v>
+      </c>
+      <c r="H22" s="133" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="23" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G23" s="132">
+        <v>2</v>
+      </c>
+      <c r="H23" s="133" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="24" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G24" s="132">
+        <v>3</v>
+      </c>
+      <c r="H24" s="133" t="s">
+        <v>457</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:K101"/>
@@ -9564,7 +10805,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:K106"/>
@@ -10390,1097 +11631,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:K140"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="89.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="99.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="46" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="46" t="s">
-        <v>384</v>
-      </c>
-      <c r="E3" s="32" t="s">
-        <v>169</v>
-      </c>
-      <c r="F3" s="32" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>363</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="96" t="str">
-        <f>CONCATENATE(B2,".",B3,"@mailinator.com")</f>
-        <v>Sam.Sonite@mailinator.com</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>294</v>
-      </c>
-      <c r="D8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="28" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" t="s">
-        <v>366</v>
-      </c>
-      <c r="F12" s="46" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E13" t="s">
-        <v>367</v>
-      </c>
-      <c r="F13" s="46" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="C16" s="28" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="B17" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="28" t="s">
-        <v>259</v>
-      </c>
-      <c r="D17" s="28" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="B18" s="50" t="s">
-        <v>258</v>
-      </c>
-      <c r="C18" s="28" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="D21" s="75"/>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B29" s="49" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B30" s="50" t="s">
-        <v>255</v>
-      </c>
-      <c r="C30" s="28"/>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B31" s="50" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C37" s="28"/>
-      <c r="K37" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B38" s="14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A39" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A40" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A43" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A46" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A47" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A48" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B48" s="12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A49" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A50" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B50" s="12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A51" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B51" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A54" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B54" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B57" s="13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A58" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B58" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A59" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B59" s="12" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A60" s="7" t="s">
-        <v>261</v>
-      </c>
-      <c r="B60" s="15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A61" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="B61" s="12" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A62" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="B62" s="76" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="B65" s="13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="14" t="s">
-        <v>308</v>
-      </c>
-      <c r="B66" s="14"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="93" t="s">
-        <v>312</v>
-      </c>
-      <c r="B67" s="93"/>
-    </row>
-    <row r="68" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="94" t="s">
-        <v>309</v>
-      </c>
-      <c r="B68" s="95" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="94" t="s">
-        <v>310</v>
-      </c>
-      <c r="B69" s="95" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="94" t="s">
-        <v>313</v>
-      </c>
-      <c r="B70" s="95" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="94" t="s">
-        <v>311</v>
-      </c>
-      <c r="B71" s="95" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="94" t="s">
-        <v>331</v>
-      </c>
-      <c r="B72" s="95" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="93" t="s">
-        <v>314</v>
-      </c>
-      <c r="B73" s="93"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="94" t="s">
-        <v>309</v>
-      </c>
-      <c r="B74" s="95" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="94" t="s">
-        <v>310</v>
-      </c>
-      <c r="B75" s="95" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="94" t="s">
-        <v>315</v>
-      </c>
-      <c r="B76" s="95" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="94" t="s">
-        <v>316</v>
-      </c>
-      <c r="B77" s="95" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="B78" s="14"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="94" t="s">
-        <v>318</v>
-      </c>
-      <c r="B79" s="95" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="94" t="s">
-        <v>319</v>
-      </c>
-      <c r="B80" s="95" t="s">
-        <v>336</v>
-      </c>
-      <c r="C80" t="s">
-        <v>339</v>
-      </c>
-      <c r="D80" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="94" t="s">
-        <v>320</v>
-      </c>
-      <c r="B81" s="95" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="94" t="s">
-        <v>321</v>
-      </c>
-      <c r="B82" s="95" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="94" t="s">
-        <v>322</v>
-      </c>
-      <c r="B83" s="95" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="100" t="s">
-        <v>341</v>
-      </c>
-      <c r="B84" s="101" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="24" x14ac:dyDescent="0.25">
-      <c r="A85" s="100" t="s">
-        <v>343</v>
-      </c>
-      <c r="B85" s="101" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="100" t="s">
-        <v>342</v>
-      </c>
-      <c r="B86" s="101" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A87" s="94" t="s">
-        <v>323</v>
-      </c>
-      <c r="B87" s="99" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="94" t="s">
-        <v>324</v>
-      </c>
-      <c r="B88" s="95" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="94" t="s">
-        <v>325</v>
-      </c>
-      <c r="B89" s="11" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="100" t="s">
-        <v>326</v>
-      </c>
-      <c r="B90" s="101" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="B91" s="14"/>
-    </row>
-    <row r="92" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A92" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="B92" s="12" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A93" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="B93" s="12" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A94" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="B94" s="12" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A95" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="B95" s="77" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A96" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="B96" s="12" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A97" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="B97" s="12" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A98" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="B98" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A99" s="97"/>
-      <c r="B99" s="98"/>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="B101" s="13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A102" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B102" s="12" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A103" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B103" s="12" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A104" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B104" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="B107" s="13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A108" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="B108" s="12" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A109" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="B109" s="12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="13" t="s">
-        <v>345</v>
-      </c>
-      <c r="B112" s="13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A113" s="7" t="s">
-        <v>358</v>
-      </c>
-      <c r="B113" s="12" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A114" s="7" t="s">
-        <v>346</v>
-      </c>
-      <c r="B114" s="12" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A115" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="B115" s="12" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A116" s="7" t="s">
-        <v>349</v>
-      </c>
-      <c r="B116" s="12" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A117" s="7" t="s">
-        <v>351</v>
-      </c>
-      <c r="B117" s="12" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A118" s="7" t="s">
-        <v>361</v>
-      </c>
-      <c r="B118" s="12" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="B123" s="13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A124" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B124" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A125" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="B125" s="12" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A126" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="B126" s="12" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A127" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="B127" s="12" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A128" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="B128" s="12" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A129" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="B129" s="12" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A130" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="B130" s="12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="B133" s="13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A134" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B134" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A135" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="B135" s="12" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A136" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="B136" s="12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A137" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="B137" s="12" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A138" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="B138" s="12" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A139" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="B139" s="12" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A140" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="B140" s="12" t="s">
-        <v>167</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-  <controls>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="21505" r:id="rId4" name="Control 1">
-          <controlPr defaultSize="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>51</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>457200</xdr:colOff>
-                <xdr:row>52</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="21505" r:id="rId4" name="Control 1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-  </controls>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'Drop Down Values'!$C$11:$C$13</xm:f>
-          </x14:formula1>
-          <xm:sqref>B5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'Drop Down Values'!$C$3:$C$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>B1</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'Drop Down Values'!$C$15:$C$16</xm:f>
-          </x14:formula1>
-          <xm:sqref>B10</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'Drop Down Values'!$C$22:$C$29</xm:f>
-          </x14:formula1>
-          <xm:sqref>B16</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'Drop Down Values'!$C$31:$C$32</xm:f>
-          </x14:formula1>
-          <xm:sqref>B17</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'Drop Down Values'!$G$3:$G$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>F4</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Changes to surefire pmo.xml and removed Testng tags
</commit_message>
<xml_diff>
--- a/src/test/java/BaseFramework/Data/DA.xlsx
+++ b/src/test/java/BaseFramework/Data/DA.xlsx
@@ -9,25 +9,26 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11775" windowHeight="7830" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11775" windowHeight="7830" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Result Summary" sheetId="11" r:id="rId1"/>
     <sheet name="Result Summary (01112018)" sheetId="15" r:id="rId2"/>
-    <sheet name="Result Summary (30102018)" sheetId="12" r:id="rId3"/>
-    <sheet name="Create Account" sheetId="1" r:id="rId4"/>
-    <sheet name="Complete_Application_PGT" sheetId="2" r:id="rId5"/>
-    <sheet name="RequestDeferral_Application" sheetId="7" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="18" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="19" r:id="rId3"/>
+    <sheet name="Result Summary (30102018)" sheetId="12" r:id="rId4"/>
+    <sheet name="Create Account" sheetId="1" r:id="rId5"/>
+    <sheet name="Complete_Application_PGT" sheetId="2" r:id="rId6"/>
+    <sheet name="RequestDeferral_Application" sheetId="7" r:id="rId7"/>
     <sheet name="Withdraw_Application" sheetId="8" r:id="rId8"/>
     <sheet name="Doctoral_Chem_Research_PHD" sheetId="10" r:id="rId9"/>
     <sheet name="Management_MBA" sheetId="13" r:id="rId10"/>
-    <sheet name="ShortCourse" sheetId="16" r:id="rId11"/>
-    <sheet name="ShortCourse Data" sheetId="17" r:id="rId12"/>
-    <sheet name="Drop Down Values" sheetId="6" r:id="rId13"/>
-    <sheet name="Requirments Sheet" sheetId="3" r:id="rId14"/>
-    <sheet name="Sheet3" sheetId="9" r:id="rId15"/>
-    <sheet name="Sheet4" sheetId="14" r:id="rId16"/>
+    <sheet name="Sheet5" sheetId="20" r:id="rId11"/>
+    <sheet name="ShortCourse" sheetId="16" r:id="rId12"/>
+    <sheet name="ShortCourse Data" sheetId="17" r:id="rId13"/>
+    <sheet name="Drop Down Values" sheetId="6" r:id="rId14"/>
+    <sheet name="Requirments Sheet" sheetId="3" r:id="rId15"/>
+    <sheet name="Sheet3" sheetId="9" r:id="rId16"/>
+    <sheet name="Sheet4" sheetId="14" r:id="rId17"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1727" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1790" uniqueCount="492">
   <si>
     <t>First Name</t>
   </si>
@@ -1270,9 +1271,6 @@
     <t>devl</t>
   </si>
   <si>
-    <t>tstnov01_123</t>
-  </si>
-  <si>
     <t>School of Public Health Taught Programmes (Occasional FT)</t>
   </si>
   <si>
@@ -1421,6 +1419,135 @@
   </si>
   <si>
     <t>abc</t>
+  </si>
+  <si>
+    <t>Issue Type</t>
+  </si>
+  <si>
+    <t>Issue key</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>Bug</t>
+  </si>
+  <si>
+    <t>DAP2-36</t>
+  </si>
+  <si>
+    <t>TEST/DEVL - MBA - Application fees payment Billing Address Country field is default to United Kingdom.</t>
+  </si>
+  <si>
+    <t>DEVL - WFE - Creating WFE account with already existing email account displays Error message</t>
+  </si>
+  <si>
+    <t>DAP2-38</t>
+  </si>
+  <si>
+    <t>TEST/DEVL - WFE  withdrawn completed application, does not update record in CRM Recruit. - Still says Submitted</t>
+  </si>
+  <si>
+    <t>DAP2-39</t>
+  </si>
+  <si>
+    <t>DEVL - WFE - Student cannot upload their English Language Certificate as supporting document as the option is completely missing</t>
+  </si>
+  <si>
+    <t>DAP2-40</t>
+  </si>
+  <si>
+    <t>TEST/DEVL - WFE  - Cancel  completed References and it  creates multiple references lines</t>
+  </si>
+  <si>
+    <t>DAP2-41</t>
+  </si>
+  <si>
+    <t>TEST/DEVL - CRM - 2. After submitting supporting documents, under &gt; My Application &gt; Status still says - Supporting Documents Required</t>
+  </si>
+  <si>
+    <t>TEST-CRM - Super user unable to switch between Registry User to Department User</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Kitchen Work top</t>
+  </si>
+  <si>
+    <t>Gas Electric Connection</t>
+  </si>
+  <si>
+    <t>Kitchen Hot Water</t>
+  </si>
+  <si>
+    <t>Kitchen</t>
+  </si>
+  <si>
+    <t>Living Room</t>
+  </si>
+  <si>
+    <t>Study Room</t>
+  </si>
+  <si>
+    <t>Painting</t>
+  </si>
+  <si>
+    <t>Underlay</t>
+  </si>
+  <si>
+    <t>Under floor heating</t>
+  </si>
+  <si>
+    <t>Laminates</t>
+  </si>
+  <si>
+    <t>Bathroom Downstairs</t>
+  </si>
+  <si>
+    <t>Tiles around window</t>
+  </si>
+  <si>
+    <t>Water Leaking Pipe</t>
+  </si>
+  <si>
+    <t>Bad Smell</t>
+  </si>
+  <si>
+    <t>Cover the base</t>
+  </si>
+  <si>
+    <t>Grout all tiles</t>
+  </si>
+  <si>
+    <t>Cover all the gaps bet shower pannels &amp; Tiles</t>
+  </si>
+  <si>
+    <t>Hang bathroom cabinate</t>
+  </si>
+  <si>
+    <t>Finish Bathroom Sealing</t>
+  </si>
+  <si>
+    <t>Room</t>
+  </si>
+  <si>
+    <t>All Doors</t>
+  </si>
+  <si>
+    <t>Paint</t>
+  </si>
+  <si>
+    <t>tstnov22_123</t>
   </si>
 </sst>
 </file>
@@ -1558,22 +1685,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="8"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="8"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1699,8 +1826,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE699"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDBDBDB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="31">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -2056,13 +2201,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2284,20 +2457,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3586,8 +3780,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:K140"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3761,9 +3955,6 @@
         <v>14</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>259</v>
-      </c>
-      <c r="D17" s="28" t="s">
         <v>254</v>
       </c>
     </row>
@@ -4675,6 +4866,117 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="N21:S25"/>
+  <sheetViews>
+    <sheetView topLeftCell="H16" workbookViewId="0">
+      <selection activeCell="Q30" sqref="Q30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="14" max="14" width="22" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="21" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="N21" s="142" t="s">
+        <v>472</v>
+      </c>
+      <c r="O21" s="142" t="s">
+        <v>474</v>
+      </c>
+      <c r="P21" s="142" t="s">
+        <v>479</v>
+      </c>
+      <c r="Q21" s="142" t="s">
+        <v>479</v>
+      </c>
+      <c r="R21" s="142" t="s">
+        <v>488</v>
+      </c>
+      <c r="S21" s="142" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="22" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="N22" s="131" t="s">
+        <v>469</v>
+      </c>
+      <c r="O22" s="131" t="s">
+        <v>476</v>
+      </c>
+      <c r="P22" s="131" t="s">
+        <v>480</v>
+      </c>
+      <c r="Q22" s="131" t="s">
+        <v>484</v>
+      </c>
+      <c r="R22" s="131" t="s">
+        <v>489</v>
+      </c>
+      <c r="S22" s="131" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="23" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="N23" s="131" t="s">
+        <v>470</v>
+      </c>
+      <c r="O23" s="131" t="s">
+        <v>477</v>
+      </c>
+      <c r="P23" s="131" t="s">
+        <v>481</v>
+      </c>
+      <c r="Q23" s="131" t="s">
+        <v>485</v>
+      </c>
+      <c r="R23" s="131" t="s">
+        <v>490</v>
+      </c>
+      <c r="S23" s="131"/>
+    </row>
+    <row r="24" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="N24" s="131" t="s">
+        <v>471</v>
+      </c>
+      <c r="O24" s="131" t="s">
+        <v>478</v>
+      </c>
+      <c r="P24" s="131" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q24" s="131" t="s">
+        <v>486</v>
+      </c>
+      <c r="R24" s="131"/>
+      <c r="S24" s="131"/>
+    </row>
+    <row r="25" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="N25" s="131"/>
+      <c r="O25" s="131" t="s">
+        <v>475</v>
+      </c>
+      <c r="P25" s="131" t="s">
+        <v>483</v>
+      </c>
+      <c r="Q25" s="131" t="s">
+        <v>487</v>
+      </c>
+      <c r="R25" s="131"/>
+      <c r="S25" s="131"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:F54"/>
@@ -5185,7 +5487,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:G54"/>
@@ -5220,7 +5522,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C2" t="s">
         <v>367</v>
@@ -5231,7 +5533,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -5288,7 +5590,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D8" t="s">
         <v>127</v>
@@ -5381,7 +5683,7 @@
         <v>126</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C18" s="28" t="s">
         <v>254</v>
@@ -5425,10 +5727,10 @@
         <v>1</v>
       </c>
       <c r="F22" s="88" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G22" s="88" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5439,16 +5741,16 @@
         <v>378</v>
       </c>
       <c r="D23" s="113" t="s">
+        <v>406</v>
+      </c>
+      <c r="E23" s="113" t="s">
         <v>407</v>
       </c>
-      <c r="E23" s="113" t="s">
+      <c r="F23" s="114" t="s">
         <v>408</v>
       </c>
-      <c r="F23" s="114" t="s">
-        <v>409</v>
-      </c>
       <c r="G23" s="115" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5459,16 +5761,16 @@
         <v>31</v>
       </c>
       <c r="D24" s="113" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E24" s="113" t="s">
+        <v>400</v>
+      </c>
+      <c r="F24" s="114" t="s">
         <v>401</v>
       </c>
-      <c r="F24" s="114" t="s">
-        <v>402</v>
-      </c>
       <c r="G24" s="115" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5479,16 +5781,16 @@
         <v>213</v>
       </c>
       <c r="D25" s="113" t="s">
+        <v>409</v>
+      </c>
+      <c r="E25" s="113" t="s">
         <v>410</v>
       </c>
-      <c r="E25" s="113" t="s">
+      <c r="F25" s="114" t="s">
         <v>411</v>
       </c>
-      <c r="F25" s="114" t="s">
-        <v>412</v>
-      </c>
       <c r="G25" s="115" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5499,17 +5801,17 @@
         <v>214</v>
       </c>
       <c r="D26" s="113" t="s">
+        <v>412</v>
+      </c>
+      <c r="E26" s="113" t="s">
         <v>413</v>
-      </c>
-      <c r="E26" s="113" t="s">
-        <v>414</v>
       </c>
       <c r="F26" s="114" t="str">
         <f t="shared" ref="F26:F42" si="0">CONCATENATE(D26,".",E26,"@mailinator.com")</f>
         <v>Med4.Devl4@mailinator.com</v>
       </c>
       <c r="G26" s="115" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5520,17 +5822,17 @@
         <v>215</v>
       </c>
       <c r="D27" s="113" t="s">
+        <v>414</v>
+      </c>
+      <c r="E27" s="113" t="s">
         <v>415</v>
-      </c>
-      <c r="E27" s="113" t="s">
-        <v>416</v>
       </c>
       <c r="F27" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med5.Devl5@mailinator.com</v>
       </c>
       <c r="G27" s="115" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5541,17 +5843,17 @@
         <v>216</v>
       </c>
       <c r="D28" s="113" t="s">
+        <v>416</v>
+      </c>
+      <c r="E28" s="113" t="s">
         <v>417</v>
-      </c>
-      <c r="E28" s="113" t="s">
-        <v>418</v>
       </c>
       <c r="F28" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med6.Devl6@mailinator.com</v>
       </c>
       <c r="G28" s="115" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5562,17 +5864,17 @@
         <v>217</v>
       </c>
       <c r="D29" s="113" t="s">
+        <v>418</v>
+      </c>
+      <c r="E29" s="113" t="s">
         <v>419</v>
-      </c>
-      <c r="E29" s="113" t="s">
-        <v>420</v>
       </c>
       <c r="F29" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med7.Devl7@mailinator.com</v>
       </c>
       <c r="G29" s="115" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5583,17 +5885,17 @@
         <v>217</v>
       </c>
       <c r="D30" s="113" t="s">
+        <v>420</v>
+      </c>
+      <c r="E30" s="113" t="s">
         <v>421</v>
-      </c>
-      <c r="E30" s="113" t="s">
-        <v>422</v>
       </c>
       <c r="F30" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med8.Devl8@mailinator.com</v>
       </c>
       <c r="G30" s="115" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5604,17 +5906,17 @@
         <v>217</v>
       </c>
       <c r="D31" s="113" t="s">
+        <v>422</v>
+      </c>
+      <c r="E31" s="113" t="s">
         <v>423</v>
-      </c>
-      <c r="E31" s="113" t="s">
-        <v>424</v>
       </c>
       <c r="F31" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med9.Devl9@mailinator.com</v>
       </c>
       <c r="G31" s="115" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5625,17 +5927,17 @@
         <v>217</v>
       </c>
       <c r="D32" s="113" t="s">
+        <v>424</v>
+      </c>
+      <c r="E32" s="113" t="s">
         <v>425</v>
-      </c>
-      <c r="E32" s="113" t="s">
-        <v>426</v>
       </c>
       <c r="F32" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med10.Devl10@mailinator.com</v>
       </c>
       <c r="G32" s="115" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5646,17 +5948,17 @@
         <v>257</v>
       </c>
       <c r="D33" s="113" t="s">
+        <v>426</v>
+      </c>
+      <c r="E33" s="113" t="s">
         <v>427</v>
-      </c>
-      <c r="E33" s="113" t="s">
-        <v>428</v>
       </c>
       <c r="F33" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med11.Devl11@mailinator.com</v>
       </c>
       <c r="G33" s="115" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5668,17 +5970,17 @@
       </c>
       <c r="C34" s="28"/>
       <c r="D34" s="113" t="s">
+        <v>428</v>
+      </c>
+      <c r="E34" s="113" t="s">
         <v>429</v>
-      </c>
-      <c r="E34" s="113" t="s">
-        <v>430</v>
       </c>
       <c r="F34" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med12.Devl12@mailinator.com</v>
       </c>
       <c r="G34" s="115" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5689,17 +5991,17 @@
         <v>256</v>
       </c>
       <c r="D35" s="113" t="s">
+        <v>430</v>
+      </c>
+      <c r="E35" s="113" t="s">
         <v>431</v>
-      </c>
-      <c r="E35" s="113" t="s">
-        <v>432</v>
       </c>
       <c r="F35" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med13.Devl13@mailinator.com</v>
       </c>
       <c r="G35" s="115" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5710,17 +6012,17 @@
         <v>52</v>
       </c>
       <c r="D36" s="113" t="s">
+        <v>432</v>
+      </c>
+      <c r="E36" s="113" t="s">
         <v>433</v>
-      </c>
-      <c r="E36" s="113" t="s">
-        <v>434</v>
       </c>
       <c r="F36" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med14.Devl14@mailinator.com</v>
       </c>
       <c r="G36" s="115" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5731,77 +6033,77 @@
         <v>51</v>
       </c>
       <c r="D37" s="113" t="s">
+        <v>434</v>
+      </c>
+      <c r="E37" s="113" t="s">
         <v>435</v>
-      </c>
-      <c r="E37" s="113" t="s">
-        <v>436</v>
       </c>
       <c r="F37" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med15.Devl15@mailinator.com</v>
       </c>
       <c r="G37" s="115" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D38" s="113" t="s">
+        <v>436</v>
+      </c>
+      <c r="E38" s="113" t="s">
         <v>437</v>
-      </c>
-      <c r="E38" s="113" t="s">
-        <v>438</v>
       </c>
       <c r="F38" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med16.Devl16@mailinator.com</v>
       </c>
       <c r="G38" s="115" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D39" s="113" t="s">
+        <v>438</v>
+      </c>
+      <c r="E39" s="113" t="s">
         <v>439</v>
-      </c>
-      <c r="E39" s="113" t="s">
-        <v>440</v>
       </c>
       <c r="F39" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med17.Devl17@mailinator.com</v>
       </c>
       <c r="G39" s="115" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D40" s="113" t="s">
+        <v>440</v>
+      </c>
+      <c r="E40" s="113" t="s">
         <v>441</v>
-      </c>
-      <c r="E40" s="113" t="s">
-        <v>442</v>
       </c>
       <c r="F40" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med18.Devl18@mailinator.com</v>
       </c>
       <c r="G40" s="115" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D41" s="113" t="s">
+        <v>442</v>
+      </c>
+      <c r="E41" s="113" t="s">
         <v>443</v>
-      </c>
-      <c r="E41" s="113" t="s">
-        <v>444</v>
       </c>
       <c r="F41" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med19.Devl19@mailinator.com</v>
       </c>
       <c r="G41" s="115" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -5812,17 +6114,17 @@
         <v>112</v>
       </c>
       <c r="D42" s="113" t="s">
+        <v>444</v>
+      </c>
+      <c r="E42" s="113" t="s">
         <v>445</v>
-      </c>
-      <c r="E42" s="113" t="s">
-        <v>446</v>
       </c>
       <c r="F42" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med20.Devl20@mailinator.com</v>
       </c>
       <c r="G42" s="115" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5979,7 +6281,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
@@ -6195,7 +6497,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B11:P49"/>
   <sheetViews>
@@ -6611,7 +6913,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E6:F13"/>
   <sheetViews>
@@ -6675,7 +6977,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="O18:O20"/>
   <sheetViews>
@@ -6710,8 +7012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:T40"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3:AB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6732,7 +7034,9 @@
     <col min="18" max="18" width="3" style="54" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="7.7109375" style="54" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="58.28515625" style="54" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="54"/>
+    <col min="21" max="27" width="9.140625" style="54"/>
+    <col min="28" max="28" width="111" style="54" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="9.140625" style="54"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -7612,6 +7916,164 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E4:I12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="7" width="9.140625" style="132"/>
+    <col min="8" max="8" width="93.85546875" style="132" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" style="132" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="132"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="133" t="s">
+        <v>449</v>
+      </c>
+      <c r="F5" s="134" t="s">
+        <v>450</v>
+      </c>
+      <c r="G5" s="134" t="s">
+        <v>451</v>
+      </c>
+      <c r="H5" s="134" t="s">
+        <v>452</v>
+      </c>
+      <c r="I5" s="134" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="6" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="138" t="s">
+        <v>453</v>
+      </c>
+      <c r="F6" s="139" t="s">
+        <v>454</v>
+      </c>
+      <c r="G6" s="139" t="s">
+        <v>187</v>
+      </c>
+      <c r="H6" s="140" t="s">
+        <v>455</v>
+      </c>
+      <c r="I6" s="139" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="7" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="138" t="s">
+        <v>453</v>
+      </c>
+      <c r="F7" s="139" t="s">
+        <v>394</v>
+      </c>
+      <c r="G7" s="139" t="s">
+        <v>187</v>
+      </c>
+      <c r="H7" s="140" t="s">
+        <v>456</v>
+      </c>
+      <c r="I7" s="139" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="8" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="138" t="s">
+        <v>453</v>
+      </c>
+      <c r="F8" s="139" t="s">
+        <v>457</v>
+      </c>
+      <c r="G8" s="139" t="s">
+        <v>187</v>
+      </c>
+      <c r="H8" s="140" t="s">
+        <v>458</v>
+      </c>
+      <c r="I8" s="139" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="9" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E9" s="138" t="s">
+        <v>453</v>
+      </c>
+      <c r="F9" s="139" t="s">
+        <v>459</v>
+      </c>
+      <c r="G9" s="139" t="s">
+        <v>187</v>
+      </c>
+      <c r="H9" s="140" t="s">
+        <v>460</v>
+      </c>
+      <c r="I9" s="139" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="10" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="138" t="s">
+        <v>453</v>
+      </c>
+      <c r="F10" s="139" t="s">
+        <v>461</v>
+      </c>
+      <c r="G10" s="139" t="s">
+        <v>187</v>
+      </c>
+      <c r="H10" s="140" t="s">
+        <v>462</v>
+      </c>
+      <c r="I10" s="139" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="11" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="138" t="s">
+        <v>453</v>
+      </c>
+      <c r="F11" s="139" t="s">
+        <v>463</v>
+      </c>
+      <c r="G11" s="139" t="s">
+        <v>187</v>
+      </c>
+      <c r="H11" s="140" t="s">
+        <v>464</v>
+      </c>
+      <c r="I11" s="139" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="12" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="135" t="s">
+        <v>453</v>
+      </c>
+      <c r="F12" s="136" t="s">
+        <v>392</v>
+      </c>
+      <c r="G12" s="136" t="s">
+        <v>187</v>
+      </c>
+      <c r="H12" s="137" t="s">
+        <v>465</v>
+      </c>
+      <c r="I12" s="141" t="s">
+        <v>468</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:P33"/>
   <sheetViews>
@@ -8212,12 +8674,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8249,7 +8711,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="87" t="s">
-        <v>399</v>
+        <v>491</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
@@ -8257,7 +8719,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
@@ -8285,7 +8747,7 @@
       </c>
       <c r="B8" s="96" t="str">
         <f>CONCATENATE(B4,".",B5,"@mailinator.com")</f>
-        <v>tstnov01_123.abc@mailinator.com</v>
+        <v>tstnov22_123.abc@mailinator.com</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
@@ -8375,13 +8837,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8409,7 +8871,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -8417,7 +8879,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -9146,7 +9608,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K101"/>
@@ -9914,59 +10376,6 @@
       </x14:dataValidations>
     </ext>
   </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="G13:H23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="6" width="9.140625" style="131"/>
-    <col min="7" max="7" width="2.85546875" style="131" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="74.28515625" style="131" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="131"/>
-  </cols>
-  <sheetData>
-    <row r="13" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G13" s="135"/>
-      <c r="H13" s="135"/>
-    </row>
-    <row r="14" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G14" s="132"/>
-      <c r="H14" s="133"/>
-    </row>
-    <row r="15" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G15" s="132"/>
-      <c r="H15" s="134"/>
-    </row>
-    <row r="16" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G16" s="132"/>
-      <c r="H16" s="133"/>
-    </row>
-    <row r="17" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G17" s="132"/>
-      <c r="H17" s="133"/>
-    </row>
-    <row r="21" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G21" s="135"/>
-      <c r="H21" s="135"/>
-    </row>
-    <row r="22" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G22" s="132"/>
-      <c r="H22" s="133"/>
-    </row>
-    <row r="23" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G23" s="132"/>
-      <c r="H23" s="133"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
End to End Jenkins Script.
</commit_message>
<xml_diff>
--- a/src/test/java/BaseFramework/Data/DA.xlsx
+++ b/src/test/java/BaseFramework/Data/DA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11775" windowHeight="7830" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11775" windowHeight="7830" firstSheet="7" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Result Summary" sheetId="11" r:id="rId1"/>
@@ -22,13 +22,12 @@
     <sheet name="Withdraw_Application" sheetId="8" r:id="rId8"/>
     <sheet name="Doctoral_Chem_Research_PHD" sheetId="10" r:id="rId9"/>
     <sheet name="Management_MBA" sheetId="13" r:id="rId10"/>
-    <sheet name="Sheet5" sheetId="20" r:id="rId11"/>
-    <sheet name="ShortCourse" sheetId="16" r:id="rId12"/>
-    <sheet name="ShortCourse Data" sheetId="17" r:id="rId13"/>
-    <sheet name="Drop Down Values" sheetId="6" r:id="rId14"/>
-    <sheet name="Requirments Sheet" sheetId="3" r:id="rId15"/>
-    <sheet name="Sheet3" sheetId="9" r:id="rId16"/>
-    <sheet name="Sheet4" sheetId="14" r:id="rId17"/>
+    <sheet name="ShortCourse" sheetId="16" r:id="rId11"/>
+    <sheet name="ShortCourse Data" sheetId="17" r:id="rId12"/>
+    <sheet name="Drop Down Values" sheetId="6" r:id="rId13"/>
+    <sheet name="Requirments Sheet" sheetId="3" r:id="rId14"/>
+    <sheet name="Sheet3" sheetId="9" r:id="rId15"/>
+    <sheet name="Sheet4" sheetId="14" r:id="rId16"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1791" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="471">
   <si>
     <t>First Name</t>
   </si>
@@ -959,19 +958,10 @@
     <t xml:space="preserve"> Student - Create Account with existing email address</t>
   </si>
   <si>
-    <t>refTst</t>
-  </si>
-  <si>
     <t>Student – Complete Application - Withdraw Application</t>
   </si>
   <si>
     <t>Student – Complete Application - Defer Application</t>
-  </si>
-  <si>
-    <t>tstenv</t>
-  </si>
-  <si>
-    <t>Defer_nov1tst</t>
   </si>
   <si>
     <t>DA - WFE</t>
@@ -990,9 +980,6 @@
 (Invalid email address message is displayed)</t>
   </si>
   <si>
-    <t>rejectatSource</t>
-  </si>
-  <si>
     <t>Total work experience to date</t>
   </si>
   <si>
@@ -1216,12 +1203,6 @@
   </si>
   <si>
     <t>Angus</t>
-  </si>
-  <si>
-    <t>Sam</t>
-  </si>
-  <si>
-    <t>Sonite</t>
   </si>
   <si>
     <t>Student – Complete Application  - MBA</t>
@@ -1265,12 +1246,6 @@
     <t>English Language Upload button missing  Defect</t>
   </si>
   <si>
-    <t>novSixteen</t>
-  </si>
-  <si>
-    <t>devl</t>
-  </si>
-  <si>
     <t>School of Public Health Taught Programmes (Occasional FT)</t>
   </si>
   <si>
@@ -1412,12 +1387,6 @@
     <t>Devl20</t>
   </si>
   <si>
-    <t>removeAssert</t>
-  </si>
-  <si>
-    <t>Createaccount</t>
-  </si>
-  <si>
     <t>Issue Type</t>
   </si>
   <si>
@@ -1478,79 +1447,43 @@
     <t>Closed</t>
   </si>
   <si>
-    <t>Kitchen Work top</t>
-  </si>
-  <si>
-    <t>Gas Electric Connection</t>
-  </si>
-  <si>
-    <t>Kitchen Hot Water</t>
-  </si>
-  <si>
-    <t>Kitchen</t>
-  </si>
-  <si>
-    <t>Living Room</t>
-  </si>
-  <si>
-    <t>Study Room</t>
-  </si>
-  <si>
-    <t>Painting</t>
-  </si>
-  <si>
-    <t>Underlay</t>
-  </si>
-  <si>
-    <t>Under floor heating</t>
-  </si>
-  <si>
-    <t>Laminates</t>
-  </si>
-  <si>
-    <t>Bathroom Downstairs</t>
-  </si>
-  <si>
-    <t>Tiles around window</t>
-  </si>
-  <si>
-    <t>Water Leaking Pipe</t>
-  </si>
-  <si>
-    <t>Bad Smell</t>
-  </si>
-  <si>
-    <t>Cover the base</t>
-  </si>
-  <si>
-    <t>Grout all tiles</t>
-  </si>
-  <si>
-    <t>Cover all the gaps bet shower pannels &amp; Tiles</t>
-  </si>
-  <si>
-    <t>Hang bathroom cabinate</t>
-  </si>
-  <si>
-    <t>Finish Bathroom Sealing</t>
-  </si>
-  <si>
-    <t>Room</t>
-  </si>
-  <si>
-    <t>All Doors</t>
-  </si>
-  <si>
-    <t>Paint</t>
-  </si>
-  <si>
     <t>Sammy.Currans@mailinator.com</t>
   </si>
   <si>
-    <t>Jaqueline</t>
-  </si>
-  <si>
-    <t>Conrad</t>
+    <t>Mariana</t>
+  </si>
+  <si>
+    <t>Burns</t>
+  </si>
+  <si>
+    <t>Lilia</t>
+  </si>
+  <si>
+    <t>Hurley</t>
+  </si>
+  <si>
+    <t>Ryder</t>
+  </si>
+  <si>
+    <t>Hester</t>
+  </si>
+  <si>
+    <t>Jean</t>
+  </si>
+  <si>
+    <t>Garcia</t>
+  </si>
+  <si>
+    <t>Yandel</t>
+  </si>
+  <si>
+    <t>Barajas</t>
+  </si>
+  <si>
+    <t>Dante</t>
+  </si>
+  <si>
+    <t>Schultz</t>
   </si>
 </sst>
 </file>
@@ -2238,7 +2171,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2460,9 +2393,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2492,9 +2422,6 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3783,8 +3710,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:K140"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24:D27"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3811,7 +3738,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>382</v>
+        <v>469</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -3819,7 +3746,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>383</v>
+        <v>470</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -3833,7 +3760,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>22</v>
@@ -3860,7 +3787,7 @@
       </c>
       <c r="B6" s="96" t="str">
         <f>CONCATENATE(B2,".",B3,"@mailinator.com")</f>
-        <v>Sam.Sonite@mailinator.com</v>
+        <v>Dante.Schultz@mailinator.com</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -3917,18 +3844,18 @@
         <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="F12" s="46" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="F13" s="46" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -4289,133 +4216,133 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B66" s="14"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="93" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B67" s="93"/>
     </row>
     <row r="68" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="94" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B68" s="95" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="94" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B69" s="95" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="94" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B70" s="95" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="94" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B71" s="95" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="94" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B72" s="95" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="93" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B73" s="93"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="94" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B74" s="95" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="94" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B75" s="95" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="94" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B76" s="95" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="94" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B77" s="95" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B78" s="14"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="94" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B79" s="95" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="94" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B80" s="95" t="s">
+        <v>331</v>
+      </c>
+      <c r="C80" t="s">
+        <v>334</v>
+      </c>
+      <c r="D80" t="s">
         <v>335</v>
-      </c>
-      <c r="C80" t="s">
-        <v>338</v>
-      </c>
-      <c r="D80" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="94" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B81" s="95" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="94" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B82" s="95" t="s">
         <v>46</v>
@@ -4423,55 +4350,55 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="94" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B83" s="95" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="100" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B84" s="101" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A85" s="100" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B85" s="101" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="100" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B86" s="101" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A87" s="94" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B87" s="99" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="94" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B88" s="95" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="94" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B89" s="11" t="s">
         <v>217</v>
@@ -4479,10 +4406,10 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="100" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B90" s="101" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -4609,7 +4536,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="13" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B112" s="13" t="s">
         <v>112</v>
@@ -4617,50 +4544,50 @@
     </row>
     <row r="113" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A113" s="7" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B113" s="12" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A114" s="7" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B114" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A115" s="7" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B115" s="12" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A116" s="7" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B116" s="12" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A117" s="7" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B117" s="12" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A118" s="7" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B118" s="12" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -4869,117 +4796,6 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="N21:S25"/>
-  <sheetViews>
-    <sheetView topLeftCell="H16" workbookViewId="0">
-      <selection activeCell="Q30" sqref="Q30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="14" max="14" width="22" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="21" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N21" s="142" t="s">
-        <v>471</v>
-      </c>
-      <c r="O21" s="142" t="s">
-        <v>473</v>
-      </c>
-      <c r="P21" s="142" t="s">
-        <v>478</v>
-      </c>
-      <c r="Q21" s="142" t="s">
-        <v>478</v>
-      </c>
-      <c r="R21" s="142" t="s">
-        <v>487</v>
-      </c>
-      <c r="S21" s="142" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="22" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N22" s="131" t="s">
-        <v>468</v>
-      </c>
-      <c r="O22" s="131" t="s">
-        <v>475</v>
-      </c>
-      <c r="P22" s="131" t="s">
-        <v>479</v>
-      </c>
-      <c r="Q22" s="131" t="s">
-        <v>483</v>
-      </c>
-      <c r="R22" s="131" t="s">
-        <v>488</v>
-      </c>
-      <c r="S22" s="131" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="23" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N23" s="131" t="s">
-        <v>469</v>
-      </c>
-      <c r="O23" s="131" t="s">
-        <v>476</v>
-      </c>
-      <c r="P23" s="131" t="s">
-        <v>480</v>
-      </c>
-      <c r="Q23" s="131" t="s">
-        <v>484</v>
-      </c>
-      <c r="R23" s="131" t="s">
-        <v>489</v>
-      </c>
-      <c r="S23" s="131"/>
-    </row>
-    <row r="24" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N24" s="131" t="s">
-        <v>470</v>
-      </c>
-      <c r="O24" s="131" t="s">
-        <v>477</v>
-      </c>
-      <c r="P24" s="131" t="s">
-        <v>481</v>
-      </c>
-      <c r="Q24" s="131" t="s">
-        <v>485</v>
-      </c>
-      <c r="R24" s="131"/>
-      <c r="S24" s="131"/>
-    </row>
-    <row r="25" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N25" s="131"/>
-      <c r="O25" s="131" t="s">
-        <v>474</v>
-      </c>
-      <c r="P25" s="131" t="s">
-        <v>482</v>
-      </c>
-      <c r="Q25" s="131" t="s">
-        <v>486</v>
-      </c>
-      <c r="R25" s="131"/>
-      <c r="S25" s="131"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:F54"/>
@@ -5012,10 +4828,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C2" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -5023,7 +4839,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -5037,7 +4853,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>22</v>
@@ -5080,7 +4896,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D8" t="s">
         <v>127</v>
@@ -5121,18 +4937,18 @@
         <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="F12" s="46" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="F13" s="46" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -5148,7 +4964,7 @@
         <v>26</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C16" s="28" t="s">
         <v>139</v>
@@ -5173,7 +4989,7 @@
         <v>126</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="C18" s="28" t="s">
         <v>254</v>
@@ -5189,34 +5005,34 @@
     </row>
     <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>371</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>372</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="B22" s="102" t="s">
         <v>373</v>
-      </c>
-      <c r="B22" s="102" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="B23" s="102" t="s">
         <v>374</v>
-      </c>
-      <c r="B23" s="102" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
@@ -5335,7 +5151,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B42" s="13" t="s">
         <v>112</v>
@@ -5490,12 +5306,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -5525,10 +5341,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="C2" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -5536,7 +5352,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -5550,7 +5366,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>22</v>
@@ -5593,7 +5409,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="D8" t="s">
         <v>127</v>
@@ -5634,18 +5450,18 @@
         <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="F12" s="46" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="F13" s="46" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -5661,7 +5477,7 @@
         <v>26</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C16" s="28" t="s">
         <v>139</v>
@@ -5686,7 +5502,7 @@
         <v>126</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="C18" s="28" t="s">
         <v>254</v>
@@ -5702,26 +5518,26 @@
     </row>
     <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>371</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>372</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="B22" s="102" t="s">
         <v>373</v>
-      </c>
-      <c r="B22" s="102" t="s">
-        <v>377</v>
       </c>
       <c r="D22" s="88" t="s">
         <v>0</v>
@@ -5730,30 +5546,30 @@
         <v>1</v>
       </c>
       <c r="F22" s="88" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="G22" s="88" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="B23" s="102" t="s">
         <v>374</v>
       </c>
-      <c r="B23" s="102" t="s">
-        <v>378</v>
-      </c>
       <c r="D23" s="113" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="E23" s="113" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="F23" s="114" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="G23" s="115" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5764,16 +5580,16 @@
         <v>31</v>
       </c>
       <c r="D24" s="113" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="E24" s="113" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="F24" s="114" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="G24" s="115" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5784,16 +5600,16 @@
         <v>213</v>
       </c>
       <c r="D25" s="113" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="E25" s="113" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="F25" s="114" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="G25" s="115" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5804,17 +5620,17 @@
         <v>214</v>
       </c>
       <c r="D26" s="113" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="E26" s="113" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="F26" s="114" t="str">
         <f t="shared" ref="F26:F42" si="0">CONCATENATE(D26,".",E26,"@mailinator.com")</f>
         <v>Med4.Devl4@mailinator.com</v>
       </c>
       <c r="G26" s="115" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5825,17 +5641,17 @@
         <v>215</v>
       </c>
       <c r="D27" s="113" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="E27" s="113" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="F27" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med5.Devl5@mailinator.com</v>
       </c>
       <c r="G27" s="115" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5846,17 +5662,17 @@
         <v>216</v>
       </c>
       <c r="D28" s="113" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="E28" s="113" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="F28" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med6.Devl6@mailinator.com</v>
       </c>
       <c r="G28" s="115" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5867,17 +5683,17 @@
         <v>217</v>
       </c>
       <c r="D29" s="113" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="E29" s="113" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="F29" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med7.Devl7@mailinator.com</v>
       </c>
       <c r="G29" s="115" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5888,17 +5704,17 @@
         <v>217</v>
       </c>
       <c r="D30" s="113" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="E30" s="113" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="F30" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med8.Devl8@mailinator.com</v>
       </c>
       <c r="G30" s="115" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5909,17 +5725,17 @@
         <v>217</v>
       </c>
       <c r="D31" s="113" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="E31" s="113" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="F31" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med9.Devl9@mailinator.com</v>
       </c>
       <c r="G31" s="115" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5930,17 +5746,17 @@
         <v>217</v>
       </c>
       <c r="D32" s="113" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="E32" s="113" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="F32" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med10.Devl10@mailinator.com</v>
       </c>
       <c r="G32" s="115" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5951,17 +5767,17 @@
         <v>257</v>
       </c>
       <c r="D33" s="113" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="E33" s="113" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="F33" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med11.Devl11@mailinator.com</v>
       </c>
       <c r="G33" s="115" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5973,17 +5789,17 @@
       </c>
       <c r="C34" s="28"/>
       <c r="D34" s="113" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="E34" s="113" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="F34" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med12.Devl12@mailinator.com</v>
       </c>
       <c r="G34" s="115" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5994,17 +5810,17 @@
         <v>256</v>
       </c>
       <c r="D35" s="113" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="E35" s="113" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="F35" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med13.Devl13@mailinator.com</v>
       </c>
       <c r="G35" s="115" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -6015,17 +5831,17 @@
         <v>52</v>
       </c>
       <c r="D36" s="113" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="E36" s="113" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="F36" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med14.Devl14@mailinator.com</v>
       </c>
       <c r="G36" s="115" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -6036,98 +5852,98 @@
         <v>51</v>
       </c>
       <c r="D37" s="113" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="E37" s="113" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="F37" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med15.Devl15@mailinator.com</v>
       </c>
       <c r="G37" s="115" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D38" s="113" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="E38" s="113" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="F38" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med16.Devl16@mailinator.com</v>
       </c>
       <c r="G38" s="115" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D39" s="113" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="E39" s="113" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="F39" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med17.Devl17@mailinator.com</v>
       </c>
       <c r="G39" s="115" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D40" s="113" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="E40" s="113" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
       <c r="F40" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med18.Devl18@mailinator.com</v>
       </c>
       <c r="G40" s="115" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D41" s="113" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="E41" s="113" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="F41" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med19.Devl19@mailinator.com</v>
       </c>
       <c r="G41" s="115" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B42" s="13" t="s">
         <v>112</v>
       </c>
       <c r="D42" s="113" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="E42" s="113" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="F42" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med20.Devl20@mailinator.com</v>
       </c>
       <c r="G42" s="115" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -6284,7 +6100,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
@@ -6473,7 +6289,7 @@
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C29" s="2" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -6500,7 +6316,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B11:P49"/>
   <sheetViews>
@@ -6916,7 +6732,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E6:F13"/>
   <sheetViews>
@@ -6980,7 +6796,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="O18:O20"/>
   <sheetViews>
@@ -7045,7 +6861,7 @@
     <row r="2" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="118" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="D3" s="119"/>
       <c r="E3" s="119"/>
@@ -7065,10 +6881,10 @@
         <v>51</v>
       </c>
       <c r="S3" s="66" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="T3" s="66" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
     <row r="4" spans="3:20" x14ac:dyDescent="0.25">
@@ -7095,16 +6911,16 @@
         <v>246</v>
       </c>
       <c r="P4" s="89" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="R4" s="110">
         <v>1</v>
       </c>
       <c r="S4" s="110" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="T4" s="111" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
     </row>
     <row r="5" spans="3:20" x14ac:dyDescent="0.25">
@@ -7126,7 +6942,7 @@
       <c r="J5" s="117"/>
       <c r="K5" s="57"/>
       <c r="M5" s="88" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="N5" s="90">
         <v>3</v>
@@ -7142,10 +6958,10 @@
         <v>2</v>
       </c>
       <c r="S5" s="110" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="T5" s="111" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
     </row>
     <row r="6" spans="3:20" x14ac:dyDescent="0.25">
@@ -7171,7 +6987,7 @@
       </c>
       <c r="K6" s="57"/>
       <c r="M6" s="88" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="N6" s="90">
         <v>7</v>
@@ -7187,10 +7003,10 @@
         <v>3</v>
       </c>
       <c r="S6" s="110" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="T6" s="111" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
     </row>
     <row r="7" spans="3:20" ht="26.25" x14ac:dyDescent="0.25">
@@ -7209,14 +7025,14 @@
         <v>2</v>
       </c>
       <c r="I7" s="83" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="J7" s="92" t="s">
         <v>246</v>
       </c>
       <c r="K7" s="57"/>
       <c r="M7" s="88" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="N7" s="90">
         <v>7</v>
@@ -7325,7 +7141,7 @@
         <v>7</v>
       </c>
       <c r="D12" s="86" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="E12" s="85" t="s">
         <v>231</v>
@@ -7336,7 +7152,7 @@
         <v>7</v>
       </c>
       <c r="I12" s="83" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="J12" s="92" t="s">
         <v>246</v>
@@ -7348,7 +7164,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="86" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="E13" s="85" t="s">
         <v>231</v>
@@ -7359,7 +7175,7 @@
         <v>8</v>
       </c>
       <c r="I13" s="83" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J13" s="92" t="s">
         <v>246</v>
@@ -7371,7 +7187,7 @@
         <v>9</v>
       </c>
       <c r="D14" s="86" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E14" s="85" t="s">
         <v>231</v>
@@ -7382,7 +7198,7 @@
         <v>9</v>
       </c>
       <c r="I14" s="83" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="J14" s="92" t="s">
         <v>246</v>
@@ -7394,7 +7210,7 @@
         <v>10</v>
       </c>
       <c r="D15" s="86" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E15" s="85" t="s">
         <v>231</v>
@@ -7405,7 +7221,7 @@
         <v>10</v>
       </c>
       <c r="I15" s="83" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J15" s="92" t="s">
         <v>246</v>
@@ -7659,7 +7475,7 @@
         <v>246</v>
       </c>
       <c r="P29" s="89" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="30" spans="3:16" x14ac:dyDescent="0.25">
@@ -7681,7 +7497,7 @@
       <c r="J30" s="117"/>
       <c r="K30" s="57"/>
       <c r="M30" s="88" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="N30" s="90">
         <v>8</v>
@@ -7716,7 +7532,7 @@
       </c>
       <c r="K31" s="57"/>
       <c r="M31" s="88" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="N31" s="90">
         <v>7</v>
@@ -7928,147 +7744,147 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="9.140625" style="132"/>
-    <col min="8" max="8" width="93.85546875" style="132" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5703125" style="132" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="132"/>
+    <col min="1" max="7" width="9.140625" style="131"/>
+    <col min="8" max="8" width="93.85546875" style="131" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" style="131" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="131"/>
   </cols>
   <sheetData>
     <row r="4" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="133" t="s">
+      <c r="E5" s="132" t="s">
+        <v>438</v>
+      </c>
+      <c r="F5" s="133" t="s">
+        <v>439</v>
+      </c>
+      <c r="G5" s="133" t="s">
+        <v>440</v>
+      </c>
+      <c r="H5" s="133" t="s">
+        <v>441</v>
+      </c>
+      <c r="I5" s="133" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="6" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="137" t="s">
+        <v>442</v>
+      </c>
+      <c r="F6" s="138" t="s">
+        <v>443</v>
+      </c>
+      <c r="G6" s="138" t="s">
+        <v>187</v>
+      </c>
+      <c r="H6" s="139" t="s">
+        <v>444</v>
+      </c>
+      <c r="I6" s="138" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="7" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="137" t="s">
+        <v>442</v>
+      </c>
+      <c r="F7" s="138" t="s">
+        <v>388</v>
+      </c>
+      <c r="G7" s="138" t="s">
+        <v>187</v>
+      </c>
+      <c r="H7" s="139" t="s">
+        <v>445</v>
+      </c>
+      <c r="I7" s="138" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="8" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="137" t="s">
+        <v>442</v>
+      </c>
+      <c r="F8" s="138" t="s">
+        <v>446</v>
+      </c>
+      <c r="G8" s="138" t="s">
+        <v>187</v>
+      </c>
+      <c r="H8" s="139" t="s">
+        <v>447</v>
+      </c>
+      <c r="I8" s="138" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="9" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E9" s="137" t="s">
+        <v>442</v>
+      </c>
+      <c r="F9" s="138" t="s">
         <v>448</v>
       </c>
-      <c r="F5" s="134" t="s">
+      <c r="G9" s="138" t="s">
+        <v>187</v>
+      </c>
+      <c r="H9" s="139" t="s">
         <v>449</v>
       </c>
-      <c r="G5" s="134" t="s">
+      <c r="I9" s="138" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="10" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="137" t="s">
+        <v>442</v>
+      </c>
+      <c r="F10" s="138" t="s">
         <v>450</v>
       </c>
-      <c r="H5" s="134" t="s">
+      <c r="G10" s="138" t="s">
+        <v>187</v>
+      </c>
+      <c r="H10" s="139" t="s">
         <v>451</v>
       </c>
-      <c r="I5" s="134" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="6" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="138" t="s">
+      <c r="I10" s="138" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="11" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="137" t="s">
+        <v>442</v>
+      </c>
+      <c r="F11" s="138" t="s">
         <v>452</v>
       </c>
-      <c r="F6" s="139" t="s">
+      <c r="G11" s="138" t="s">
+        <v>187</v>
+      </c>
+      <c r="H11" s="139" t="s">
         <v>453</v>
       </c>
-      <c r="G6" s="139" t="s">
+      <c r="I11" s="138" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="12" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="134" t="s">
+        <v>442</v>
+      </c>
+      <c r="F12" s="135" t="s">
+        <v>386</v>
+      </c>
+      <c r="G12" s="135" t="s">
         <v>187</v>
       </c>
-      <c r="H6" s="140" t="s">
+      <c r="H12" s="136" t="s">
         <v>454</v>
       </c>
-      <c r="I6" s="139" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="7" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E7" s="138" t="s">
-        <v>452</v>
-      </c>
-      <c r="F7" s="139" t="s">
-        <v>394</v>
-      </c>
-      <c r="G7" s="139" t="s">
-        <v>187</v>
-      </c>
-      <c r="H7" s="140" t="s">
-        <v>455</v>
-      </c>
-      <c r="I7" s="139" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="8" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E8" s="138" t="s">
-        <v>452</v>
-      </c>
-      <c r="F8" s="139" t="s">
-        <v>456</v>
-      </c>
-      <c r="G8" s="139" t="s">
-        <v>187</v>
-      </c>
-      <c r="H8" s="140" t="s">
+      <c r="I12" s="140" t="s">
         <v>457</v>
-      </c>
-      <c r="I8" s="139" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="9" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E9" s="138" t="s">
-        <v>452</v>
-      </c>
-      <c r="F9" s="139" t="s">
-        <v>458</v>
-      </c>
-      <c r="G9" s="139" t="s">
-        <v>187</v>
-      </c>
-      <c r="H9" s="140" t="s">
-        <v>459</v>
-      </c>
-      <c r="I9" s="139" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="10" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="138" t="s">
-        <v>452</v>
-      </c>
-      <c r="F10" s="139" t="s">
-        <v>460</v>
-      </c>
-      <c r="G10" s="139" t="s">
-        <v>187</v>
-      </c>
-      <c r="H10" s="140" t="s">
-        <v>461</v>
-      </c>
-      <c r="I10" s="139" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="11" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E11" s="138" t="s">
-        <v>452</v>
-      </c>
-      <c r="F11" s="139" t="s">
-        <v>462</v>
-      </c>
-      <c r="G11" s="139" t="s">
-        <v>187</v>
-      </c>
-      <c r="H11" s="140" t="s">
-        <v>463</v>
-      </c>
-      <c r="I11" s="139" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="12" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E12" s="135" t="s">
-        <v>452</v>
-      </c>
-      <c r="F12" s="136" t="s">
-        <v>392</v>
-      </c>
-      <c r="G12" s="136" t="s">
-        <v>187</v>
-      </c>
-      <c r="H12" s="137" t="s">
-        <v>464</v>
-      </c>
-      <c r="I12" s="141" t="s">
-        <v>467</v>
       </c>
     </row>
   </sheetData>
@@ -8681,8 +8497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8715,7 +8531,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="87" t="s">
-        <v>491</v>
+        <v>459</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -8723,7 +8539,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>492</v>
+        <v>460</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -8751,7 +8567,7 @@
       </c>
       <c r="B8" s="96" t="str">
         <f>CONCATENATE(B4,".",B5,"@mailinator.com")</f>
-        <v>Jaqueline.Conrad@mailinator.com</v>
+        <v>Mariana.Burns@mailinator.com</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -8797,7 +8613,7 @@
         <v>16</v>
       </c>
       <c r="F13" t="s">
-        <v>490</v>
+        <v>458</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -8850,7 +8666,7 @@
   <dimension ref="A1:K101"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8878,7 +8694,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>446</v>
+        <v>461</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -8886,7 +8702,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>447</v>
+        <v>462</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -8927,7 +8743,7 @@
       </c>
       <c r="B6" s="96" t="str">
         <f>CONCATENATE(B2,".",B3,"@mailinator.com")</f>
-        <v>removeAssert.Createaccount@mailinator.com</v>
+        <v>Lilia.Hurley@mailinator.com</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -9621,7 +9437,7 @@
   <dimension ref="A1:K101"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9649,7 +9465,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>300</v>
+        <v>463</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -9657,7 +9473,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>299</v>
+        <v>464</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -9698,7 +9514,7 @@
       </c>
       <c r="B6" s="96" t="str">
         <f>CONCATENATE(B2,".",B3,"@mailinator.com")</f>
-        <v>Defer_nov1tst.tstenv@mailinator.com</v>
+        <v>Ryder.Hester@mailinator.com</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -10392,7 +10208,7 @@
   <dimension ref="A1:K101"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10420,7 +10236,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>306</v>
+        <v>465</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -10428,7 +10244,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>296</v>
+        <v>466</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -10469,7 +10285,7 @@
       </c>
       <c r="B6" s="96" t="str">
         <f>CONCATENATE(B2,".",B3,"@mailinator.com")</f>
-        <v>rejectatSource.refTst@mailinator.com</v>
+        <v>Jean.Garcia@mailinator.com</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -11163,7 +10979,7 @@
   <dimension ref="A1:K106"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11190,7 +11006,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="96" t="s">
-        <v>397</v>
+        <v>467</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -11198,7 +11014,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>398</v>
+        <v>468</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -11239,7 +11055,7 @@
       </c>
       <c r="B6" s="96" t="str">
         <f>CONCATENATE(B2,".",B3,"@mailinator.com")</f>
-        <v>novSixteen.devl@mailinator.com</v>
+        <v>Yandel.Barajas@mailinator.com</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Modified Supporting documents work around.
</commit_message>
<xml_diff>
--- a/src/test/java/BaseFramework/Data/DA.xlsx
+++ b/src/test/java/BaseFramework/Data/DA.xlsx
@@ -9,15 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11775" windowHeight="7830" firstSheet="7" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11775" windowHeight="7830" firstSheet="7" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Result Summary" sheetId="11" r:id="rId1"/>
     <sheet name="Result Summary (01112018)" sheetId="15" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="19" r:id="rId3"/>
     <sheet name="Result Summary (30102018)" sheetId="12" r:id="rId4"/>
-    <sheet name="Create Account" sheetId="1" r:id="rId5"/>
-    <sheet name="Complete_Application_PGT" sheetId="2" r:id="rId6"/>
+    <sheet name="01_Create Account" sheetId="1" r:id="rId5"/>
+    <sheet name="02_PGT_Advance" sheetId="2" r:id="rId6"/>
     <sheet name="RequestDeferral_Application" sheetId="7" r:id="rId7"/>
     <sheet name="Withdraw_Application" sheetId="8" r:id="rId8"/>
     <sheet name="Doctoral_Chem_Research_PHD" sheetId="10" r:id="rId9"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1768" uniqueCount="473">
   <si>
     <t>First Name</t>
   </si>
@@ -1199,12 +1199,6 @@
     <t>English Language</t>
   </si>
   <si>
-    <t>Georgia</t>
-  </si>
-  <si>
-    <t>Angus</t>
-  </si>
-  <si>
     <t>Student – Complete Application  - MBA</t>
   </si>
   <si>
@@ -1450,40 +1444,52 @@
     <t>Sammy.Currans@mailinator.com</t>
   </si>
   <si>
-    <t>Mariana</t>
-  </si>
-  <si>
-    <t>Burns</t>
-  </si>
-  <si>
-    <t>Lilia</t>
+    <t>05/09/2009</t>
+  </si>
+  <si>
+    <t>Derick.Kirby@mailinator.com</t>
+  </si>
+  <si>
+    <t>Enzo</t>
   </si>
   <si>
     <t>Hurley</t>
   </si>
   <si>
-    <t>Ryder</t>
-  </si>
-  <si>
-    <t>Hester</t>
-  </si>
-  <si>
-    <t>Jean</t>
-  </si>
-  <si>
-    <t>Garcia</t>
-  </si>
-  <si>
-    <t>Yandel</t>
-  </si>
-  <si>
-    <t>Barajas</t>
-  </si>
-  <si>
-    <t>Dante</t>
-  </si>
-  <si>
-    <t>Schultz</t>
+    <t>Raina</t>
+  </si>
+  <si>
+    <t>Haas</t>
+  </si>
+  <si>
+    <t>Paula</t>
+  </si>
+  <si>
+    <t>Preston</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>Lutz</t>
+  </si>
+  <si>
+    <t>Anne</t>
+  </si>
+  <si>
+    <t>Grant</t>
+  </si>
+  <si>
+    <t>Adalyn</t>
+  </si>
+  <si>
+    <t>Middleton</t>
+  </si>
+  <si>
+    <t>Tia</t>
+  </si>
+  <si>
+    <t>Orr</t>
   </si>
 </sst>
 </file>
@@ -2348,6 +2354,36 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2392,36 +2428,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3130,36 +3136,36 @@
   <sheetData>
     <row r="2" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="118" t="s">
+      <c r="C3" s="128" t="s">
         <v>249</v>
       </c>
-      <c r="D3" s="119"/>
-      <c r="E3" s="119"/>
-      <c r="F3" s="119"/>
-      <c r="G3" s="119"/>
-      <c r="H3" s="119"/>
-      <c r="I3" s="119"/>
-      <c r="J3" s="119"/>
-      <c r="K3" s="120"/>
-      <c r="M3" s="121" t="s">
+      <c r="D3" s="129"/>
+      <c r="E3" s="129"/>
+      <c r="F3" s="129"/>
+      <c r="G3" s="129"/>
+      <c r="H3" s="129"/>
+      <c r="I3" s="129"/>
+      <c r="J3" s="129"/>
+      <c r="K3" s="130"/>
+      <c r="M3" s="131" t="s">
         <v>245</v>
       </c>
-      <c r="N3" s="121"/>
-      <c r="O3" s="121"/>
+      <c r="N3" s="131"/>
+      <c r="O3" s="131"/>
     </row>
     <row r="4" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C4" s="56"/>
-      <c r="D4" s="122" t="s">
+      <c r="D4" s="132" t="s">
         <v>244</v>
       </c>
-      <c r="E4" s="122"/>
+      <c r="E4" s="132"/>
       <c r="F4" s="71"/>
       <c r="G4" s="72"/>
       <c r="H4" s="73"/>
-      <c r="I4" s="122" t="s">
+      <c r="I4" s="132" t="s">
         <v>245</v>
       </c>
-      <c r="J4" s="122"/>
+      <c r="J4" s="132"/>
       <c r="K4" s="57"/>
       <c r="M4" s="66" t="s">
         <v>253</v>
@@ -3173,17 +3179,17 @@
     </row>
     <row r="5" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C5" s="56"/>
-      <c r="D5" s="117" t="s">
+      <c r="D5" s="127" t="s">
         <v>235</v>
       </c>
-      <c r="E5" s="117"/>
+      <c r="E5" s="127"/>
       <c r="F5" s="71"/>
       <c r="G5" s="72"/>
       <c r="H5" s="73"/>
-      <c r="I5" s="117" t="s">
+      <c r="I5" s="127" t="s">
         <v>235</v>
       </c>
-      <c r="J5" s="117"/>
+      <c r="J5" s="127"/>
       <c r="K5" s="57"/>
       <c r="M5" s="66" t="s">
         <v>250</v>
@@ -3312,17 +3318,17 @@
     </row>
     <row r="12" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C12" s="56"/>
-      <c r="D12" s="117" t="s">
+      <c r="D12" s="127" t="s">
         <v>243</v>
       </c>
-      <c r="E12" s="117"/>
+      <c r="E12" s="127"/>
       <c r="F12" s="71"/>
       <c r="G12" s="72"/>
       <c r="H12" s="73"/>
-      <c r="I12" s="117" t="s">
+      <c r="I12" s="127" t="s">
         <v>243</v>
       </c>
-      <c r="J12" s="117"/>
+      <c r="J12" s="127"/>
       <c r="K12" s="57"/>
     </row>
     <row r="13" spans="3:16" x14ac:dyDescent="0.25">
@@ -3473,36 +3479,36 @@
     </row>
     <row r="22" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="118" t="s">
+      <c r="C23" s="128" t="s">
         <v>248</v>
       </c>
-      <c r="D23" s="119"/>
-      <c r="E23" s="119"/>
-      <c r="F23" s="119"/>
-      <c r="G23" s="119"/>
-      <c r="H23" s="119"/>
-      <c r="I23" s="119"/>
-      <c r="J23" s="119"/>
-      <c r="K23" s="120"/>
-      <c r="M23" s="121" t="s">
+      <c r="D23" s="129"/>
+      <c r="E23" s="129"/>
+      <c r="F23" s="129"/>
+      <c r="G23" s="129"/>
+      <c r="H23" s="129"/>
+      <c r="I23" s="129"/>
+      <c r="J23" s="129"/>
+      <c r="K23" s="130"/>
+      <c r="M23" s="131" t="s">
         <v>252</v>
       </c>
-      <c r="N23" s="121"/>
-      <c r="O23" s="121"/>
+      <c r="N23" s="131"/>
+      <c r="O23" s="131"/>
     </row>
     <row r="24" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C24" s="56"/>
-      <c r="D24" s="122" t="s">
+      <c r="D24" s="132" t="s">
         <v>244</v>
       </c>
-      <c r="E24" s="122"/>
+      <c r="E24" s="132"/>
       <c r="F24" s="71"/>
       <c r="G24" s="74"/>
       <c r="H24" s="73"/>
-      <c r="I24" s="116" t="s">
+      <c r="I24" s="126" t="s">
         <v>245</v>
       </c>
-      <c r="J24" s="116"/>
+      <c r="J24" s="126"/>
       <c r="K24" s="57"/>
       <c r="M24" s="66" t="s">
         <v>253</v>
@@ -3516,17 +3522,17 @@
     </row>
     <row r="25" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C25" s="56"/>
-      <c r="D25" s="117" t="s">
+      <c r="D25" s="127" t="s">
         <v>247</v>
       </c>
-      <c r="E25" s="117"/>
+      <c r="E25" s="127"/>
       <c r="F25" s="71"/>
       <c r="G25" s="74"/>
       <c r="H25" s="73"/>
-      <c r="I25" s="117" t="s">
+      <c r="I25" s="127" t="s">
         <v>247</v>
       </c>
-      <c r="J25" s="117"/>
+      <c r="J25" s="127"/>
       <c r="K25" s="57"/>
       <c r="M25" s="66" t="s">
         <v>250</v>
@@ -3787,7 +3793,7 @@
       </c>
       <c r="B6" s="96" t="str">
         <f>CONCATENATE(B2,".",B3,"@mailinator.com")</f>
-        <v>Dante.Schultz@mailinator.com</v>
+        <v>Adalyn.Middleton@mailinator.com</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -4800,8 +4806,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4828,7 +4834,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>376</v>
+        <v>471</v>
       </c>
       <c r="C2" t="s">
         <v>363</v>
@@ -4839,7 +4845,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>377</v>
+        <v>472</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -4880,7 +4886,7 @@
       </c>
       <c r="B6" s="96" t="str">
         <f>CONCATENATE(B2,".",B3,"@mailinator.com")</f>
-        <v>Georgia.Angus@mailinator.com</v>
+        <v>Tia.Orr@mailinator.com</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -5311,8 +5317,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5341,7 +5347,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C2" t="s">
         <v>363</v>
@@ -5352,7 +5358,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -5409,7 +5415,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D8" t="s">
         <v>127</v>
@@ -5502,7 +5508,7 @@
         <v>126</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C18" s="28" t="s">
         <v>254</v>
@@ -5546,10 +5552,10 @@
         <v>1</v>
       </c>
       <c r="F22" s="88" t="s">
+        <v>393</v>
+      </c>
+      <c r="G22" s="88" t="s">
         <v>395</v>
-      </c>
-      <c r="G22" s="88" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5560,16 +5566,16 @@
         <v>374</v>
       </c>
       <c r="D23" s="113" t="s">
+        <v>396</v>
+      </c>
+      <c r="E23" s="113" t="s">
+        <v>397</v>
+      </c>
+      <c r="F23" s="114" t="s">
         <v>398</v>
       </c>
-      <c r="E23" s="113" t="s">
-        <v>399</v>
-      </c>
-      <c r="F23" s="114" t="s">
-        <v>400</v>
-      </c>
       <c r="G23" s="115" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5580,16 +5586,16 @@
         <v>31</v>
       </c>
       <c r="D24" s="113" t="s">
+        <v>392</v>
+      </c>
+      <c r="E24" s="113" t="s">
+        <v>390</v>
+      </c>
+      <c r="F24" s="114" t="s">
+        <v>391</v>
+      </c>
+      <c r="G24" s="115" t="s">
         <v>394</v>
-      </c>
-      <c r="E24" s="113" t="s">
-        <v>392</v>
-      </c>
-      <c r="F24" s="114" t="s">
-        <v>393</v>
-      </c>
-      <c r="G24" s="115" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5600,16 +5606,16 @@
         <v>213</v>
       </c>
       <c r="D25" s="113" t="s">
+        <v>399</v>
+      </c>
+      <c r="E25" s="113" t="s">
+        <v>400</v>
+      </c>
+      <c r="F25" s="114" t="s">
         <v>401</v>
       </c>
-      <c r="E25" s="113" t="s">
-        <v>402</v>
-      </c>
-      <c r="F25" s="114" t="s">
-        <v>403</v>
-      </c>
       <c r="G25" s="115" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5620,17 +5626,17 @@
         <v>214</v>
       </c>
       <c r="D26" s="113" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="E26" s="113" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F26" s="114" t="str">
         <f t="shared" ref="F26:F42" si="0">CONCATENATE(D26,".",E26,"@mailinator.com")</f>
         <v>Med4.Devl4@mailinator.com</v>
       </c>
       <c r="G26" s="115" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5641,17 +5647,17 @@
         <v>215</v>
       </c>
       <c r="D27" s="113" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="E27" s="113" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F27" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med5.Devl5@mailinator.com</v>
       </c>
       <c r="G27" s="115" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5662,17 +5668,17 @@
         <v>216</v>
       </c>
       <c r="D28" s="113" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E28" s="113" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="F28" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med6.Devl6@mailinator.com</v>
       </c>
       <c r="G28" s="115" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5683,17 +5689,17 @@
         <v>217</v>
       </c>
       <c r="D29" s="113" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E29" s="113" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="F29" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med7.Devl7@mailinator.com</v>
       </c>
       <c r="G29" s="115" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5704,17 +5710,17 @@
         <v>217</v>
       </c>
       <c r="D30" s="113" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E30" s="113" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="F30" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med8.Devl8@mailinator.com</v>
       </c>
       <c r="G30" s="115" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5725,17 +5731,17 @@
         <v>217</v>
       </c>
       <c r="D31" s="113" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E31" s="113" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="F31" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med9.Devl9@mailinator.com</v>
       </c>
       <c r="G31" s="115" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5746,17 +5752,17 @@
         <v>217</v>
       </c>
       <c r="D32" s="113" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E32" s="113" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="F32" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med10.Devl10@mailinator.com</v>
       </c>
       <c r="G32" s="115" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5767,17 +5773,17 @@
         <v>257</v>
       </c>
       <c r="D33" s="113" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E33" s="113" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F33" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med11.Devl11@mailinator.com</v>
       </c>
       <c r="G33" s="115" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5789,17 +5795,17 @@
       </c>
       <c r="C34" s="28"/>
       <c r="D34" s="113" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E34" s="113" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F34" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med12.Devl12@mailinator.com</v>
       </c>
       <c r="G34" s="115" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5810,17 +5816,17 @@
         <v>256</v>
       </c>
       <c r="D35" s="113" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E35" s="113" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F35" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med13.Devl13@mailinator.com</v>
       </c>
       <c r="G35" s="115" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5831,17 +5837,17 @@
         <v>52</v>
       </c>
       <c r="D36" s="113" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E36" s="113" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="F36" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med14.Devl14@mailinator.com</v>
       </c>
       <c r="G36" s="115" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5852,77 +5858,77 @@
         <v>51</v>
       </c>
       <c r="D37" s="113" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E37" s="113" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="F37" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med15.Devl15@mailinator.com</v>
       </c>
       <c r="G37" s="115" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D38" s="113" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E38" s="113" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="F38" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med16.Devl16@mailinator.com</v>
       </c>
       <c r="G38" s="115" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D39" s="113" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="E39" s="113" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F39" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med17.Devl17@mailinator.com</v>
       </c>
       <c r="G39" s="115" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D40" s="113" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E40" s="113" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="F40" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med18.Devl18@mailinator.com</v>
       </c>
       <c r="G40" s="115" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D41" s="113" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="E41" s="113" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F41" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med19.Devl19@mailinator.com</v>
       </c>
       <c r="G41" s="115" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -5933,17 +5939,17 @@
         <v>112</v>
       </c>
       <c r="D42" s="113" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E42" s="113" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F42" s="114" t="str">
         <f t="shared" si="0"/>
         <v>Med20.Devl20@mailinator.com</v>
       </c>
       <c r="G42" s="115" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -6116,15 +6122,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="128" t="s">
+      <c r="A1" s="138" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="128"/>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
-      <c r="E1" s="128"/>
-      <c r="F1" s="128"/>
-      <c r="G1" s="128"/>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="138"/>
+      <c r="F1" s="138"/>
+      <c r="G1" s="138"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -6342,13 +6348,13 @@
   </cols>
   <sheetData>
     <row r="11" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="F11" s="130" t="s">
+      <c r="F11" s="140" t="s">
         <v>207</v>
       </c>
-      <c r="G11" s="130"/>
-      <c r="H11" s="130"/>
-      <c r="I11" s="130"/>
-      <c r="J11" s="130"/>
+      <c r="G11" s="140"/>
+      <c r="H11" s="140"/>
+      <c r="I11" s="140"/>
+      <c r="J11" s="140"/>
     </row>
     <row r="12" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
@@ -6478,11 +6484,11 @@
       <c r="P33" s="2"/>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E34" s="129" t="s">
+      <c r="E34" s="139" t="s">
         <v>173</v>
       </c>
-      <c r="F34" s="129"/>
-      <c r="G34" s="129"/>
+      <c r="F34" s="139"/>
+      <c r="G34" s="139"/>
       <c r="I34" s="17" t="s">
         <v>179</v>
       </c>
@@ -6860,46 +6866,46 @@
   <sheetData>
     <row r="2" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="118" t="s">
-        <v>383</v>
-      </c>
-      <c r="D3" s="119"/>
-      <c r="E3" s="119"/>
-      <c r="F3" s="119"/>
-      <c r="G3" s="119"/>
-      <c r="H3" s="119"/>
-      <c r="I3" s="119"/>
-      <c r="J3" s="119"/>
-      <c r="K3" s="120"/>
-      <c r="M3" s="123" t="s">
+      <c r="C3" s="128" t="s">
+        <v>381</v>
+      </c>
+      <c r="D3" s="129"/>
+      <c r="E3" s="129"/>
+      <c r="F3" s="129"/>
+      <c r="G3" s="129"/>
+      <c r="H3" s="129"/>
+      <c r="I3" s="129"/>
+      <c r="J3" s="129"/>
+      <c r="K3" s="130"/>
+      <c r="M3" s="133" t="s">
         <v>245</v>
       </c>
-      <c r="N3" s="124"/>
-      <c r="O3" s="124"/>
-      <c r="P3" s="125"/>
+      <c r="N3" s="134"/>
+      <c r="O3" s="134"/>
+      <c r="P3" s="135"/>
       <c r="R3" s="66" t="s">
         <v>51</v>
       </c>
       <c r="S3" s="66" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="T3" s="66" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="4" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C4" s="103"/>
-      <c r="D4" s="127" t="s">
+      <c r="D4" s="137" t="s">
         <v>244</v>
       </c>
-      <c r="E4" s="127"/>
+      <c r="E4" s="137"/>
       <c r="F4" s="104"/>
       <c r="G4" s="72"/>
       <c r="H4" s="106"/>
-      <c r="I4" s="127" t="s">
+      <c r="I4" s="137" t="s">
         <v>245</v>
       </c>
-      <c r="J4" s="127"/>
+      <c r="J4" s="137"/>
       <c r="K4" s="107"/>
       <c r="M4" s="88" t="s">
         <v>253</v>
@@ -6917,29 +6923,29 @@
         <v>1</v>
       </c>
       <c r="S4" s="110" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="T4" s="111" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="5" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C5" s="108" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="117" t="s">
+      <c r="D5" s="127" t="s">
         <v>235</v>
       </c>
-      <c r="E5" s="117"/>
+      <c r="E5" s="127"/>
       <c r="F5" s="71"/>
       <c r="G5" s="72"/>
       <c r="H5" s="108" t="s">
         <v>51</v>
       </c>
-      <c r="I5" s="117" t="s">
+      <c r="I5" s="127" t="s">
         <v>235</v>
       </c>
-      <c r="J5" s="117"/>
+      <c r="J5" s="127"/>
       <c r="K5" s="57"/>
       <c r="M5" s="88" t="s">
         <v>298</v>
@@ -6958,10 +6964,10 @@
         <v>2</v>
       </c>
       <c r="S5" s="110" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="T5" s="111" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="6" spans="3:20" x14ac:dyDescent="0.25">
@@ -7003,10 +7009,10 @@
         <v>3</v>
       </c>
       <c r="S6" s="110" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="T6" s="111" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="7" spans="3:20" ht="26.25" x14ac:dyDescent="0.25">
@@ -7141,7 +7147,7 @@
         <v>7</v>
       </c>
       <c r="D12" s="86" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E12" s="85" t="s">
         <v>231</v>
@@ -7152,7 +7158,7 @@
         <v>7</v>
       </c>
       <c r="I12" s="83" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="J12" s="92" t="s">
         <v>246</v>
@@ -7164,7 +7170,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="86" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E13" s="85" t="s">
         <v>231</v>
@@ -7175,7 +7181,7 @@
         <v>8</v>
       </c>
       <c r="I13" s="83" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="J13" s="92" t="s">
         <v>246</v>
@@ -7244,19 +7250,19 @@
       <c r="C18" s="108" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="126" t="s">
+      <c r="D18" s="136" t="s">
         <v>243</v>
       </c>
-      <c r="E18" s="126"/>
+      <c r="E18" s="136"/>
       <c r="F18" s="104"/>
       <c r="G18" s="105"/>
       <c r="H18" s="108" t="s">
         <v>51</v>
       </c>
-      <c r="I18" s="126" t="s">
+      <c r="I18" s="136" t="s">
         <v>243</v>
       </c>
-      <c r="J18" s="126"/>
+      <c r="J18" s="136"/>
       <c r="K18" s="107"/>
     </row>
     <row r="19" spans="3:16" x14ac:dyDescent="0.25">
@@ -7433,37 +7439,37 @@
     </row>
     <row r="27" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="118" t="s">
+      <c r="C28" s="128" t="s">
         <v>248</v>
       </c>
-      <c r="D28" s="119"/>
-      <c r="E28" s="119"/>
-      <c r="F28" s="119"/>
-      <c r="G28" s="119"/>
-      <c r="H28" s="119"/>
-      <c r="I28" s="119"/>
-      <c r="J28" s="119"/>
-      <c r="K28" s="120"/>
-      <c r="M28" s="121" t="s">
+      <c r="D28" s="129"/>
+      <c r="E28" s="129"/>
+      <c r="F28" s="129"/>
+      <c r="G28" s="129"/>
+      <c r="H28" s="129"/>
+      <c r="I28" s="129"/>
+      <c r="J28" s="129"/>
+      <c r="K28" s="130"/>
+      <c r="M28" s="131" t="s">
         <v>252</v>
       </c>
-      <c r="N28" s="121"/>
-      <c r="O28" s="121"/>
-      <c r="P28" s="121"/>
+      <c r="N28" s="131"/>
+      <c r="O28" s="131"/>
+      <c r="P28" s="131"/>
     </row>
     <row r="29" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C29" s="56"/>
-      <c r="D29" s="122" t="s">
+      <c r="D29" s="132" t="s">
         <v>244</v>
       </c>
-      <c r="E29" s="122"/>
+      <c r="E29" s="132"/>
       <c r="F29" s="71"/>
       <c r="G29" s="74"/>
       <c r="H29" s="73"/>
-      <c r="I29" s="116" t="s">
+      <c r="I29" s="126" t="s">
         <v>245</v>
       </c>
-      <c r="J29" s="116"/>
+      <c r="J29" s="126"/>
       <c r="K29" s="57"/>
       <c r="M29" s="88" t="s">
         <v>253</v>
@@ -7482,19 +7488,19 @@
       <c r="C30" s="108" t="s">
         <v>51</v>
       </c>
-      <c r="D30" s="117" t="s">
+      <c r="D30" s="127" t="s">
         <v>247</v>
       </c>
-      <c r="E30" s="117"/>
+      <c r="E30" s="127"/>
       <c r="F30" s="71"/>
       <c r="G30" s="74"/>
       <c r="H30" s="108" t="s">
         <v>51</v>
       </c>
-      <c r="I30" s="117" t="s">
+      <c r="I30" s="127" t="s">
         <v>247</v>
       </c>
-      <c r="J30" s="117"/>
+      <c r="J30" s="127"/>
       <c r="K30" s="57"/>
       <c r="M30" s="88" t="s">
         <v>298</v>
@@ -7744,147 +7750,147 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="9.140625" style="131"/>
-    <col min="8" max="8" width="93.85546875" style="131" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5703125" style="131" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="131"/>
+    <col min="1" max="7" width="9.140625" style="116"/>
+    <col min="8" max="8" width="93.85546875" style="116" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" style="116" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="116"/>
   </cols>
   <sheetData>
     <row r="4" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="132" t="s">
+      <c r="E5" s="117" t="s">
+        <v>436</v>
+      </c>
+      <c r="F5" s="118" t="s">
+        <v>437</v>
+      </c>
+      <c r="G5" s="118" t="s">
         <v>438</v>
       </c>
-      <c r="F5" s="133" t="s">
+      <c r="H5" s="118" t="s">
         <v>439</v>
       </c>
-      <c r="G5" s="133" t="s">
+      <c r="I5" s="118" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="6" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="122" t="s">
         <v>440</v>
       </c>
-      <c r="H5" s="133" t="s">
+      <c r="F6" s="123" t="s">
         <v>441</v>
       </c>
-      <c r="I5" s="133" t="s">
+      <c r="G6" s="123" t="s">
+        <v>187</v>
+      </c>
+      <c r="H6" s="124" t="s">
+        <v>442</v>
+      </c>
+      <c r="I6" s="123" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="7" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="122" t="s">
+        <v>440</v>
+      </c>
+      <c r="F7" s="123" t="s">
+        <v>386</v>
+      </c>
+      <c r="G7" s="123" t="s">
+        <v>187</v>
+      </c>
+      <c r="H7" s="124" t="s">
+        <v>443</v>
+      </c>
+      <c r="I7" s="123" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="8" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="122" t="s">
+        <v>440</v>
+      </c>
+      <c r="F8" s="123" t="s">
+        <v>444</v>
+      </c>
+      <c r="G8" s="123" t="s">
+        <v>187</v>
+      </c>
+      <c r="H8" s="124" t="s">
+        <v>445</v>
+      </c>
+      <c r="I8" s="123" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="9" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E9" s="122" t="s">
+        <v>440</v>
+      </c>
+      <c r="F9" s="123" t="s">
+        <v>446</v>
+      </c>
+      <c r="G9" s="123" t="s">
+        <v>187</v>
+      </c>
+      <c r="H9" s="124" t="s">
+        <v>447</v>
+      </c>
+      <c r="I9" s="123" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="10" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="122" t="s">
+        <v>440</v>
+      </c>
+      <c r="F10" s="123" t="s">
+        <v>448</v>
+      </c>
+      <c r="G10" s="123" t="s">
+        <v>187</v>
+      </c>
+      <c r="H10" s="124" t="s">
+        <v>449</v>
+      </c>
+      <c r="I10" s="123" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="11" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="122" t="s">
+        <v>440</v>
+      </c>
+      <c r="F11" s="123" t="s">
+        <v>450</v>
+      </c>
+      <c r="G11" s="123" t="s">
+        <v>187</v>
+      </c>
+      <c r="H11" s="124" t="s">
+        <v>451</v>
+      </c>
+      <c r="I11" s="123" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="12" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="119" t="s">
+        <v>440</v>
+      </c>
+      <c r="F12" s="120" t="s">
+        <v>384</v>
+      </c>
+      <c r="G12" s="120" t="s">
+        <v>187</v>
+      </c>
+      <c r="H12" s="121" t="s">
+        <v>452</v>
+      </c>
+      <c r="I12" s="125" t="s">
         <v>455</v>
-      </c>
-    </row>
-    <row r="6" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="137" t="s">
-        <v>442</v>
-      </c>
-      <c r="F6" s="138" t="s">
-        <v>443</v>
-      </c>
-      <c r="G6" s="138" t="s">
-        <v>187</v>
-      </c>
-      <c r="H6" s="139" t="s">
-        <v>444</v>
-      </c>
-      <c r="I6" s="138" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="7" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E7" s="137" t="s">
-        <v>442</v>
-      </c>
-      <c r="F7" s="138" t="s">
-        <v>388</v>
-      </c>
-      <c r="G7" s="138" t="s">
-        <v>187</v>
-      </c>
-      <c r="H7" s="139" t="s">
-        <v>445</v>
-      </c>
-      <c r="I7" s="138" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="8" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E8" s="137" t="s">
-        <v>442</v>
-      </c>
-      <c r="F8" s="138" t="s">
-        <v>446</v>
-      </c>
-      <c r="G8" s="138" t="s">
-        <v>187</v>
-      </c>
-      <c r="H8" s="139" t="s">
-        <v>447</v>
-      </c>
-      <c r="I8" s="138" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="9" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E9" s="137" t="s">
-        <v>442</v>
-      </c>
-      <c r="F9" s="138" t="s">
-        <v>448</v>
-      </c>
-      <c r="G9" s="138" t="s">
-        <v>187</v>
-      </c>
-      <c r="H9" s="139" t="s">
-        <v>449</v>
-      </c>
-      <c r="I9" s="138" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="10" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="137" t="s">
-        <v>442</v>
-      </c>
-      <c r="F10" s="138" t="s">
-        <v>450</v>
-      </c>
-      <c r="G10" s="138" t="s">
-        <v>187</v>
-      </c>
-      <c r="H10" s="139" t="s">
-        <v>451</v>
-      </c>
-      <c r="I10" s="138" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="11" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E11" s="137" t="s">
-        <v>442</v>
-      </c>
-      <c r="F11" s="138" t="s">
-        <v>452</v>
-      </c>
-      <c r="G11" s="138" t="s">
-        <v>187</v>
-      </c>
-      <c r="H11" s="139" t="s">
-        <v>453</v>
-      </c>
-      <c r="I11" s="138" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="12" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E12" s="134" t="s">
-        <v>442</v>
-      </c>
-      <c r="F12" s="135" t="s">
-        <v>386</v>
-      </c>
-      <c r="G12" s="135" t="s">
-        <v>187</v>
-      </c>
-      <c r="H12" s="136" t="s">
-        <v>454</v>
-      </c>
-      <c r="I12" s="140" t="s">
-        <v>457</v>
       </c>
     </row>
   </sheetData>
@@ -7918,36 +7924,36 @@
   <sheetData>
     <row r="2" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="118" t="s">
+      <c r="C3" s="128" t="s">
         <v>292</v>
       </c>
-      <c r="D3" s="119"/>
-      <c r="E3" s="119"/>
-      <c r="F3" s="119"/>
-      <c r="G3" s="119"/>
-      <c r="H3" s="119"/>
-      <c r="I3" s="119"/>
-      <c r="J3" s="119"/>
-      <c r="K3" s="120"/>
-      <c r="M3" s="121" t="s">
+      <c r="D3" s="129"/>
+      <c r="E3" s="129"/>
+      <c r="F3" s="129"/>
+      <c r="G3" s="129"/>
+      <c r="H3" s="129"/>
+      <c r="I3" s="129"/>
+      <c r="J3" s="129"/>
+      <c r="K3" s="130"/>
+      <c r="M3" s="131" t="s">
         <v>245</v>
       </c>
-      <c r="N3" s="121"/>
-      <c r="O3" s="121"/>
+      <c r="N3" s="131"/>
+      <c r="O3" s="131"/>
     </row>
     <row r="4" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C4" s="56"/>
-      <c r="D4" s="122" t="s">
+      <c r="D4" s="132" t="s">
         <v>244</v>
       </c>
-      <c r="E4" s="122"/>
+      <c r="E4" s="132"/>
       <c r="F4" s="71"/>
       <c r="G4" s="72"/>
       <c r="H4" s="73"/>
-      <c r="I4" s="122" t="s">
+      <c r="I4" s="132" t="s">
         <v>245</v>
       </c>
-      <c r="J4" s="122"/>
+      <c r="J4" s="132"/>
       <c r="K4" s="57"/>
       <c r="M4" s="66" t="s">
         <v>253</v>
@@ -7961,17 +7967,17 @@
     </row>
     <row r="5" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C5" s="56"/>
-      <c r="D5" s="117" t="s">
+      <c r="D5" s="127" t="s">
         <v>235</v>
       </c>
-      <c r="E5" s="117"/>
+      <c r="E5" s="127"/>
       <c r="F5" s="71"/>
       <c r="G5" s="72"/>
       <c r="H5" s="73"/>
-      <c r="I5" s="117" t="s">
+      <c r="I5" s="127" t="s">
         <v>235</v>
       </c>
-      <c r="J5" s="117"/>
+      <c r="J5" s="127"/>
       <c r="K5" s="57"/>
       <c r="M5" s="66" t="s">
         <v>293</v>
@@ -8100,17 +8106,17 @@
     </row>
     <row r="12" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C12" s="56"/>
-      <c r="D12" s="117" t="s">
+      <c r="D12" s="127" t="s">
         <v>243</v>
       </c>
-      <c r="E12" s="117"/>
+      <c r="E12" s="127"/>
       <c r="F12" s="71"/>
       <c r="G12" s="72"/>
       <c r="H12" s="73"/>
-      <c r="I12" s="117" t="s">
+      <c r="I12" s="127" t="s">
         <v>243</v>
       </c>
-      <c r="J12" s="117"/>
+      <c r="J12" s="127"/>
       <c r="K12" s="57"/>
     </row>
     <row r="13" spans="3:16" x14ac:dyDescent="0.25">
@@ -8261,36 +8267,36 @@
     </row>
     <row r="22" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="118" t="s">
+      <c r="C23" s="128" t="s">
         <v>248</v>
       </c>
-      <c r="D23" s="119"/>
-      <c r="E23" s="119"/>
-      <c r="F23" s="119"/>
-      <c r="G23" s="119"/>
-      <c r="H23" s="119"/>
-      <c r="I23" s="119"/>
-      <c r="J23" s="119"/>
-      <c r="K23" s="120"/>
-      <c r="M23" s="121" t="s">
+      <c r="D23" s="129"/>
+      <c r="E23" s="129"/>
+      <c r="F23" s="129"/>
+      <c r="G23" s="129"/>
+      <c r="H23" s="129"/>
+      <c r="I23" s="129"/>
+      <c r="J23" s="129"/>
+      <c r="K23" s="130"/>
+      <c r="M23" s="131" t="s">
         <v>252</v>
       </c>
-      <c r="N23" s="121"/>
-      <c r="O23" s="121"/>
+      <c r="N23" s="131"/>
+      <c r="O23" s="131"/>
     </row>
     <row r="24" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C24" s="56"/>
-      <c r="D24" s="122" t="s">
+      <c r="D24" s="132" t="s">
         <v>244</v>
       </c>
-      <c r="E24" s="122"/>
+      <c r="E24" s="132"/>
       <c r="F24" s="71"/>
       <c r="G24" s="74"/>
       <c r="H24" s="73"/>
-      <c r="I24" s="116" t="s">
+      <c r="I24" s="126" t="s">
         <v>245</v>
       </c>
-      <c r="J24" s="116"/>
+      <c r="J24" s="126"/>
       <c r="K24" s="57"/>
       <c r="M24" s="66" t="s">
         <v>253</v>
@@ -8304,17 +8310,17 @@
     </row>
     <row r="25" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C25" s="56"/>
-      <c r="D25" s="117" t="s">
+      <c r="D25" s="127" t="s">
         <v>247</v>
       </c>
-      <c r="E25" s="117"/>
+      <c r="E25" s="127"/>
       <c r="F25" s="71"/>
       <c r="G25" s="74"/>
       <c r="H25" s="73"/>
-      <c r="I25" s="117" t="s">
+      <c r="I25" s="127" t="s">
         <v>247</v>
       </c>
-      <c r="J25" s="117"/>
+      <c r="J25" s="127"/>
       <c r="K25" s="57"/>
       <c r="M25" s="66" t="s">
         <v>250</v>
@@ -8473,6 +8479,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="C23:K23"/>
     <mergeCell ref="M23:O23"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="I24:J24"/>
@@ -8482,11 +8493,6 @@
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="I5:J5"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="C23:K23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8498,7 +8504,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8531,7 +8537,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="87" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -8539,7 +8545,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -8567,7 +8573,7 @@
       </c>
       <c r="B8" s="96" t="str">
         <f>CONCATENATE(B4,".",B5,"@mailinator.com")</f>
-        <v>Mariana.Burns@mailinator.com</v>
+        <v>Raina.Haas@mailinator.com</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -8613,7 +8619,7 @@
         <v>16</v>
       </c>
       <c r="F13" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -8678,7 +8684,7 @@
     <col min="5" max="6" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
@@ -8689,20 +8695,20 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -8711,12 +8717,12 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>18</v>
+      <c r="B4" s="15" t="s">
+        <v>457</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>22</v>
@@ -8725,7 +8731,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
@@ -8737,16 +8743,16 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="96" t="str">
         <f>CONCATENATE(B2,".",B3,"@mailinator.com")</f>
-        <v>Lilia.Hurley@mailinator.com</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+        <v>Enzo.Hurley@mailinator.com</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>5</v>
       </c>
@@ -8754,7 +8760,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>6</v>
       </c>
@@ -8762,7 +8768,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>7</v>
       </c>
@@ -8770,7 +8776,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>8</v>
       </c>
@@ -8781,7 +8787,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>9</v>
       </c>
@@ -8789,7 +8795,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
@@ -8797,7 +8803,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>25</v>
       </c>
@@ -8805,7 +8816,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>26</v>
       </c>
@@ -9357,13 +9368,14 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="2049" r:id="rId3" name="Control 1">
-          <controlPr defaultSize="0" r:id="rId4">
+        <control shapeId="2049" r:id="rId4" name="Control 1">
+          <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -9382,7 +9394,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="2049" r:id="rId3" name="Control 1"/>
+        <control shapeId="2049" r:id="rId4" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -9514,7 +9526,7 @@
       </c>
       <c r="B6" s="96" t="str">
         <f>CONCATENATE(B2,".",B3,"@mailinator.com")</f>
-        <v>Ryder.Hester@mailinator.com</v>
+        <v>Paula.Preston@mailinator.com</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -10285,7 +10297,7 @@
       </c>
       <c r="B6" s="96" t="str">
         <f>CONCATENATE(B2,".",B3,"@mailinator.com")</f>
-        <v>Jean.Garcia@mailinator.com</v>
+        <v>Case.Lutz@mailinator.com</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -11055,7 +11067,7 @@
       </c>
       <c r="B6" s="96" t="str">
         <f>CONCATENATE(B2,".",B3,"@mailinator.com")</f>
-        <v>Yandel.Barajas@mailinator.com</v>
+        <v>Anne.Grant@mailinator.com</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
PGT - Offer Made
</commit_message>
<xml_diff>
--- a/src/test/java/BaseFramework/Data/DA.xlsx
+++ b/src/test/java/BaseFramework/Data/DA.xlsx
@@ -9,22 +9,23 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11775" windowHeight="7830"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11775" windowHeight="7830" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="01_Create Account" sheetId="1" r:id="rId1"/>
-    <sheet name="02_PGT_Advance" sheetId="2" r:id="rId2"/>
-    <sheet name="03_Doctoral_Chem_Research_PHD" sheetId="10" r:id="rId3"/>
-    <sheet name="04_Management_MBA" sheetId="13" r:id="rId4"/>
-    <sheet name="05_ShortCourse" sheetId="16" r:id="rId5"/>
-    <sheet name="06_Withdraw_Application" sheetId="8" r:id="rId6"/>
-    <sheet name="07_RequestDeferral_Application" sheetId="7" r:id="rId7"/>
-    <sheet name="ShortCourse Data" sheetId="17" r:id="rId8"/>
-    <sheet name="Drop Down Values" sheetId="6" r:id="rId9"/>
-    <sheet name="Requirments Sheet" sheetId="3" r:id="rId10"/>
-    <sheet name="Result Summary" sheetId="11" r:id="rId11"/>
-    <sheet name="Result Summary (01112018)" sheetId="15" r:id="rId12"/>
-    <sheet name="Result Summary (30102018)" sheetId="12" r:id="rId13"/>
+    <sheet name="Recruit_Users" sheetId="18" r:id="rId1"/>
+    <sheet name="01_Create Account" sheetId="1" r:id="rId2"/>
+    <sheet name="02_PGT_Advance" sheetId="2" r:id="rId3"/>
+    <sheet name="03_Doctoral_Chem_Research_PHD" sheetId="10" r:id="rId4"/>
+    <sheet name="04_Management_MBA" sheetId="13" r:id="rId5"/>
+    <sheet name="05_ShortCourse" sheetId="16" r:id="rId6"/>
+    <sheet name="06_Withdraw_Application" sheetId="8" r:id="rId7"/>
+    <sheet name="07_RequestDeferral_Application" sheetId="7" r:id="rId8"/>
+    <sheet name="ShortCourse Data" sheetId="17" r:id="rId9"/>
+    <sheet name="Drop Down Values" sheetId="6" r:id="rId10"/>
+    <sheet name="Requirments Sheet" sheetId="3" r:id="rId11"/>
+    <sheet name="Result Summary" sheetId="11" r:id="rId12"/>
+    <sheet name="Result Summary (01112018)" sheetId="15" r:id="rId13"/>
+    <sheet name="Result Summary (30102018)" sheetId="12" r:id="rId14"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1718" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1736" uniqueCount="465">
   <si>
     <t>First Name</t>
   </si>
@@ -1375,16 +1376,70 @@
     <t>Randall.Monroe@mailinator.com</t>
   </si>
   <si>
-    <t>Nayeli</t>
-  </si>
-  <si>
-    <t>Marshall</t>
-  </si>
-  <si>
     <t>Quinten</t>
   </si>
   <si>
     <t>Dorsey</t>
+  </si>
+  <si>
+    <t>crmrec2@ic.ac.uk</t>
+  </si>
+  <si>
+    <t>crmrec2</t>
+  </si>
+  <si>
+    <t>TstBanner2</t>
+  </si>
+  <si>
+    <t>crmrec1@ic.ac.uk</t>
+  </si>
+  <si>
+    <t>crmrec1</t>
+  </si>
+  <si>
+    <t>TstBanner1</t>
+  </si>
+  <si>
+    <t>crmrec3@ic.ac.uk</t>
+  </si>
+  <si>
+    <t>crmrec4@ic.ac.uk</t>
+  </si>
+  <si>
+    <t>crmrec3</t>
+  </si>
+  <si>
+    <t>crmrec4</t>
+  </si>
+  <si>
+    <t>TstBanner3</t>
+  </si>
+  <si>
+    <t>TstBanner4</t>
+  </si>
+  <si>
+    <t>0,0</t>
+  </si>
+  <si>
+    <t>0,1</t>
+  </si>
+  <si>
+    <t>0,2</t>
+  </si>
+  <si>
+    <t>Email(1,0)</t>
+  </si>
+  <si>
+    <t>User Name (1,1)</t>
+  </si>
+  <si>
+    <t>Password (2,2)</t>
+  </si>
+  <si>
+    <t>Kendall</t>
+  </si>
+  <si>
+    <t>Vasquez</t>
   </si>
 </sst>
 </file>
@@ -1394,7 +1449,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1507,6 +1562,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF008000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="22">
@@ -1998,7 +2060,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2172,6 +2234,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2208,14 +2279,8 @@
     <xf numFmtId="0" fontId="11" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2902,172 +2967,308 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="46.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>457</v>
+      </c>
+      <c r="B1" t="s">
+        <v>458</v>
+      </c>
+      <c r="C1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>171</v>
-      </c>
-      <c r="B2" s="33"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="35" t="s">
-        <v>132</v>
-      </c>
-      <c r="C3" s="46" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="86" t="s">
+        <v>460</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>461</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="130" t="s">
+        <v>448</v>
+      </c>
+      <c r="B3" s="130" t="s">
+        <v>449</v>
+      </c>
+      <c r="C3" s="130" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="130" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="45" t="s">
+      <c r="B4" s="130" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="46" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="95" t="str">
-        <f>CONCATENATE(B4,".",B5,"@mailinator.com")</f>
-        <v>Quinten.Dorsey@mailinator.com</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="30" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="46" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="37" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="B15" s="22"/>
+      <c r="C4" s="130" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="130" t="s">
+        <v>451</v>
+      </c>
+      <c r="B5" s="130" t="s">
+        <v>453</v>
+      </c>
+      <c r="C5" s="130" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="130" t="s">
+        <v>452</v>
+      </c>
+      <c r="B6" s="130" t="s">
+        <v>454</v>
+      </c>
+      <c r="C6" s="130" t="s">
+        <v>456</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'Drop Down Values'!$C$15:$C$16</xm:f>
-          </x14:formula1>
-          <xm:sqref>B12</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'Drop Down Values'!$C$3:$C$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>B3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'Drop Down Values'!$C$11:$C$13</xm:f>
-          </x14:formula1>
-          <xm:sqref>B7</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="48.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="115" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="24"/>
+      <c r="C4" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="24"/>
+      <c r="C5" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" s="21"/>
+      <c r="G5" s="26" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="24"/>
+      <c r="C6" s="25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="24"/>
+      <c r="C7" s="25" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="24"/>
+      <c r="C8" s="25" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="21"/>
+      <c r="C9" s="26" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B11" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="24"/>
+      <c r="C12" s="25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="21"/>
+      <c r="C13" s="26" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B15" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="21"/>
+      <c r="C16" s="22"/>
+    </row>
+    <row r="17" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="2:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B18" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="24"/>
+      <c r="C19" s="25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="21"/>
+      <c r="C20" s="26" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="2:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B22" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="24"/>
+      <c r="C23" s="25" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="24"/>
+      <c r="C24" s="25" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="24"/>
+      <c r="C25" s="25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="24"/>
+      <c r="C26" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="21"/>
+      <c r="C27" s="26" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="50"/>
+      <c r="C28" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="2:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B31" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="21"/>
+      <c r="C32" s="26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B11:P49"/>
   <sheetViews>
@@ -3093,13 +3294,13 @@
   </cols>
   <sheetData>
     <row r="11" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="F11" s="129" t="s">
+      <c r="F11" s="117" t="s">
         <v>201</v>
       </c>
-      <c r="G11" s="129"/>
-      <c r="H11" s="129"/>
-      <c r="I11" s="129"/>
-      <c r="J11" s="129"/>
+      <c r="G11" s="117"/>
+      <c r="H11" s="117"/>
+      <c r="I11" s="117"/>
+      <c r="J11" s="117"/>
     </row>
     <row r="12" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
@@ -3229,11 +3430,11 @@
       <c r="P33" s="2"/>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E34" s="128" t="s">
+      <c r="E34" s="116" t="s">
         <v>173</v>
       </c>
-      <c r="F34" s="128"/>
-      <c r="G34" s="128"/>
+      <c r="F34" s="116"/>
+      <c r="G34" s="116"/>
       <c r="I34" s="17" t="s">
         <v>179</v>
       </c>
@@ -3483,7 +3684,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:P33"/>
   <sheetViews>
@@ -3507,36 +3708,36 @@
   <sheetData>
     <row r="2" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="117" t="s">
+      <c r="C3" s="120" t="s">
         <v>242</v>
       </c>
-      <c r="D3" s="118"/>
-      <c r="E3" s="118"/>
-      <c r="F3" s="118"/>
-      <c r="G3" s="118"/>
-      <c r="H3" s="118"/>
-      <c r="I3" s="118"/>
-      <c r="J3" s="118"/>
-      <c r="K3" s="119"/>
-      <c r="M3" s="120" t="s">
+      <c r="D3" s="121"/>
+      <c r="E3" s="121"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="121"/>
+      <c r="I3" s="121"/>
+      <c r="J3" s="121"/>
+      <c r="K3" s="122"/>
+      <c r="M3" s="123" t="s">
         <v>238</v>
       </c>
-      <c r="N3" s="120"/>
-      <c r="O3" s="120"/>
+      <c r="N3" s="123"/>
+      <c r="O3" s="123"/>
     </row>
     <row r="4" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C4" s="55"/>
-      <c r="D4" s="121" t="s">
+      <c r="D4" s="124" t="s">
         <v>237</v>
       </c>
-      <c r="E4" s="121"/>
+      <c r="E4" s="124"/>
       <c r="F4" s="70"/>
       <c r="G4" s="71"/>
       <c r="H4" s="72"/>
-      <c r="I4" s="121" t="s">
+      <c r="I4" s="124" t="s">
         <v>238</v>
       </c>
-      <c r="J4" s="121"/>
+      <c r="J4" s="124"/>
       <c r="K4" s="56"/>
       <c r="M4" s="65" t="s">
         <v>246</v>
@@ -3550,17 +3751,17 @@
     </row>
     <row r="5" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C5" s="55"/>
-      <c r="D5" s="116" t="s">
+      <c r="D5" s="119" t="s">
         <v>228</v>
       </c>
-      <c r="E5" s="116"/>
+      <c r="E5" s="119"/>
       <c r="F5" s="70"/>
       <c r="G5" s="71"/>
       <c r="H5" s="72"/>
-      <c r="I5" s="116" t="s">
+      <c r="I5" s="119" t="s">
         <v>228</v>
       </c>
-      <c r="J5" s="116"/>
+      <c r="J5" s="119"/>
       <c r="K5" s="56"/>
       <c r="M5" s="65" t="s">
         <v>243</v>
@@ -3689,17 +3890,17 @@
     </row>
     <row r="12" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C12" s="55"/>
-      <c r="D12" s="116" t="s">
+      <c r="D12" s="119" t="s">
         <v>236</v>
       </c>
-      <c r="E12" s="116"/>
+      <c r="E12" s="119"/>
       <c r="F12" s="70"/>
       <c r="G12" s="71"/>
       <c r="H12" s="72"/>
-      <c r="I12" s="116" t="s">
+      <c r="I12" s="119" t="s">
         <v>236</v>
       </c>
-      <c r="J12" s="116"/>
+      <c r="J12" s="119"/>
       <c r="K12" s="56"/>
     </row>
     <row r="13" spans="3:16" x14ac:dyDescent="0.25">
@@ -3850,36 +4051,36 @@
     </row>
     <row r="22" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="117" t="s">
+      <c r="C23" s="120" t="s">
         <v>241</v>
       </c>
-      <c r="D23" s="118"/>
-      <c r="E23" s="118"/>
-      <c r="F23" s="118"/>
-      <c r="G23" s="118"/>
-      <c r="H23" s="118"/>
-      <c r="I23" s="118"/>
-      <c r="J23" s="118"/>
-      <c r="K23" s="119"/>
-      <c r="M23" s="120" t="s">
+      <c r="D23" s="121"/>
+      <c r="E23" s="121"/>
+      <c r="F23" s="121"/>
+      <c r="G23" s="121"/>
+      <c r="H23" s="121"/>
+      <c r="I23" s="121"/>
+      <c r="J23" s="121"/>
+      <c r="K23" s="122"/>
+      <c r="M23" s="123" t="s">
         <v>245</v>
       </c>
-      <c r="N23" s="120"/>
-      <c r="O23" s="120"/>
+      <c r="N23" s="123"/>
+      <c r="O23" s="123"/>
     </row>
     <row r="24" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C24" s="55"/>
-      <c r="D24" s="121" t="s">
+      <c r="D24" s="124" t="s">
         <v>237</v>
       </c>
-      <c r="E24" s="121"/>
+      <c r="E24" s="124"/>
       <c r="F24" s="70"/>
       <c r="G24" s="73"/>
       <c r="H24" s="72"/>
-      <c r="I24" s="115" t="s">
+      <c r="I24" s="118" t="s">
         <v>238</v>
       </c>
-      <c r="J24" s="115"/>
+      <c r="J24" s="118"/>
       <c r="K24" s="56"/>
       <c r="M24" s="65" t="s">
         <v>246</v>
@@ -3893,17 +4094,17 @@
     </row>
     <row r="25" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C25" s="55"/>
-      <c r="D25" s="116" t="s">
+      <c r="D25" s="119" t="s">
         <v>240</v>
       </c>
-      <c r="E25" s="116"/>
+      <c r="E25" s="119"/>
       <c r="F25" s="70"/>
       <c r="G25" s="73"/>
       <c r="H25" s="72"/>
-      <c r="I25" s="116" t="s">
+      <c r="I25" s="119" t="s">
         <v>240</v>
       </c>
-      <c r="J25" s="116"/>
+      <c r="J25" s="119"/>
       <c r="K25" s="56"/>
       <c r="M25" s="65" t="s">
         <v>243</v>
@@ -4082,7 +4283,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:T40"/>
   <sheetViews>
@@ -4115,23 +4316,23 @@
   <sheetData>
     <row r="2" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="117" t="s">
+      <c r="C3" s="120" t="s">
         <v>374</v>
       </c>
-      <c r="D3" s="118"/>
-      <c r="E3" s="118"/>
-      <c r="F3" s="118"/>
-      <c r="G3" s="118"/>
-      <c r="H3" s="118"/>
-      <c r="I3" s="118"/>
-      <c r="J3" s="118"/>
-      <c r="K3" s="119"/>
-      <c r="M3" s="122" t="s">
+      <c r="D3" s="121"/>
+      <c r="E3" s="121"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="121"/>
+      <c r="I3" s="121"/>
+      <c r="J3" s="121"/>
+      <c r="K3" s="122"/>
+      <c r="M3" s="125" t="s">
         <v>238</v>
       </c>
-      <c r="N3" s="123"/>
-      <c r="O3" s="123"/>
-      <c r="P3" s="124"/>
+      <c r="N3" s="126"/>
+      <c r="O3" s="126"/>
+      <c r="P3" s="127"/>
       <c r="R3" s="65" t="s">
         <v>51</v>
       </c>
@@ -4144,17 +4345,17 @@
     </row>
     <row r="4" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C4" s="102"/>
-      <c r="D4" s="126" t="s">
+      <c r="D4" s="129" t="s">
         <v>237</v>
       </c>
-      <c r="E4" s="126"/>
+      <c r="E4" s="129"/>
       <c r="F4" s="103"/>
       <c r="G4" s="71"/>
       <c r="H4" s="105"/>
-      <c r="I4" s="126" t="s">
+      <c r="I4" s="129" t="s">
         <v>238</v>
       </c>
-      <c r="J4" s="126"/>
+      <c r="J4" s="129"/>
       <c r="K4" s="106"/>
       <c r="M4" s="87" t="s">
         <v>246</v>
@@ -4182,19 +4383,19 @@
       <c r="C5" s="107" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="116" t="s">
+      <c r="D5" s="119" t="s">
         <v>228</v>
       </c>
-      <c r="E5" s="116"/>
+      <c r="E5" s="119"/>
       <c r="F5" s="70"/>
       <c r="G5" s="71"/>
       <c r="H5" s="107" t="s">
         <v>51</v>
       </c>
-      <c r="I5" s="116" t="s">
+      <c r="I5" s="119" t="s">
         <v>228</v>
       </c>
-      <c r="J5" s="116"/>
+      <c r="J5" s="119"/>
       <c r="K5" s="56"/>
       <c r="M5" s="87" t="s">
         <v>291</v>
@@ -4499,19 +4700,19 @@
       <c r="C18" s="107" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="125" t="s">
+      <c r="D18" s="128" t="s">
         <v>236</v>
       </c>
-      <c r="E18" s="125"/>
+      <c r="E18" s="128"/>
       <c r="F18" s="103"/>
       <c r="G18" s="104"/>
       <c r="H18" s="107" t="s">
         <v>51</v>
       </c>
-      <c r="I18" s="125" t="s">
+      <c r="I18" s="128" t="s">
         <v>236</v>
       </c>
-      <c r="J18" s="125"/>
+      <c r="J18" s="128"/>
       <c r="K18" s="106"/>
     </row>
     <row r="19" spans="3:16" x14ac:dyDescent="0.25">
@@ -4688,37 +4889,37 @@
     </row>
     <row r="27" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="117" t="s">
+      <c r="C28" s="120" t="s">
         <v>241</v>
       </c>
-      <c r="D28" s="118"/>
-      <c r="E28" s="118"/>
-      <c r="F28" s="118"/>
-      <c r="G28" s="118"/>
-      <c r="H28" s="118"/>
-      <c r="I28" s="118"/>
-      <c r="J28" s="118"/>
-      <c r="K28" s="119"/>
-      <c r="M28" s="120" t="s">
+      <c r="D28" s="121"/>
+      <c r="E28" s="121"/>
+      <c r="F28" s="121"/>
+      <c r="G28" s="121"/>
+      <c r="H28" s="121"/>
+      <c r="I28" s="121"/>
+      <c r="J28" s="121"/>
+      <c r="K28" s="122"/>
+      <c r="M28" s="123" t="s">
         <v>245</v>
       </c>
-      <c r="N28" s="120"/>
-      <c r="O28" s="120"/>
-      <c r="P28" s="120"/>
+      <c r="N28" s="123"/>
+      <c r="O28" s="123"/>
+      <c r="P28" s="123"/>
     </row>
     <row r="29" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C29" s="55"/>
-      <c r="D29" s="121" t="s">
+      <c r="D29" s="124" t="s">
         <v>237</v>
       </c>
-      <c r="E29" s="121"/>
+      <c r="E29" s="124"/>
       <c r="F29" s="70"/>
       <c r="G29" s="73"/>
       <c r="H29" s="72"/>
-      <c r="I29" s="115" t="s">
+      <c r="I29" s="118" t="s">
         <v>238</v>
       </c>
-      <c r="J29" s="115"/>
+      <c r="J29" s="118"/>
       <c r="K29" s="56"/>
       <c r="M29" s="87" t="s">
         <v>246</v>
@@ -4737,19 +4938,19 @@
       <c r="C30" s="107" t="s">
         <v>51</v>
       </c>
-      <c r="D30" s="116" t="s">
+      <c r="D30" s="119" t="s">
         <v>240</v>
       </c>
-      <c r="E30" s="116"/>
+      <c r="E30" s="119"/>
       <c r="F30" s="70"/>
       <c r="G30" s="73"/>
       <c r="H30" s="107" t="s">
         <v>51</v>
       </c>
-      <c r="I30" s="116" t="s">
+      <c r="I30" s="119" t="s">
         <v>240</v>
       </c>
-      <c r="J30" s="116"/>
+      <c r="J30" s="119"/>
       <c r="K30" s="56"/>
       <c r="M30" s="87" t="s">
         <v>291</v>
@@ -4989,7 +5190,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:P33"/>
   <sheetViews>
@@ -5015,36 +5216,36 @@
   <sheetData>
     <row r="2" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="117" t="s">
+      <c r="C3" s="120" t="s">
         <v>285</v>
       </c>
-      <c r="D3" s="118"/>
-      <c r="E3" s="118"/>
-      <c r="F3" s="118"/>
-      <c r="G3" s="118"/>
-      <c r="H3" s="118"/>
-      <c r="I3" s="118"/>
-      <c r="J3" s="118"/>
-      <c r="K3" s="119"/>
-      <c r="M3" s="120" t="s">
+      <c r="D3" s="121"/>
+      <c r="E3" s="121"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="121"/>
+      <c r="I3" s="121"/>
+      <c r="J3" s="121"/>
+      <c r="K3" s="122"/>
+      <c r="M3" s="123" t="s">
         <v>238</v>
       </c>
-      <c r="N3" s="120"/>
-      <c r="O3" s="120"/>
+      <c r="N3" s="123"/>
+      <c r="O3" s="123"/>
     </row>
     <row r="4" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C4" s="55"/>
-      <c r="D4" s="121" t="s">
+      <c r="D4" s="124" t="s">
         <v>237</v>
       </c>
-      <c r="E4" s="121"/>
+      <c r="E4" s="124"/>
       <c r="F4" s="70"/>
       <c r="G4" s="71"/>
       <c r="H4" s="72"/>
-      <c r="I4" s="121" t="s">
+      <c r="I4" s="124" t="s">
         <v>238</v>
       </c>
-      <c r="J4" s="121"/>
+      <c r="J4" s="124"/>
       <c r="K4" s="56"/>
       <c r="M4" s="65" t="s">
         <v>246</v>
@@ -5058,17 +5259,17 @@
     </row>
     <row r="5" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C5" s="55"/>
-      <c r="D5" s="116" t="s">
+      <c r="D5" s="119" t="s">
         <v>228</v>
       </c>
-      <c r="E5" s="116"/>
+      <c r="E5" s="119"/>
       <c r="F5" s="70"/>
       <c r="G5" s="71"/>
       <c r="H5" s="72"/>
-      <c r="I5" s="116" t="s">
+      <c r="I5" s="119" t="s">
         <v>228</v>
       </c>
-      <c r="J5" s="116"/>
+      <c r="J5" s="119"/>
       <c r="K5" s="56"/>
       <c r="M5" s="65" t="s">
         <v>286</v>
@@ -5197,17 +5398,17 @@
     </row>
     <row r="12" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C12" s="55"/>
-      <c r="D12" s="116" t="s">
+      <c r="D12" s="119" t="s">
         <v>236</v>
       </c>
-      <c r="E12" s="116"/>
+      <c r="E12" s="119"/>
       <c r="F12" s="70"/>
       <c r="G12" s="71"/>
       <c r="H12" s="72"/>
-      <c r="I12" s="116" t="s">
+      <c r="I12" s="119" t="s">
         <v>236</v>
       </c>
-      <c r="J12" s="116"/>
+      <c r="J12" s="119"/>
       <c r="K12" s="56"/>
     </row>
     <row r="13" spans="3:16" x14ac:dyDescent="0.25">
@@ -5358,36 +5559,36 @@
     </row>
     <row r="22" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="117" t="s">
+      <c r="C23" s="120" t="s">
         <v>241</v>
       </c>
-      <c r="D23" s="118"/>
-      <c r="E23" s="118"/>
-      <c r="F23" s="118"/>
-      <c r="G23" s="118"/>
-      <c r="H23" s="118"/>
-      <c r="I23" s="118"/>
-      <c r="J23" s="118"/>
-      <c r="K23" s="119"/>
-      <c r="M23" s="120" t="s">
+      <c r="D23" s="121"/>
+      <c r="E23" s="121"/>
+      <c r="F23" s="121"/>
+      <c r="G23" s="121"/>
+      <c r="H23" s="121"/>
+      <c r="I23" s="121"/>
+      <c r="J23" s="121"/>
+      <c r="K23" s="122"/>
+      <c r="M23" s="123" t="s">
         <v>245</v>
       </c>
-      <c r="N23" s="120"/>
-      <c r="O23" s="120"/>
+      <c r="N23" s="123"/>
+      <c r="O23" s="123"/>
     </row>
     <row r="24" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C24" s="55"/>
-      <c r="D24" s="121" t="s">
+      <c r="D24" s="124" t="s">
         <v>237</v>
       </c>
-      <c r="E24" s="121"/>
+      <c r="E24" s="124"/>
       <c r="F24" s="70"/>
       <c r="G24" s="73"/>
       <c r="H24" s="72"/>
-      <c r="I24" s="115" t="s">
+      <c r="I24" s="118" t="s">
         <v>238</v>
       </c>
-      <c r="J24" s="115"/>
+      <c r="J24" s="118"/>
       <c r="K24" s="56"/>
       <c r="M24" s="65" t="s">
         <v>246</v>
@@ -5401,17 +5602,17 @@
     </row>
     <row r="25" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C25" s="55"/>
-      <c r="D25" s="116" t="s">
+      <c r="D25" s="119" t="s">
         <v>240</v>
       </c>
-      <c r="E25" s="116"/>
+      <c r="E25" s="119"/>
       <c r="F25" s="70"/>
       <c r="G25" s="73"/>
       <c r="H25" s="72"/>
-      <c r="I25" s="116" t="s">
+      <c r="I25" s="119" t="s">
         <v>240</v>
       </c>
-      <c r="J25" s="116"/>
+      <c r="J25" s="119"/>
       <c r="K25" s="56"/>
       <c r="M25" s="65" t="s">
         <v>243</v>
@@ -5570,11 +5771,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="C23:K23"/>
     <mergeCell ref="M23:O23"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="I24:J24"/>
@@ -5584,6 +5780,11 @@
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="I5:J5"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="C23:K23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5591,11 +5792,178 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="46.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="32.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="33"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" s="46" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="86" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="46" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="95" t="str">
+        <f>CONCATENATE(B4,".",B5,"@mailinator.com")</f>
+        <v>Quinten.Dorsey@mailinator.com</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="46" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="B15" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$C$15:$C$16</xm:f>
+          </x14:formula1>
+          <xm:sqref>B12</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$C$3:$C$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>B3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Drop Down Values'!$C$11:$C$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>B7</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -5624,7 +5992,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>443</v>
+        <v>463</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -5632,7 +6000,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>444</v>
+        <v>464</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -5671,9 +6039,9 @@
       <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="95" t="str">
+      <c r="B6" s="10" t="str">
         <f>CONCATENATE(B2,".",B3,"@mailinator.com")</f>
-        <v>Nayeli.Marshall@mailinator.com</v>
+        <v>Kendall.Vasquez@mailinator.com</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -6312,9 +6680,9 @@
               </from>
               <to>
                 <xdr:col>0</xdr:col>
-                <xdr:colOff>314325</xdr:colOff>
-                <xdr:row>51</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>457200</xdr:colOff>
+                <xdr:row>52</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -6370,7 +6738,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:K106"/>
@@ -7140,9 +7508,9 @@
               </from>
               <to>
                 <xdr:col>0</xdr:col>
-                <xdr:colOff>314325</xdr:colOff>
-                <xdr:row>51</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>457200</xdr:colOff>
+                <xdr:row>52</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -7198,13 +7566,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:K140"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8230,9 +8598,9 @@
               </from>
               <to>
                 <xdr:col>0</xdr:col>
-                <xdr:colOff>314325</xdr:colOff>
-                <xdr:row>51</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>457200</xdr:colOff>
+                <xdr:row>52</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -8288,7 +8656,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:F54"/>
@@ -8741,9 +9109,9 @@
               </from>
               <to>
                 <xdr:col>0</xdr:col>
-                <xdr:colOff>314325</xdr:colOff>
-                <xdr:row>40</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>457200</xdr:colOff>
+                <xdr:row>41</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -8799,7 +9167,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:K101"/>
@@ -9512,9 +9880,9 @@
               </from>
               <to>
                 <xdr:col>0</xdr:col>
-                <xdr:colOff>314325</xdr:colOff>
-                <xdr:row>51</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>457200</xdr:colOff>
+                <xdr:row>52</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -9570,7 +9938,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K101"/>
@@ -10283,9 +10651,9 @@
               </from>
               <to>
                 <xdr:col>0</xdr:col>
-                <xdr:colOff>314325</xdr:colOff>
-                <xdr:row>51</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>457200</xdr:colOff>
+                <xdr:row>52</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -10341,7 +10709,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:G54"/>
@@ -11077,9 +11445,9 @@
               </from>
               <to>
                 <xdr:col>0</xdr:col>
-                <xdr:colOff>314325</xdr:colOff>
-                <xdr:row>40</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>457200</xdr:colOff>
+                <xdr:row>41</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -11133,220 +11501,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
-  <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="48.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="127" t="s">
-        <v>129</v>
-      </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="127"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="F3" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
-      <c r="C4" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="F4" s="24"/>
-      <c r="G4" s="25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="24"/>
-      <c r="C5" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="26" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="24"/>
-      <c r="C6" s="25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="24"/>
-      <c r="C7" s="25" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="24"/>
-      <c r="C8" s="25" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="21"/>
-      <c r="C9" s="26" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B11" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="24"/>
-      <c r="C12" s="25" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="21"/>
-      <c r="C13" s="26" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B15" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="21"/>
-      <c r="C16" s="22"/>
-    </row>
-    <row r="17" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="2:3" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B18" s="27" t="s">
-        <v>136</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="24"/>
-      <c r="C19" s="25" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="21"/>
-      <c r="C20" s="26" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="2:3" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B22" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="23" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="24"/>
-      <c r="C23" s="25" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="24"/>
-      <c r="C24" s="25" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="24"/>
-      <c r="C25" s="25" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="24"/>
-      <c r="C26" s="25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="21"/>
-      <c r="C27" s="26" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="50"/>
-      <c r="C28" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C29" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="2:3" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B31" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="C31" s="23" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="21"/>
-      <c r="C32" s="26" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>